<commit_message>
some functionality for fully connected layer
</commit_message>
<xml_diff>
--- a/vika_conv2.xlsx
+++ b/vika_conv2.xlsx
@@ -20,9 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t xml:space="preserve">Изображение</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+  <si>
+    <t xml:space="preserve">Изображение (8x9)</t>
   </si>
   <si>
     <t xml:space="preserve">Ядро свёртки</t>
@@ -41,6 +41,45 @@
   </si>
   <si>
     <t xml:space="preserve">Maxpooling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Веса fully connected (для трёх выходов)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Вход</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Перемножение веса и входа</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Выход</t>
+  </si>
+  <si>
+    <t xml:space="preserve">out1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">out2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">out3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maxpool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Выход активированный</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Производная активации</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Желаемое</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ошибка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">δ</t>
   </si>
 </sst>
 </file>
@@ -50,7 +89,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -79,19 +118,19 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FF993300"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -128,7 +167,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -137,8 +176,20 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -158,10 +209,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K39"/>
+  <dimension ref="A1:M59"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H26" activeCellId="0" sqref="H26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M54" activeCellId="0" sqref="M54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -184,236 +235,236 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>-1</v>
+        <v>-0.1</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>3</v>
+        <v>0.3</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>4</v>
+        <v>0.4</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>6</v>
+        <v>0.6</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>7</v>
+        <v>0.7</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>8</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>-9</v>
+        <v>-0.9</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>-10</v>
+        <v>-0.1</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>11</v>
+        <v>0.11</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>12</v>
+        <v>0.12</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>13</v>
+        <v>0.13</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>14</v>
+        <v>0.14</v>
       </c>
       <c r="G3" s="0" t="n">
-        <v>15</v>
+        <v>0.15</v>
       </c>
       <c r="H3" s="0" t="n">
-        <v>16</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>-17</v>
+        <v>-0.17</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>18</v>
+        <v>0.18</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>-19</v>
+        <v>-0.19</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>20</v>
+        <v>0.2</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>21</v>
+        <v>0.21</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>22</v>
+        <v>0.22</v>
       </c>
       <c r="G4" s="0" t="n">
-        <v>23</v>
+        <v>0.23</v>
       </c>
       <c r="H4" s="0" t="n">
-        <v>24</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>-25</v>
+        <v>-0.25</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>26</v>
+        <v>0.26</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>27</v>
+        <v>0.27</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>-28</v>
+        <v>-0.28</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>29</v>
+        <v>0.29</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>30</v>
+        <v>0.3</v>
       </c>
       <c r="G5" s="0" t="n">
-        <v>31</v>
+        <v>0.31</v>
       </c>
       <c r="H5" s="0" t="n">
-        <v>32</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>-33</v>
+        <v>-0.33</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>34</v>
+        <v>0.34</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>35</v>
+        <v>0.35</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>36</v>
+        <v>0.36</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>-37</v>
+        <v>-0.37</v>
       </c>
       <c r="F6" s="0" t="n">
-        <v>38</v>
+        <v>0.38</v>
       </c>
       <c r="G6" s="0" t="n">
-        <v>39</v>
+        <v>0.39</v>
       </c>
       <c r="H6" s="0" t="n">
-        <v>40</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>-41</v>
+        <v>-0.41</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>42</v>
+        <v>0.42</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>43</v>
+        <v>0.43</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>44</v>
+        <v>0.44</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>45</v>
+        <v>0.45</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>-46</v>
+        <v>-0.46</v>
       </c>
       <c r="G7" s="0" t="n">
-        <v>47</v>
+        <v>0.47</v>
       </c>
       <c r="H7" s="0" t="n">
-        <v>48</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>-49</v>
+        <v>-0.49</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>50</v>
+        <v>0.5</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>51</v>
+        <v>0.51</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>52</v>
+        <v>0.52</v>
       </c>
       <c r="E8" s="0" t="n">
-        <v>53</v>
+        <v>0.53</v>
       </c>
       <c r="F8" s="0" t="n">
-        <v>54</v>
+        <v>0.54</v>
       </c>
       <c r="G8" s="0" t="n">
-        <v>-55</v>
+        <v>-0.55</v>
       </c>
       <c r="H8" s="0" t="n">
-        <v>56</v>
+        <v>0.56</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>-57</v>
+        <v>-0.57</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>58</v>
+        <v>0.58</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>59</v>
+        <v>0.59</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>60</v>
+        <v>0.6</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>61</v>
+        <v>0.61</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>62</v>
+        <v>0.62</v>
       </c>
       <c r="G9" s="0" t="n">
-        <v>63</v>
+        <v>0.63</v>
       </c>
       <c r="H9" s="0" t="n">
-        <v>-64</v>
+        <v>-0.64</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>-65</v>
+        <v>-0.65</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>66</v>
+        <v>0.66</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>67</v>
+        <v>0.67</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>68</v>
+        <v>0.68</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>69</v>
+        <v>0.69</v>
       </c>
       <c r="F10" s="0" t="n">
-        <v>70</v>
+        <v>0.7</v>
       </c>
       <c r="G10" s="0" t="n">
-        <v>71</v>
+        <v>0.71</v>
       </c>
       <c r="H10" s="0" t="n">
-        <v>72</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -552,183 +603,183 @@
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <f aca="false">$A$13*A2+$B$13*B2+$C$13*C2+$A$14*A3+$B$14*B3+$C$14*C3+$A$15*A4+$B$15*B4+$C$15*C4</f>
-        <v>13.4983855930265</v>
+        <v>0.29973878860774</v>
       </c>
       <c r="B18" s="0" t="n">
         <f aca="false">$A$13*B2+$B$13*C2+$C$13*D2+$A$14*B3+$B$14*C3+$C$14*D3+$A$15*B4+$B$15*C4+$C$15*D4</f>
-        <v>-5.1281735924311</v>
+        <v>0.14573618884283</v>
       </c>
       <c r="C18" s="0" t="n">
         <f aca="false">$A$13*C2+$B$13*D2+$C$13*E2+$A$14*C3+$B$14*D3+$C$14*E3+$A$15*C4+$B$15*D4+$C$15*E4</f>
-        <v>-3.34233491987629</v>
+        <v>0.227470224200259</v>
       </c>
       <c r="D18" s="0" t="n">
         <f aca="false">$A$13*D2+$B$13*E2+$C$13*F2+$A$14*D3+$B$14*E3+$C$14*F3+$A$15*D4+$B$15*E4+$C$15*F4</f>
-        <v>-20.270098210379</v>
+        <v>0.122068239927113</v>
       </c>
       <c r="E18" s="0" t="n">
         <f aca="false">$A$13*E2+$B$13*F2+$C$13*G2+$A$14*E3+$B$14*F3+$C$14*G3+$A$15*E4+$B$15*F4+$C$15*G4</f>
-        <v>-20.6920682311457</v>
+        <v>0.181724188351327</v>
       </c>
       <c r="F18" s="0" t="n">
         <f aca="false">$A$13*F2+$B$13*G2+$C$13*H2+$A$14*F3+$B$14*G3+$C$14*H3+$A$15*F4+$B$15*G4+$C$15*H4</f>
-        <v>-21.1140382519125</v>
+        <v>0.24138013677554</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <f aca="false">$A$13*A3+$B$13*B3+$C$13*C3+$A$14*A4+$B$14*B4+$C$14*C4+$A$15*A5+$B$15*B5+$C$15*C5</f>
-        <v>-16.3374253529275</v>
+        <v>-0.248149086792767</v>
       </c>
       <c r="B19" s="0" t="n">
         <f aca="false">$A$13*B3+$B$13*C3+$C$13*D3+$A$14*B4+$B$14*C4+$C$14*D4+$A$15*B5+$B$15*C5+$C$15*D5</f>
-        <v>0.538357957508739</v>
+        <v>0.00538357957508741</v>
       </c>
       <c r="C19" s="0" t="n">
         <f aca="false">$A$13*C3+$B$13*D3+$C$13*E3+$A$14*C4+$B$14*D4+$C$14*E4+$A$15*C5+$B$15*D5+$C$15*E5</f>
-        <v>-1.62210573388792</v>
+        <v>-0.0162210573388792</v>
       </c>
       <c r="D19" s="0" t="n">
         <f aca="false">$A$13*D3+$B$13*E3+$C$13*F3+$A$14*D4+$B$14*E4+$C$14*F4+$A$15*D5+$B$15*E5+$C$15*F5</f>
-        <v>0.678468547308199</v>
+        <v>0.00678468547308203</v>
       </c>
       <c r="E19" s="0" t="n">
         <f aca="false">$A$13*E3+$B$13*F3+$C$13*G3+$A$14*E4+$B$14*F4+$C$14*G4+$A$15*E5+$B$15*F5+$C$15*G5</f>
-        <v>-24.0678283972799</v>
+        <v>-0.240678283972799</v>
       </c>
       <c r="F19" s="0" t="n">
         <f aca="false">$A$13*F3+$B$13*G3+$C$13*H3+$A$14*F4+$B$14*G4+$C$14*H4+$A$15*F5+$B$15*G5+$C$15*H5</f>
-        <v>-24.4897984180467</v>
+        <v>-0.244897984180467</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
         <f aca="false">$A$13*A4+$B$13*B4+$C$13*C4+$A$14*A5+$B$14*B5+$C$14*C5+$A$15*A6+$B$15*B6+$C$15*C6</f>
-        <v>-3.78519292165913</v>
+        <v>-0.0378519292165913</v>
       </c>
       <c r="B20" s="0" t="n">
         <f aca="false">$A$13*B4+$B$13*C4+$C$13*D4+$A$14*B5+$B$14*C5+$C$14*D5+$A$15*B6+$B$15*C6+$C$15*D6</f>
-        <v>-53.3791159273823</v>
+        <v>-0.533791159273823</v>
       </c>
       <c r="C20" s="0" t="n">
         <f aca="false">$A$13*C4+$B$13*D4+$C$13*E4+$A$14*C5+$B$14*D5+$C$14*E5+$A$15*C6+$B$15*D6+$C$15*E6</f>
-        <v>3.46781629923113</v>
+        <v>0.0346781629923112</v>
       </c>
       <c r="D20" s="0" t="n">
         <f aca="false">$A$13*D4+$B$13*E4+$C$13*F4+$A$14*D5+$B$14*E5+$C$14*F5+$A$15*D6+$B$15*E6+$C$15*F6</f>
-        <v>1.88396212465526</v>
+        <v>0.0188396212465526</v>
       </c>
       <c r="E20" s="0" t="n">
         <f aca="false">$A$13*E4+$B$13*F4+$C$13*G4+$A$14*E5+$B$14*F5+$C$14*G5+$A$15*E6+$B$15*F6+$C$15*G6</f>
-        <v>4.69927201449269</v>
+        <v>0.0469927201449269</v>
       </c>
       <c r="F20" s="0" t="n">
         <f aca="false">$A$13*F4+$B$13*G4+$C$13*H4+$A$14*F5+$B$14*G5+$C$14*H5+$A$15*F6+$B$15*G6+$C$15*H6</f>
-        <v>-27.8655585841809</v>
+        <v>-0.278655585841809</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <f aca="false">$A$13*A5+$B$13*B5+$C$13*C5+$A$14*A6+$B$14*B6+$C$14*C6+$A$15*A7+$B$15*B7+$C$15*C7</f>
-        <v>5.3641450243641</v>
+        <v>0.0536414502436411</v>
       </c>
       <c r="B21" s="0" t="n">
         <f aca="false">$A$13*B5+$B$13*C5+$C$13*D5+$A$14*B6+$B$14*C6+$C$14*D6+$A$15*B7+$B$15*C7+$C$15*D7</f>
-        <v>-38.7688016474834</v>
+        <v>-0.387688016474834</v>
       </c>
       <c r="C21" s="0" t="n">
         <f aca="false">$A$13*C5+$B$13*D5+$C$13*E5+$A$14*C6+$B$14*D6+$C$14*E6+$A$15*C7+$B$15*D7+$C$15*E7</f>
-        <v>-68.4688250107015</v>
+        <v>-0.684688250107015</v>
       </c>
       <c r="D21" s="0" t="n">
         <f aca="false">$A$13*D5+$B$13*E5+$C$13*F5+$A$14*D6+$B$14*E6+$C$14*F6+$A$15*D7+$B$15*E7+$C$15*F7</f>
-        <v>6.39727464095352</v>
+        <v>0.0639727464095352</v>
       </c>
       <c r="E21" s="0" t="n">
         <f aca="false">$A$13*E5+$B$13*F5+$C$13*G5+$A$14*E6+$B$14*F6+$C$14*G6+$A$15*E7+$B$15*F7+$C$15*G7</f>
-        <v>5.39002998319843</v>
+        <v>0.0539002998319844</v>
       </c>
       <c r="F21" s="0" t="n">
         <f aca="false">$A$13*F5+$B$13*G5+$C$13*H5+$A$14*F6+$B$14*G6+$C$14*H6+$A$15*F7+$B$15*G7+$C$15*H7</f>
-        <v>8.72007548167719</v>
+        <v>0.0872007548167718</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
         <f aca="false">$A$13*A6+$B$13*B6+$C$13*C6+$A$14*A7+$B$14*B7+$C$14*C7+$A$15*A8+$B$15*B8+$C$15*C8</f>
-        <v>8.26020094808472</v>
+        <v>0.0826020094808472</v>
       </c>
       <c r="B22" s="0" t="n">
         <f aca="false">$A$13*B6+$B$13*C6+$C$13*D6+$A$14*B7+$B$14*C7+$C$14*D7+$A$15*B8+$B$15*C8+$C$15*D8</f>
-        <v>-32.9291988333821</v>
+        <v>-0.329291988333821</v>
       </c>
       <c r="C22" s="0" t="n">
         <f aca="false">$A$13*C6+$B$13*D6+$C$13*E6+$A$14*C7+$B$14*D7+$C$14*E7+$A$15*C8+$B$15*D8+$C$15*E8</f>
-        <v>-45.5286127923172</v>
+        <v>-0.455286127923171</v>
       </c>
       <c r="D22" s="0" t="n">
         <f aca="false">$A$13*D6+$B$13*E6+$C$13*F6+$A$14*D7+$B$14*E7+$C$14*F7+$A$15*D8+$B$15*E8+$C$15*F8</f>
-        <v>-83.5585340940206</v>
+        <v>-0.835585340940206</v>
       </c>
       <c r="E22" s="0" t="n">
         <f aca="false">$A$13*E6+$B$13*F6+$C$13*G6+$A$14*E7+$B$14*F7+$C$14*G7+$A$15*E8+$B$15*F8+$C$15*G8</f>
-        <v>9.32673298267591</v>
+        <v>0.093267329826759</v>
       </c>
       <c r="F22" s="0" t="n">
         <f aca="false">$A$13*F6+$B$13*G6+$C$13*H6+$A$14*F7+$B$14*G7+$C$14*H7+$A$15*F8+$B$15*G8+$C$15*H8</f>
-        <v>8.89609784174161</v>
+        <v>0.088960978417416</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
         <f aca="false">$A$13*A7+$B$13*B7+$C$13*C7+$A$14*A8+$B$14*B8+$C$14*C8+$A$15*A9+$B$15*B9+$C$15*C9</f>
-        <v>11.1562568718053</v>
+        <v>0.111562568718053</v>
       </c>
       <c r="B23" s="0" t="n">
         <f aca="false">$A$13*B7+$B$13*C7+$C$13*D7+$A$14*B8+$B$14*C8+$C$14*D8+$A$15*B9+$B$15*C9+$C$15*D9</f>
-        <v>-36.3049589995163</v>
+        <v>-0.363049589995163</v>
       </c>
       <c r="C23" s="0" t="n">
         <f aca="false">$A$13*C7+$B$13*D7+$C$13*E7+$A$14*C8+$B$14*D8+$C$14*E8+$A$15*C9+$B$15*D9+$C$15*E9</f>
-        <v>-36.7269290202831</v>
+        <v>-0.36726929020283</v>
       </c>
       <c r="D23" s="0" t="n">
         <f aca="false">$A$13*D7+$B$13*E7+$C$13*F7+$A$14*D8+$B$14*E8+$C$14*F8+$A$15*D9+$B$15*E9+$C$15*F9</f>
-        <v>-52.2884239371509</v>
+        <v>-0.522884239371509</v>
       </c>
       <c r="E23" s="0" t="n">
         <f aca="false">$A$13*E7+$B$13*F7+$C$13*G7+$A$14*E8+$B$14*F8+$C$14*G8+$A$15*E9+$B$15*F9+$C$15*G9</f>
-        <v>-98.6482431773397</v>
+        <v>-0.986482431773397</v>
       </c>
       <c r="F23" s="0" t="n">
         <f aca="false">$A$13*F7+$B$13*G7+$C$13*H7+$A$14*F8+$B$14*G8+$C$14*H8+$A$15*F9+$B$15*G9+$C$15*H9</f>
-        <v>12.2561913243983</v>
+        <v>0.122561913243983</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
         <f aca="false">$A$13*A8+$B$13*B8+$C$13*C8+$A$14*A9+$B$14*B9+$C$14*C9+$A$15*A10+$B$15*B10+$C$15*C10</f>
-        <v>14.0523127955259</v>
+        <v>0.140523127955259</v>
       </c>
       <c r="B24" s="0" t="n">
         <f aca="false">$A$13*B8+$B$13*C8+$C$13*D8+$A$14*B9+$B$14*C9+$C$14*D9+$A$15*B10+$B$15*C10+$C$15*D10</f>
-        <v>-39.6807191656505</v>
+        <v>-0.396807191656504</v>
       </c>
       <c r="C24" s="0" t="n">
         <f aca="false">$A$13*C8+$B$13*D8+$C$13*E8+$A$14*C9+$B$14*D9+$C$14*E9+$A$15*C10+$B$15*D10+$C$15*E10</f>
-        <v>-40.1026891864172</v>
+        <v>-0.401026891864172</v>
       </c>
       <c r="D24" s="0" t="n">
         <f aca="false">$A$13*D8+$B$13*E8+$C$13*F8+$A$14*D9+$B$14*E9+$C$14*F9+$A$15*D10+$B$15*E10+$C$15*F10</f>
-        <v>-40.524659207184</v>
+        <v>-0.40524659207184</v>
       </c>
       <c r="E24" s="0" t="n">
         <f aca="false">$A$13*E8+$B$13*F8+$C$13*G8+$A$14*E9+$B$14*F9+$C$14*G9+$A$15*E10+$B$15*F10+$C$15*G10</f>
-        <v>-59.0482350819847</v>
+        <v>-0.590482350819847</v>
       </c>
       <c r="F24" s="0" t="n">
         <f aca="false">$A$13*F8+$B$13*G8+$C$13*H8+$A$14*F9+$B$14*G9+$C$14*H9+$A$15*F10+$B$15*G10+$C$15*H10</f>
-        <v>-113.737952260659</v>
+        <v>-1.13737952260659</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -745,27 +796,27 @@
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
         <f aca="false">IF(A18&lt;0,0,A18)</f>
-        <v>13.4983855930265</v>
+        <v>0.29973878860774</v>
       </c>
       <c r="B27" s="0" t="n">
         <f aca="false">IF(B18&lt;0,0,B18)</f>
-        <v>0</v>
+        <v>0.14573618884283</v>
       </c>
       <c r="C27" s="0" t="n">
         <f aca="false">IF(C18&lt;0,0,C18)</f>
-        <v>0</v>
+        <v>0.227470224200259</v>
       </c>
       <c r="D27" s="0" t="n">
         <f aca="false">IF(D18&lt;0,0,D18)</f>
-        <v>0</v>
+        <v>0.122068239927113</v>
       </c>
       <c r="E27" s="0" t="n">
         <f aca="false">IF(E18&lt;0,0,E18)</f>
-        <v>0</v>
+        <v>0.181724188351327</v>
       </c>
       <c r="F27" s="0" t="n">
         <f aca="false">IF(F18&lt;0,0,F18)</f>
-        <v>0</v>
+        <v>0.24138013677554</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -775,7 +826,7 @@
       </c>
       <c r="B28" s="0" t="n">
         <f aca="false">IF(B19&lt;0,0,B19)</f>
-        <v>0.538357957508739</v>
+        <v>0.00538357957508741</v>
       </c>
       <c r="C28" s="0" t="n">
         <f aca="false">IF(C19&lt;0,0,C19)</f>
@@ -783,7 +834,7 @@
       </c>
       <c r="D28" s="0" t="n">
         <f aca="false">IF(D19&lt;0,0,D19)</f>
-        <v>0.678468547308199</v>
+        <v>0.00678468547308203</v>
       </c>
       <c r="E28" s="0" t="n">
         <f aca="false">IF(E19&lt;0,0,E19)</f>
@@ -805,15 +856,15 @@
       </c>
       <c r="C29" s="0" t="n">
         <f aca="false">IF(C20&lt;0,0,C20)</f>
-        <v>3.46781629923113</v>
+        <v>0.0346781629923112</v>
       </c>
       <c r="D29" s="0" t="n">
         <f aca="false">IF(D20&lt;0,0,D20)</f>
-        <v>1.88396212465526</v>
+        <v>0.0188396212465526</v>
       </c>
       <c r="E29" s="0" t="n">
         <f aca="false">IF(E20&lt;0,0,E20)</f>
-        <v>4.69927201449269</v>
+        <v>0.0469927201449269</v>
       </c>
       <c r="F29" s="0" t="n">
         <f aca="false">IF(F20&lt;0,0,F20)</f>
@@ -823,7 +874,7 @@
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
         <f aca="false">IF(A21&lt;0,0,A21)</f>
-        <v>5.3641450243641</v>
+        <v>0.0536414502436411</v>
       </c>
       <c r="B30" s="0" t="n">
         <f aca="false">IF(B21&lt;0,0,B21)</f>
@@ -835,21 +886,21 @@
       </c>
       <c r="D30" s="0" t="n">
         <f aca="false">IF(D21&lt;0,0,D21)</f>
-        <v>6.39727464095352</v>
+        <v>0.0639727464095352</v>
       </c>
       <c r="E30" s="0" t="n">
         <f aca="false">IF(E21&lt;0,0,E21)</f>
-        <v>5.39002998319843</v>
+        <v>0.0539002998319844</v>
       </c>
       <c r="F30" s="0" t="n">
         <f aca="false">IF(F21&lt;0,0,F21)</f>
-        <v>8.72007548167719</v>
+        <v>0.0872007548167718</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
         <f aca="false">IF(A22&lt;0,0,A22)</f>
-        <v>8.26020094808472</v>
+        <v>0.0826020094808472</v>
       </c>
       <c r="B31" s="0" t="n">
         <f aca="false">IF(B22&lt;0,0,B22)</f>
@@ -865,17 +916,17 @@
       </c>
       <c r="E31" s="0" t="n">
         <f aca="false">IF(E22&lt;0,0,E22)</f>
-        <v>9.32673298267591</v>
+        <v>0.093267329826759</v>
       </c>
       <c r="F31" s="0" t="n">
         <f aca="false">IF(F22&lt;0,0,F22)</f>
-        <v>8.89609784174161</v>
+        <v>0.088960978417416</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
         <f aca="false">IF(A23&lt;0,0,A23)</f>
-        <v>11.1562568718053</v>
+        <v>0.111562568718053</v>
       </c>
       <c r="B32" s="0" t="n">
         <f aca="false">IF(B23&lt;0,0,B23)</f>
@@ -895,13 +946,13 @@
       </c>
       <c r="F32" s="0" t="n">
         <f aca="false">IF(F23&lt;0,0,F23)</f>
-        <v>12.2561913243983</v>
+        <v>0.122561913243983</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
         <f aca="false">IF(A24&lt;0,0,A24)</f>
-        <v>14.0523127955259</v>
+        <v>0.140523127955259</v>
       </c>
       <c r="B33" s="0" t="n">
         <f aca="false">IF(B24&lt;0,0,B24)</f>
@@ -935,43 +986,37 @@
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
         <f aca="false">MAX(A27:B28)</f>
-        <v>13.4983855930265</v>
+        <v>0.29973878860774</v>
       </c>
       <c r="B36" s="0" t="n">
         <f aca="false">MAX(C27:D28)</f>
-        <v>0.678468547308199</v>
+        <v>0.227470224200259</v>
       </c>
       <c r="C36" s="0" t="n">
         <f aca="false">MAX(E27:F28)</f>
-        <v>0</v>
-      </c>
-      <c r="D36" s="2" t="n">
-        <f aca="false">MAX(G27:H28)</f>
-        <v>0</v>
-      </c>
+        <v>0.24138013677554</v>
+      </c>
+      <c r="D36" s="2"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
         <f aca="false">MAX(A29:B30)</f>
-        <v>5.3641450243641</v>
+        <v>0.0536414502436411</v>
       </c>
       <c r="B37" s="0" t="n">
         <f aca="false">MAX(C29:D30)</f>
-        <v>6.39727464095352</v>
+        <v>0.0639727464095352</v>
       </c>
       <c r="C37" s="0" t="n">
         <f aca="false">MAX(E29:F30)</f>
-        <v>8.72007548167719</v>
-      </c>
-      <c r="D37" s="2" t="n">
-        <f aca="false">MAX(G29:H30)</f>
-        <v>0</v>
-      </c>
+        <v>0.0872007548167718</v>
+      </c>
+      <c r="D37" s="2"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
         <f aca="false">MAX(A31:B32)</f>
-        <v>11.1562568718053</v>
+        <v>0.111562568718053</v>
       </c>
       <c r="B38" s="0" t="n">
         <f aca="false">MAX(C31:D32)</f>
@@ -979,17 +1024,14 @@
       </c>
       <c r="C38" s="0" t="n">
         <f aca="false">MAX(E31:F32)</f>
-        <v>12.2561913243983</v>
-      </c>
-      <c r="D38" s="2" t="n">
-        <f aca="false">MAX(G31:H32)</f>
-        <v>0</v>
-      </c>
+        <v>0.122561913243983</v>
+      </c>
+      <c r="D38" s="2"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="n">
         <f aca="false">MAX(A33:B34)</f>
-        <v>14.0523127955259</v>
+        <v>0.140523127955259</v>
       </c>
       <c r="B39" s="2" t="n">
         <f aca="false">MAX(C33:D34)</f>
@@ -999,13 +1041,486 @@
         <f aca="false">MAX(E33:F34)</f>
         <v>0</v>
       </c>
-      <c r="D39" s="2" t="n">
-        <f aca="false">MAX(G33:H34)</f>
-        <v>0</v>
+      <c r="D39" s="2"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="E42" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+      <c r="K42" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L42" s="3"/>
+      <c r="M42" s="3"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G43" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H43" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="I43" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="K43" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="L43" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="M43" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="n">
+        <v>0.300911860585287</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <v>0.515212628502065</v>
+      </c>
+      <c r="C44" s="0" t="n">
+        <v>0.813639960990097</v>
+      </c>
+      <c r="E44" s="0" t="n">
+        <f aca="false">A36</f>
+        <v>0.29973878860774</v>
+      </c>
+      <c r="G44" s="0" t="n">
+        <f aca="false">E44*A44</f>
+        <v>0.0901949565695351</v>
+      </c>
+      <c r="H44" s="0" t="n">
+        <f aca="false">E44*B44</f>
+        <v>0.154429209142619</v>
+      </c>
+      <c r="I44" s="0" t="n">
+        <f aca="false">E44*C44</f>
+        <v>0.24387945627002</v>
+      </c>
+      <c r="K44" s="0" t="n">
+        <f aca="false">SUM(G44:G55)</f>
+        <v>0.518244508934845</v>
+      </c>
+      <c r="L44" s="0" t="n">
+        <f aca="false">SUM(H44:H55)</f>
+        <v>0.607847365098408</v>
+      </c>
+      <c r="M44" s="0" t="n">
+        <f aca="false">SUM(I44:I55)</f>
+        <v>0.703388535941197</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="n">
+        <v>0.214263872582375</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <v>0.380657189299686</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <v>0.31805817433033</v>
+      </c>
+      <c r="E45" s="0" t="n">
+        <f aca="false">B36</f>
+        <v>0.227470224200259</v>
+      </c>
+      <c r="G45" s="0" t="n">
+        <f aca="false">E45*A45</f>
+        <v>0.0487386511343286</v>
+      </c>
+      <c r="H45" s="0" t="n">
+        <f aca="false">E45*B45</f>
+        <v>0.0865881761934401</v>
+      </c>
+      <c r="I45" s="0" t="n">
+        <f aca="false">E45*C45</f>
+        <v>0.0723487642236453</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="n">
+        <v>0.468889844902423</v>
+      </c>
+      <c r="B46" s="0" t="n">
+        <v>0.283034151180445</v>
+      </c>
+      <c r="C46" s="0" t="n">
+        <v>0.293101857336816</v>
+      </c>
+      <c r="E46" s="0" t="n">
+        <f aca="false">C36</f>
+        <v>0.24138013677554</v>
+      </c>
+      <c r="G46" s="0" t="n">
+        <f aca="false">E46*A46</f>
+        <v>0.113180694895209</v>
+      </c>
+      <c r="H46" s="0" t="n">
+        <f aca="false">E46*B46</f>
+        <v>0.0683188221240847</v>
+      </c>
+      <c r="I46" s="0" t="n">
+        <f aca="false">E46*C46</f>
+        <v>0.0707489664131254</v>
+      </c>
+      <c r="K46" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L46" s="3"/>
+      <c r="M46" s="3"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="n">
+        <v>0.679084675920216</v>
+      </c>
+      <c r="B47" s="0" t="n">
+        <v>0.218553052592764</v>
+      </c>
+      <c r="C47" s="0" t="n">
+        <v>0.203186876647323</v>
+      </c>
+      <c r="E47" s="0" t="n">
+        <f aca="false">A37</f>
+        <v>0.0536414502436411</v>
+      </c>
+      <c r="G47" s="0" t="n">
+        <f aca="false">E47*A47</f>
+        <v>0.0364270868545934</v>
+      </c>
+      <c r="H47" s="0" t="n">
+        <f aca="false">E47*B47</f>
+        <v>0.0117235026962506</v>
+      </c>
+      <c r="I47" s="0" t="n">
+        <f aca="false">E47*C47</f>
+        <v>0.0108992387338382</v>
+      </c>
+      <c r="K47" s="0" t="n">
+        <f aca="false">1/(1+EXP(-1*K44))</f>
+        <v>0.626737182249149</v>
+      </c>
+      <c r="L47" s="0" t="n">
+        <f aca="false">1/(1+EXP(-1*L44))</f>
+        <v>0.647449600718403</v>
+      </c>
+      <c r="M47" s="0" t="n">
+        <f aca="false">1/(1+EXP(-1*M44))</f>
+        <v>0.668938625570398</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="n">
+        <v>0.360871416856906</v>
+      </c>
+      <c r="B48" s="0" t="n">
+        <v>0.570673276071023</v>
+      </c>
+      <c r="C48" s="0" t="n">
+        <v>0.862491437447886</v>
+      </c>
+      <c r="E48" s="0" t="n">
+        <f aca="false">B37</f>
+        <v>0.0639727464095352</v>
+      </c>
+      <c r="G48" s="0" t="n">
+        <f aca="false">E48*A48</f>
+        <v>0.0230859356370365</v>
+      </c>
+      <c r="H48" s="0" t="n">
+        <f aca="false">E48*B48</f>
+        <v>0.0365075367727902</v>
+      </c>
+      <c r="I48" s="0" t="n">
+        <f aca="false">E48*C48</f>
+        <v>0.0551759460082491</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="n">
+        <v>0.293114244553858</v>
+      </c>
+      <c r="B49" s="0" t="n">
+        <v>0.297082563556292</v>
+      </c>
+      <c r="C49" s="0" t="n">
+        <v>0.752573035551612</v>
+      </c>
+      <c r="E49" s="0" t="n">
+        <f aca="false">C37</f>
+        <v>0.0872007548167718</v>
+      </c>
+      <c r="G49" s="0" t="n">
+        <f aca="false">E49*A49</f>
+        <v>0.0255597833726443</v>
+      </c>
+      <c r="H49" s="0" t="n">
+        <f aca="false">E49*B49</f>
+        <v>0.0259058237850102</v>
+      </c>
+      <c r="I49" s="0" t="n">
+        <f aca="false">E49*C49</f>
+        <v>0.0656249367548498</v>
+      </c>
+      <c r="K49" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L49" s="3"/>
+      <c r="M49" s="3"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="n">
+        <v>0.206582661913699</v>
+      </c>
+      <c r="B50" s="0" t="n">
+        <v>0.865335013001561</v>
+      </c>
+      <c r="C50" s="0" t="n">
+        <v>0.696719165746635</v>
+      </c>
+      <c r="E50" s="0" t="n">
+        <f aca="false">A38</f>
+        <v>0.111562568718053</v>
+      </c>
+      <c r="G50" s="0" t="n">
+        <f aca="false">E50*A50</f>
+        <v>0.0230468924157054</v>
+      </c>
+      <c r="H50" s="0" t="n">
+        <f aca="false">E50*B50</f>
+        <v>0.0965389968521242</v>
+      </c>
+      <c r="I50" s="0" t="n">
+        <f aca="false">E50*C50</f>
+        <v>0.0777277798057937</v>
+      </c>
+      <c r="K50" s="0" t="n">
+        <f aca="false">K47*(1-K47)</f>
+        <v>0.233937686635546</v>
+      </c>
+      <c r="L50" s="0" t="n">
+        <f aca="false">L47*(1-L47)</f>
+        <v>0.228258615247984</v>
+      </c>
+      <c r="M50" s="0" t="n">
+        <f aca="false">M47*(1-M47)</f>
+        <v>0.221459740790385</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="n">
+        <v>0.523820306050001</v>
+      </c>
+      <c r="B51" s="0" t="n">
+        <v>0.02830308332589</v>
+      </c>
+      <c r="C51" s="0" t="n">
+        <v>0.158328277745128</v>
+      </c>
+      <c r="E51" s="0" t="n">
+        <f aca="false">B38</f>
+        <v>0</v>
+      </c>
+      <c r="G51" s="0" t="n">
+        <f aca="false">E51*A51</f>
+        <v>0</v>
+      </c>
+      <c r="H51" s="0" t="n">
+        <f aca="false">E51*B51</f>
+        <v>0</v>
+      </c>
+      <c r="I51" s="0" t="n">
+        <f aca="false">E51*C51</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="n">
+        <v>0.607253439545515</v>
+      </c>
+      <c r="B52" s="0" t="n">
+        <v>0.975241618860578</v>
+      </c>
+      <c r="C52" s="0" t="n">
+        <v>0.079453623373872</v>
+      </c>
+      <c r="E52" s="0" t="n">
+        <f aca="false">C38</f>
+        <v>0.122561913243983</v>
+      </c>
+      <c r="G52" s="0" t="n">
+        <f aca="false">E52*A52</f>
+        <v>0.0744261433746876</v>
+      </c>
+      <c r="H52" s="0" t="n">
+        <f aca="false">E52*B52</f>
+        <v>0.119527478682712</v>
+      </c>
+      <c r="I52" s="0" t="n">
+        <f aca="false">E52*C52</f>
+        <v>0.00973798809486859</v>
+      </c>
+      <c r="K52" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L52" s="3"/>
+      <c r="M52" s="3"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="n">
+        <v>0.594808597683063</v>
+      </c>
+      <c r="B53" s="0" t="n">
+        <v>0.0591206513138753</v>
+      </c>
+      <c r="C53" s="0" t="n">
+        <v>0.692024587353112</v>
+      </c>
+      <c r="E53" s="0" t="n">
+        <f aca="false">A39</f>
+        <v>0.140523127955259</v>
+      </c>
+      <c r="G53" s="0" t="n">
+        <f aca="false">E53*A53</f>
+        <v>0.0835843646811054</v>
+      </c>
+      <c r="H53" s="0" t="n">
+        <f aca="false">E53*B53</f>
+        <v>0.00830781884937798</v>
+      </c>
+      <c r="I53" s="0" t="n">
+        <f aca="false">E53*C53</f>
+        <v>0.097245459636807</v>
+      </c>
+      <c r="K53" s="4" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="L53" s="0" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="M53" s="0" t="n">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="n">
+        <v>0.30152268100656</v>
+      </c>
+      <c r="B54" s="0" t="n">
+        <v>0.173266238182705</v>
+      </c>
+      <c r="C54" s="0" t="n">
+        <v>0.541099855008735</v>
+      </c>
+      <c r="E54" s="0" t="n">
+        <f aca="false">B39</f>
+        <v>0</v>
+      </c>
+      <c r="G54" s="0" t="n">
+        <f aca="false">E54*A54</f>
+        <v>0</v>
+      </c>
+      <c r="H54" s="0" t="n">
+        <f aca="false">E54*B54</f>
+        <v>0</v>
+      </c>
+      <c r="I54" s="0" t="n">
+        <f aca="false">E54*C54</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="n">
+        <v>0.544155573000885</v>
+      </c>
+      <c r="B55" s="0" t="n">
+        <v>0.278507621816109</v>
+      </c>
+      <c r="C55" s="0" t="n">
+        <v>0.423152201571828</v>
+      </c>
+      <c r="E55" s="0" t="n">
+        <f aca="false">C39</f>
+        <v>0</v>
+      </c>
+      <c r="G55" s="0" t="n">
+        <f aca="false">E55*A55</f>
+        <v>0</v>
+      </c>
+      <c r="H55" s="0" t="n">
+        <f aca="false">E55*B55</f>
+        <v>0</v>
+      </c>
+      <c r="I55" s="0" t="n">
+        <f aca="false">E55*C55</f>
+        <v>0</v>
+      </c>
+      <c r="K55" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L55" s="3"/>
+      <c r="M55" s="3"/>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K56" s="0" t="n">
+        <f aca="false">K53-K47</f>
+        <v>-0.306737182249149</v>
+      </c>
+      <c r="L56" s="0" t="n">
+        <f aca="false">L53-L47</f>
+        <v>-0.197449600718403</v>
+      </c>
+      <c r="M56" s="0" t="n">
+        <f aca="false">M53-M47</f>
+        <v>0.291061374429602</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K58" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L58" s="5"/>
+      <c r="M58" s="5"/>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K59" s="0" t="n">
+        <f aca="false">K56*K50</f>
+        <v>-0.0717573868204718</v>
+      </c>
+      <c r="L59" s="0" t="n">
+        <f aca="false">L56*L50</f>
+        <v>-0.0450695724412499</v>
+      </c>
+      <c r="M59" s="0" t="n">
+        <f aca="false">M56*M50</f>
+        <v>0.0644583765352729</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="16">
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="E12:G12"/>
@@ -1013,6 +1528,15 @@
     <mergeCell ref="A17:G17"/>
     <mergeCell ref="A26:G26"/>
     <mergeCell ref="A35:D35"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="G42:I42"/>
+    <mergeCell ref="K42:M42"/>
+    <mergeCell ref="K46:M46"/>
+    <mergeCell ref="K49:M49"/>
+    <mergeCell ref="K52:M52"/>
+    <mergeCell ref="K55:M55"/>
+    <mergeCell ref="K58:M58"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
eval fully connected gradients
</commit_message>
<xml_diff>
--- a/vika_conv2.xlsx
+++ b/vika_conv2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t xml:space="preserve">Изображение (8x9)</t>
   </si>
@@ -80,6 +80,12 @@
   </si>
   <si>
     <t xml:space="preserve">δ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">δ с весами</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сумма</t>
   </si>
 </sst>
 </file>
@@ -209,10 +215,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M59"/>
+  <dimension ref="A1:O73"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M54" activeCellId="0" sqref="M54"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q63" activeCellId="0" sqref="Q63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1486,16 +1492,16 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K56" s="0" t="n">
-        <f aca="false">K53-K47</f>
-        <v>-0.306737182249149</v>
+        <f aca="false">K47-K53</f>
+        <v>0.306737182249149</v>
       </c>
       <c r="L56" s="0" t="n">
-        <f aca="false">L53-L47</f>
-        <v>-0.197449600718403</v>
+        <f aca="false">L47-L53</f>
+        <v>0.197449600718403</v>
       </c>
       <c r="M56" s="0" t="n">
-        <f aca="false">M53-M47</f>
-        <v>0.291061374429602</v>
+        <f aca="false">M47-M53</f>
+        <v>-0.291061374429602</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1508,19 +1514,245 @@
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K59" s="0" t="n">
         <f aca="false">K56*K50</f>
-        <v>-0.0717573868204718</v>
+        <v>0.0717573868204718</v>
       </c>
       <c r="L59" s="0" t="n">
         <f aca="false">L56*L50</f>
-        <v>-0.0450695724412499</v>
+        <v>0.0450695724412499</v>
       </c>
       <c r="M59" s="0" t="n">
         <f aca="false">M56*M50</f>
-        <v>0.0644583765352729</v>
+        <v>-0.0644583765352729</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K61" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="L61" s="5"/>
+      <c r="M61" s="5"/>
+      <c r="O61" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K62" s="0" t="n">
+        <f aca="false">$K$59*A44</f>
+        <v>0.0215926487788863</v>
+      </c>
+      <c r="L62" s="0" t="n">
+        <f aca="false">$L$59*B44</f>
+        <v>0.0232204128829206</v>
+      </c>
+      <c r="M62" s="0" t="n">
+        <f aca="false">$M$59*C44</f>
+        <v>-0.0524459109696444</v>
+      </c>
+      <c r="O62" s="0" t="n">
+        <f aca="false">SUM(K62:M62)</f>
+        <v>-0.0076328493078375</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K63" s="0" t="n">
+        <f aca="false">$K$59*A45</f>
+        <v>0.0153750155865458</v>
+      </c>
+      <c r="L63" s="0" t="n">
+        <f aca="false">$L$59*B45</f>
+        <v>0.0171560567684248</v>
+      </c>
+      <c r="M63" s="0" t="n">
+        <f aca="false">$M$59*C45</f>
+        <v>-0.0205015135611059</v>
+      </c>
+      <c r="O63" s="0" t="n">
+        <f aca="false">SUM(K63:M63)</f>
+        <v>0.0120295587938647</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K64" s="0" t="n">
+        <f aca="false">$K$59*A46</f>
+        <v>0.0336463099768542</v>
+      </c>
+      <c r="L64" s="0" t="n">
+        <f aca="false">$L$59*B46</f>
+        <v>0.0127562281799747</v>
+      </c>
+      <c r="M64" s="0" t="n">
+        <f aca="false">$M$59*C46</f>
+        <v>-0.0188928698834043</v>
+      </c>
+      <c r="O64" s="0" t="n">
+        <f aca="false">SUM(K64:M64)</f>
+        <v>0.0275096682734246</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K65" s="0" t="n">
+        <f aca="false">$K$59*A47</f>
+        <v>0.0487293417738617</v>
+      </c>
+      <c r="L65" s="0" t="n">
+        <f aca="false">$L$59*B47</f>
+        <v>0.00985009263608588</v>
+      </c>
+      <c r="M65" s="0" t="n">
+        <f aca="false">$M$59*C47</f>
+        <v>-0.0130970962019592</v>
+      </c>
+      <c r="O65" s="0" t="n">
+        <f aca="false">SUM(K65:M65)</f>
+        <v>0.0454823382079884</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K66" s="0" t="n">
+        <f aca="false">$K$59*A48</f>
+        <v>0.0258951898518527</v>
+      </c>
+      <c r="L66" s="0" t="n">
+        <f aca="false">$L$59*B48</f>
+        <v>0.0257200005561683</v>
+      </c>
+      <c r="M66" s="0" t="n">
+        <f aca="false">$M$59*C48</f>
+        <v>-0.0555947978334647</v>
+      </c>
+      <c r="O66" s="0" t="n">
+        <f aca="false">SUM(K66:M66)</f>
+        <v>-0.00397960742544357</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K67" s="0" t="n">
+        <f aca="false">$K$59*A49</f>
+        <v>0.0210331122290416</v>
+      </c>
+      <c r="L67" s="0" t="n">
+        <f aca="false">$L$59*B49</f>
+        <v>0.0133893841192325</v>
+      </c>
+      <c r="M67" s="0" t="n">
+        <f aca="false">$M$59*C49</f>
+        <v>-0.0485096360958791</v>
+      </c>
+      <c r="O67" s="0" t="n">
+        <f aca="false">SUM(K67:M67)</f>
+        <v>-0.0140871397476051</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K68" s="0" t="n">
+        <f aca="false">$K$59*A50</f>
+        <v>0.014823831981344</v>
+      </c>
+      <c r="L68" s="0" t="n">
+        <f aca="false">$L$59*B50</f>
+        <v>0.0390002790544238</v>
+      </c>
+      <c r="M68" s="0" t="n">
+        <f aca="false">$M$59*C50</f>
+        <v>-0.0449093863250378</v>
+      </c>
+      <c r="O68" s="0" t="n">
+        <f aca="false">SUM(K68:M68)</f>
+        <v>0.00891472471072997</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K69" s="0" t="n">
+        <f aca="false">$K$59*A51</f>
+        <v>0.0375879763256478</v>
+      </c>
+      <c r="L69" s="0" t="n">
+        <f aca="false">$L$59*B51</f>
+        <v>0.00127560786426693</v>
+      </c>
+      <c r="M69" s="0" t="n">
+        <f aca="false">$M$59*C51</f>
+        <v>-0.0102055837430767</v>
+      </c>
+      <c r="O69" s="0" t="n">
+        <f aca="false">SUM(K69:M69)</f>
+        <v>0.0286580004468381</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K70" s="0" t="n">
+        <f aca="false">$K$59*A52</f>
+        <v>0.0435749199595295</v>
+      </c>
+      <c r="L70" s="0" t="n">
+        <f aca="false">$L$59*B52</f>
+        <v>0.0439537227889586</v>
+      </c>
+      <c r="M70" s="0" t="n">
+        <f aca="false">$M$59*C52</f>
+        <v>-0.0051214515725248</v>
+      </c>
+      <c r="O70" s="0" t="n">
+        <f aca="false">SUM(K70:M70)</f>
+        <v>0.0824071911759634</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K71" s="0" t="n">
+        <f aca="false">$K$59*A53</f>
+        <v>0.0426819106280859</v>
+      </c>
+      <c r="L71" s="0" t="n">
+        <f aca="false">$L$59*B53</f>
+        <v>0.00266454247716458</v>
+      </c>
+      <c r="M71" s="0" t="n">
+        <f aca="false">$M$59*C53</f>
+        <v>-0.0446067814232738</v>
+      </c>
+      <c r="O71" s="0" t="n">
+        <f aca="false">SUM(K71:M71)</f>
+        <v>0.000739671681976736</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K72" s="0" t="n">
+        <f aca="false">$K$59*A54</f>
+        <v>0.0216364796561335</v>
+      </c>
+      <c r="L72" s="0" t="n">
+        <f aca="false">$L$59*B54</f>
+        <v>0.00780903527339829</v>
+      </c>
+      <c r="M72" s="0" t="n">
+        <f aca="false">$M$59*C54</f>
+        <v>-0.0348784181973346</v>
+      </c>
+      <c r="O72" s="0" t="n">
+        <f aca="false">SUM(K72:M72)</f>
+        <v>-0.0054329032678029</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K73" s="0" t="n">
+        <f aca="false">$K$59*A55</f>
+        <v>0.03904718194234</v>
+      </c>
+      <c r="L73" s="0" t="n">
+        <f aca="false">$L$59*B55</f>
+        <v>0.0125522194368813</v>
+      </c>
+      <c r="M73" s="0" t="n">
+        <f aca="false">$M$59*C55</f>
+        <v>-0.0272757039406466</v>
+      </c>
+      <c r="O73" s="0" t="n">
+        <f aca="false">SUM(K73:M73)</f>
+        <v>0.0243236974385747</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="17">
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="E12:G12"/>
@@ -1537,6 +1769,7 @@
     <mergeCell ref="K52:M52"/>
     <mergeCell ref="K55:M55"/>
     <mergeCell ref="K58:M58"/>
+    <mergeCell ref="K61:M61"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
backpropagate + example for fully connected layer
</commit_message>
<xml_diff>
--- a/vika_conv2.xlsx
+++ b/vika_conv2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t xml:space="preserve">Изображение (8x9)</t>
   </si>
@@ -55,6 +55,9 @@
     <t xml:space="preserve">Выход</t>
   </si>
   <si>
+    <t xml:space="preserve">learning rate</t>
+  </si>
+  <si>
     <t xml:space="preserve">out1</t>
   </si>
   <si>
@@ -82,16 +85,36 @@
     <t xml:space="preserve">δ</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">сумма (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">δ * weight) * learning rate</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Output * сумма (δ * weight) * learning rate</t>
+  </si>
+  <si>
     <t xml:space="preserve">δ (выход) * w (выход-1)</t>
   </si>
   <si>
     <t xml:space="preserve">Сумма</t>
   </si>
   <si>
-    <t xml:space="preserve">delta W</t>
-  </si>
-  <si>
-    <t xml:space="preserve">learning rate</t>
+    <t xml:space="preserve">updated weights</t>
   </si>
 </sst>
 </file>
@@ -179,7 +202,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -204,6 +227,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -221,10 +248,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O73"/>
+  <dimension ref="A1:O89"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A30" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D64" activeCellId="0" sqref="D64"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A45" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A78" activeCellId="0" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1074,37 +1101,43 @@
       </c>
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
+      <c r="O42" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B43" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G43" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C43" s="0" t="s">
+      <c r="H43" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="E43" s="3" t="s">
+      <c r="I43" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="G43" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="H43" s="0" t="s">
+      <c r="K43" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="I43" s="0" t="s">
+      <c r="L43" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="K43" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="L43" s="0" t="s">
-        <v>12</v>
-      </c>
       <c r="M43" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="O43" s="0" t="n">
+        <v>0.3</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1200,7 +1233,7 @@
         <v>0.0707489664131254</v>
       </c>
       <c r="K46" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L46" s="3"/>
       <c r="M46" s="3"/>
@@ -1298,7 +1331,7 @@
         <v>0.0656249367548498</v>
       </c>
       <c r="K49" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L49" s="3"/>
       <c r="M49" s="3"/>
@@ -1396,7 +1429,7 @@
         <v>0.00973798809486859</v>
       </c>
       <c r="K52" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L52" s="3"/>
       <c r="M52" s="3"/>
@@ -1491,7 +1524,7 @@
         <v>0</v>
       </c>
       <c r="K55" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L55" s="3"/>
       <c r="M55" s="3"/>
@@ -1512,7 +1545,7 @@
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K58" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L58" s="5"/>
       <c r="M58" s="5"/>
@@ -1532,23 +1565,50 @@
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+      <c r="E61" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F61" s="3"/>
+      <c r="G61" s="3"/>
       <c r="K61" s="5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="L61" s="5"/>
       <c r="M61" s="5"/>
       <c r="O61" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B62" s="3"/>
-      <c r="C62" s="3"/>
-      <c r="H62" s="0" t="s">
-        <v>23</v>
+      <c r="A62" s="6" t="n">
+        <f aca="false">K62*$O$43</f>
+        <v>0.0064777946336659</v>
+      </c>
+      <c r="B62" s="6" t="n">
+        <f aca="false">L62*$O$43</f>
+        <v>0.00696612386487618</v>
+      </c>
+      <c r="C62" s="6" t="n">
+        <f aca="false">M62*$O$43</f>
+        <v>-0.0157337732908933</v>
+      </c>
+      <c r="D62" s="6"/>
+      <c r="E62" s="2" t="n">
+        <f aca="false">A62*$E44</f>
+        <v>0.00194164631634474</v>
+      </c>
+      <c r="F62" s="2" t="n">
+        <f aca="false">B62*$E44</f>
+        <v>0.00208801752854945</v>
+      </c>
+      <c r="G62" s="2" t="n">
+        <f aca="false">C62*$E44</f>
+        <v>-0.00471602214644118</v>
       </c>
       <c r="K62" s="0" t="n">
         <f aca="false">$K$59*A44</f>
@@ -1568,17 +1628,30 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B63" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C63" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H63" s="0" t="n">
-        <v>0.3</v>
+      <c r="A63" s="6" t="n">
+        <f aca="false">K63*$O$43</f>
+        <v>0.00461250467596373</v>
+      </c>
+      <c r="B63" s="6" t="n">
+        <f aca="false">L63*$O$43</f>
+        <v>0.00514681703052743</v>
+      </c>
+      <c r="C63" s="6" t="n">
+        <f aca="false">M63*$O$43</f>
+        <v>-0.00615045406833176</v>
+      </c>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2" t="n">
+        <f aca="false">A63*$E45</f>
+        <v>0.00104920747276621</v>
+      </c>
+      <c r="F63" s="2" t="n">
+        <f aca="false">B63*$E45</f>
+        <v>0.00117074762385179</v>
+      </c>
+      <c r="G63" s="2" t="n">
+        <f aca="false">C63*$E45</f>
+        <v>-0.00139904516585682</v>
       </c>
       <c r="K63" s="0" t="n">
         <f aca="false">$K$59*A45</f>
@@ -1598,17 +1671,30 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="n">
-        <f aca="false">$H$63*K62*E44</f>
-        <v>0.00194164631634474</v>
-      </c>
-      <c r="B64" s="0" t="n">
-        <f aca="false">$H$63*L62*E44</f>
-        <v>0.00208801752854945</v>
-      </c>
-      <c r="C64" s="0" t="n">
-        <f aca="false">$H$63*M62*E44</f>
-        <v>-0.00471602214644118</v>
+      <c r="A64" s="6" t="n">
+        <f aca="false">K64*$O$43</f>
+        <v>0.0100938929930563</v>
+      </c>
+      <c r="B64" s="6" t="n">
+        <f aca="false">L64*$O$43</f>
+        <v>0.00382686845399242</v>
+      </c>
+      <c r="C64" s="6" t="n">
+        <f aca="false">M64*$O$43</f>
+        <v>-0.0056678609650213</v>
+      </c>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2" t="n">
+        <f aca="false">A64*$E46</f>
+        <v>0.00243646527126159</v>
+      </c>
+      <c r="F64" s="2" t="n">
+        <f aca="false">B64*$E46</f>
+        <v>0.00092373003084669</v>
+      </c>
+      <c r="G64" s="2" t="n">
+        <f aca="false">C64*$E46</f>
+        <v>-0.00136810905496158</v>
       </c>
       <c r="K64" s="0" t="n">
         <f aca="false">$K$59*A46</f>
@@ -1628,17 +1714,30 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="n">
-        <f aca="false">$H$63*K63*E45</f>
-        <v>0.00104920747276621</v>
-      </c>
-      <c r="B65" s="0" t="n">
-        <f aca="false">$H$63*L63*E45</f>
-        <v>0.00117074762385179</v>
-      </c>
-      <c r="C65" s="0" t="n">
-        <f aca="false">$H$63*M63*E45</f>
-        <v>-0.00139904516585682</v>
+      <c r="A65" s="6" t="n">
+        <f aca="false">K65*$O$43</f>
+        <v>0.0146188025321585</v>
+      </c>
+      <c r="B65" s="6" t="n">
+        <f aca="false">L65*$O$43</f>
+        <v>0.00295502779082577</v>
+      </c>
+      <c r="C65" s="6" t="n">
+        <f aca="false">M65*$O$43</f>
+        <v>-0.00392912886058776</v>
+      </c>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2" t="n">
+        <f aca="false">A65*$E47</f>
+        <v>0.000784173768650395</v>
+      </c>
+      <c r="F65" s="2" t="n">
+        <f aca="false">B65*$E47</f>
+        <v>0.000158511976210157</v>
+      </c>
+      <c r="G65" s="2" t="n">
+        <f aca="false">C65*$E47</f>
+        <v>-0.000210764170276072</v>
       </c>
       <c r="K65" s="0" t="n">
         <f aca="false">$K$59*A47</f>
@@ -1658,17 +1757,30 @@
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="n">
-        <f aca="false">$H$63*K64*E46</f>
-        <v>0.00243646527126159</v>
-      </c>
-      <c r="B66" s="0" t="n">
-        <f aca="false">$H$63*L64*E46</f>
-        <v>0.00092373003084669</v>
-      </c>
-      <c r="C66" s="0" t="n">
-        <f aca="false">$H$63*M64*E46</f>
-        <v>-0.00136810905496158</v>
+      <c r="A66" s="6" t="n">
+        <f aca="false">K66*$O$43</f>
+        <v>0.00776855695555582</v>
+      </c>
+      <c r="B66" s="6" t="n">
+        <f aca="false">L66*$O$43</f>
+        <v>0.0077160001668505</v>
+      </c>
+      <c r="C66" s="6" t="n">
+        <f aca="false">M66*$O$43</f>
+        <v>-0.0166784393500394</v>
+      </c>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2" t="n">
+        <f aca="false">A66*$E48</f>
+        <v>0.000496975924085803</v>
+      </c>
+      <c r="F66" s="2" t="n">
+        <f aca="false">B66*$E48</f>
+        <v>0.000493613721969858</v>
+      </c>
+      <c r="G66" s="2" t="n">
+        <f aca="false">C66*$E48</f>
+        <v>-0.00106696557104688</v>
       </c>
       <c r="K66" s="0" t="n">
         <f aca="false">$K$59*A48</f>
@@ -1688,17 +1800,30 @@
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="n">
-        <f aca="false">$H$63*K65*E47</f>
-        <v>0.000784173768650395</v>
-      </c>
-      <c r="B67" s="0" t="n">
-        <f aca="false">$H$63*L65*E47</f>
-        <v>0.000158511976210157</v>
-      </c>
-      <c r="C67" s="0" t="n">
-        <f aca="false">$H$63*M65*E47</f>
-        <v>-0.000210764170276072</v>
+      <c r="A67" s="6" t="n">
+        <f aca="false">K67*$O$43</f>
+        <v>0.00630993366871247</v>
+      </c>
+      <c r="B67" s="6" t="n">
+        <f aca="false">L67*$O$43</f>
+        <v>0.00401681523576975</v>
+      </c>
+      <c r="C67" s="6" t="n">
+        <f aca="false">M67*$O$43</f>
+        <v>-0.0145528908287637</v>
+      </c>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2" t="n">
+        <f aca="false">A67*$E49</f>
+        <v>0.00055023097875549</v>
+      </c>
+      <c r="F67" s="2" t="n">
+        <f aca="false">B67*$E49</f>
+        <v>0.000350269320518632</v>
+      </c>
+      <c r="G67" s="2" t="n">
+        <f aca="false">C67*$E49</f>
+        <v>-0.00126902306503427</v>
       </c>
       <c r="K67" s="0" t="n">
         <f aca="false">$K$59*A49</f>
@@ -1718,17 +1843,30 @@
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="n">
-        <f aca="false">$H$63*K66*E48</f>
-        <v>0.000496975924085803</v>
-      </c>
-      <c r="B68" s="0" t="n">
-        <f aca="false">$H$63*L66*E48</f>
-        <v>0.000493613721969858</v>
-      </c>
-      <c r="C68" s="0" t="n">
-        <f aca="false">$H$63*M66*E48</f>
-        <v>-0.00106696557104688</v>
+      <c r="A68" s="6" t="n">
+        <f aca="false">K68*$O$43</f>
+        <v>0.00444714959440321</v>
+      </c>
+      <c r="B68" s="6" t="n">
+        <f aca="false">L68*$O$43</f>
+        <v>0.0117000837163271</v>
+      </c>
+      <c r="C68" s="6" t="n">
+        <f aca="false">M68*$O$43</f>
+        <v>-0.0134728158975113</v>
+      </c>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2" t="n">
+        <f aca="false">A68*$E50</f>
+        <v>0.000496135432225071</v>
+      </c>
+      <c r="F68" s="2" t="n">
+        <f aca="false">B68*$E50</f>
+        <v>0.00130529139360972</v>
+      </c>
+      <c r="G68" s="2" t="n">
+        <f aca="false">C68*$E50</f>
+        <v>-0.00150306194939179</v>
       </c>
       <c r="K68" s="0" t="n">
         <f aca="false">$K$59*A50</f>
@@ -1748,17 +1886,30 @@
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="n">
-        <f aca="false">$H$63*K67*E49</f>
-        <v>0.00055023097875549</v>
-      </c>
-      <c r="B69" s="0" t="n">
-        <f aca="false">$H$63*L67*E49</f>
-        <v>0.000350269320518632</v>
-      </c>
-      <c r="C69" s="0" t="n">
-        <f aca="false">$H$63*M67*E49</f>
-        <v>-0.00126902306503427</v>
+      <c r="A69" s="6" t="n">
+        <f aca="false">K69*$O$43</f>
+        <v>0.0112763928976944</v>
+      </c>
+      <c r="B69" s="6" t="n">
+        <f aca="false">L69*$O$43</f>
+        <v>0.000382682359280079</v>
+      </c>
+      <c r="C69" s="6" t="n">
+        <f aca="false">M69*$O$43</f>
+        <v>-0.00306167512292301</v>
+      </c>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2" t="n">
+        <f aca="false">A69*$E51</f>
+        <v>0</v>
+      </c>
+      <c r="F69" s="2" t="n">
+        <f aca="false">B69*$E51</f>
+        <v>0</v>
+      </c>
+      <c r="G69" s="2" t="n">
+        <f aca="false">C69*$E51</f>
+        <v>-0</v>
       </c>
       <c r="K69" s="0" t="n">
         <f aca="false">$K$59*A51</f>
@@ -1778,17 +1929,30 @@
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="n">
-        <f aca="false">$H$63*K68*E50</f>
-        <v>0.000496135432225071</v>
-      </c>
-      <c r="B70" s="0" t="n">
-        <f aca="false">$H$63*L68*E50</f>
-        <v>0.00130529139360972</v>
-      </c>
-      <c r="C70" s="0" t="n">
-        <f aca="false">$H$63*M68*E50</f>
-        <v>-0.00150306194939179</v>
+      <c r="A70" s="6" t="n">
+        <f aca="false">K70*$O$43</f>
+        <v>0.0130724759878589</v>
+      </c>
+      <c r="B70" s="6" t="n">
+        <f aca="false">L70*$O$43</f>
+        <v>0.0131861168366876</v>
+      </c>
+      <c r="C70" s="6" t="n">
+        <f aca="false">M70*$O$43</f>
+        <v>-0.00153643547175744</v>
+      </c>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2" t="n">
+        <f aca="false">A70*$E52</f>
+        <v>0.00160218766790801</v>
+      </c>
+      <c r="F70" s="2" t="n">
+        <f aca="false">B70*$E52</f>
+        <v>0.00161611570776313</v>
+      </c>
+      <c r="G70" s="2" t="n">
+        <f aca="false">C70*$E52</f>
+        <v>-0.000188308470994513</v>
       </c>
       <c r="K70" s="0" t="n">
         <f aca="false">$K$59*A52</f>
@@ -1808,17 +1972,30 @@
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="n">
-        <f aca="false">$H$63*K69*E51</f>
-        <v>0</v>
-      </c>
-      <c r="B71" s="0" t="n">
-        <f aca="false">$H$63*L69*E51</f>
-        <v>0</v>
-      </c>
-      <c r="C71" s="0" t="n">
-        <f aca="false">$H$63*M69*E51</f>
-        <v>-0</v>
+      <c r="A71" s="6" t="n">
+        <f aca="false">K71*$O$43</f>
+        <v>0.0128045731884258</v>
+      </c>
+      <c r="B71" s="6" t="n">
+        <f aca="false">L71*$O$43</f>
+        <v>0.000799362743149373</v>
+      </c>
+      <c r="C71" s="6" t="n">
+        <f aca="false">M71*$O$43</f>
+        <v>-0.0133820344269821</v>
+      </c>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2" t="n">
+        <f aca="false">A71*$E53</f>
+        <v>0.00179933867656964</v>
+      </c>
+      <c r="F71" s="2" t="n">
+        <f aca="false">B71*$E53</f>
+        <v>0.000112328953038247</v>
+      </c>
+      <c r="G71" s="2" t="n">
+        <f aca="false">C71*$E53</f>
+        <v>-0.0018804853360845</v>
       </c>
       <c r="K71" s="0" t="n">
         <f aca="false">$K$59*A53</f>
@@ -1838,17 +2015,30 @@
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="n">
-        <f aca="false">$H$63*K70*E52</f>
-        <v>0.00160218766790801</v>
-      </c>
-      <c r="B72" s="0" t="n">
-        <f aca="false">$H$63*L70*E52</f>
-        <v>0.00161611570776313</v>
-      </c>
-      <c r="C72" s="0" t="n">
-        <f aca="false">$H$63*M70*E52</f>
-        <v>-0.000188308470994513</v>
+      <c r="A72" s="6" t="n">
+        <f aca="false">K72*$O$43</f>
+        <v>0.00649094389684004</v>
+      </c>
+      <c r="B72" s="6" t="n">
+        <f aca="false">L72*$O$43</f>
+        <v>0.00234271058201949</v>
+      </c>
+      <c r="C72" s="6" t="n">
+        <f aca="false">M72*$O$43</f>
+        <v>-0.0104635254592004</v>
+      </c>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2" t="n">
+        <f aca="false">A72*$E54</f>
+        <v>0</v>
+      </c>
+      <c r="F72" s="2" t="n">
+        <f aca="false">B72*$E54</f>
+        <v>0</v>
+      </c>
+      <c r="G72" s="2" t="n">
+        <f aca="false">C72*$E54</f>
+        <v>-0</v>
       </c>
       <c r="K72" s="0" t="n">
         <f aca="false">$K$59*A54</f>
@@ -1868,17 +2058,30 @@
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="n">
-        <f aca="false">$H$63*K71*E53</f>
-        <v>0.00179933867656964</v>
-      </c>
-      <c r="B73" s="0" t="n">
-        <f aca="false">$H$63*L71*E53</f>
-        <v>0.000112328953038247</v>
-      </c>
-      <c r="C73" s="0" t="n">
-        <f aca="false">$H$63*M71*E53</f>
-        <v>-0.0018804853360845</v>
+      <c r="A73" s="6" t="n">
+        <f aca="false">K73*$O$43</f>
+        <v>0.011714154582702</v>
+      </c>
+      <c r="B73" s="6" t="n">
+        <f aca="false">L73*$O$43</f>
+        <v>0.0037656658310644</v>
+      </c>
+      <c r="C73" s="6" t="n">
+        <f aca="false">M73*$O$43</f>
+        <v>-0.00818271118219398</v>
+      </c>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2" t="n">
+        <f aca="false">A73*$E55</f>
+        <v>0</v>
+      </c>
+      <c r="F73" s="2" t="n">
+        <f aca="false">B73*$E55</f>
+        <v>0</v>
+      </c>
+      <c r="G73" s="2" t="n">
+        <f aca="false">C73*$E55</f>
+        <v>-0</v>
       </c>
       <c r="K73" s="0" t="n">
         <f aca="false">$K$59*A55</f>
@@ -1897,8 +2100,199 @@
         <v>0.0243236974385747</v>
       </c>
     </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="2"/>
+      <c r="B74" s="2"/>
+      <c r="C74" s="2"/>
+      <c r="D74" s="2"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="2"/>
+      <c r="B75" s="2"/>
+      <c r="C75" s="2"/>
+      <c r="D75" s="2"/>
+      <c r="E75" s="2"/>
+      <c r="F75" s="2"/>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B77" s="3"/>
+      <c r="C77" s="3"/>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="n">
+        <f aca="false">A44+E62</f>
+        <v>0.302853506901632</v>
+      </c>
+      <c r="B78" s="0" t="n">
+        <f aca="false">B44+F62</f>
+        <v>0.517300646030615</v>
+      </c>
+      <c r="C78" s="0" t="n">
+        <f aca="false">C44+G62</f>
+        <v>0.808923938843656</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="n">
+        <f aca="false">A45+E63</f>
+        <v>0.215313080055141</v>
+      </c>
+      <c r="B79" s="0" t="n">
+        <f aca="false">B45+F63</f>
+        <v>0.381827936923538</v>
+      </c>
+      <c r="C79" s="0" t="n">
+        <f aca="false">C45+G63</f>
+        <v>0.316659129164473</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="n">
+        <f aca="false">A46+E64</f>
+        <v>0.471326310173685</v>
+      </c>
+      <c r="B80" s="0" t="n">
+        <f aca="false">B46+F64</f>
+        <v>0.283957881211292</v>
+      </c>
+      <c r="C80" s="0" t="n">
+        <f aca="false">C46+G64</f>
+        <v>0.291733748281854</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="n">
+        <f aca="false">A47+E65</f>
+        <v>0.679868849688867</v>
+      </c>
+      <c r="B81" s="0" t="n">
+        <f aca="false">B47+F65</f>
+        <v>0.218711564568974</v>
+      </c>
+      <c r="C81" s="0" t="n">
+        <f aca="false">C47+G65</f>
+        <v>0.202976112477047</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="n">
+        <f aca="false">A48+E66</f>
+        <v>0.361368392780992</v>
+      </c>
+      <c r="B82" s="0" t="n">
+        <f aca="false">B48+F66</f>
+        <v>0.571166889792992</v>
+      </c>
+      <c r="C82" s="0" t="n">
+        <f aca="false">C48+G66</f>
+        <v>0.861424471876839</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="n">
+        <f aca="false">A49+E67</f>
+        <v>0.293664475532614</v>
+      </c>
+      <c r="B83" s="0" t="n">
+        <f aca="false">B49+F67</f>
+        <v>0.29743283287681</v>
+      </c>
+      <c r="C83" s="0" t="n">
+        <f aca="false">C49+G67</f>
+        <v>0.751304012486578</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="n">
+        <f aca="false">A50+E68</f>
+        <v>0.207078797345924</v>
+      </c>
+      <c r="B84" s="0" t="n">
+        <f aca="false">B50+F68</f>
+        <v>0.866640304395171</v>
+      </c>
+      <c r="C84" s="0" t="n">
+        <f aca="false">C50+G68</f>
+        <v>0.695216103797243</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="n">
+        <f aca="false">A51+E69</f>
+        <v>0.523820306050001</v>
+      </c>
+      <c r="B85" s="0" t="n">
+        <f aca="false">B51+F69</f>
+        <v>0.02830308332589</v>
+      </c>
+      <c r="C85" s="0" t="n">
+        <f aca="false">C51+G69</f>
+        <v>0.158328277745128</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="n">
+        <f aca="false">A52+E70</f>
+        <v>0.608855627213423</v>
+      </c>
+      <c r="B86" s="0" t="n">
+        <f aca="false">B52+F70</f>
+        <v>0.976857734568342</v>
+      </c>
+      <c r="C86" s="0" t="n">
+        <f aca="false">C52+G70</f>
+        <v>0.0792653149028775</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="n">
+        <f aca="false">A53+E71</f>
+        <v>0.596607936359632</v>
+      </c>
+      <c r="B87" s="0" t="n">
+        <f aca="false">B53+F71</f>
+        <v>0.0592329802669135</v>
+      </c>
+      <c r="C87" s="0" t="n">
+        <f aca="false">C53+G71</f>
+        <v>0.690144102017027</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="n">
+        <f aca="false">A54+E72</f>
+        <v>0.30152268100656</v>
+      </c>
+      <c r="B88" s="0" t="n">
+        <f aca="false">B54+F72</f>
+        <v>0.173266238182705</v>
+      </c>
+      <c r="C88" s="0" t="n">
+        <f aca="false">C54+G72</f>
+        <v>0.541099855008735</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="n">
+        <f aca="false">A55+E73</f>
+        <v>0.544155573000885</v>
+      </c>
+      <c r="B89" s="0" t="n">
+        <f aca="false">B55+F73</f>
+        <v>0.278507621816109</v>
+      </c>
+      <c r="C89" s="0" t="n">
+        <f aca="false">C55+G73</f>
+        <v>0.423152201571828</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="20">
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="E12:G12"/>
@@ -1915,8 +2309,10 @@
     <mergeCell ref="K52:M52"/>
     <mergeCell ref="K55:M55"/>
     <mergeCell ref="K58:M58"/>
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="E61:G61"/>
     <mergeCell ref="K61:M61"/>
-    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="A77:C77"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
sort tensor data, add pooled indecies to maxpool layer, cal gradients for maxpool layer
</commit_message>
<xml_diff>
--- a/vika_conv2.xlsx
+++ b/vika_conv2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t xml:space="preserve">Изображение (8x9)</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t xml:space="preserve">ReLU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maxpooling local gradients</t>
   </si>
   <si>
     <t xml:space="preserve">Maxpooling</t>
@@ -144,7 +147,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -153,8 +156,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF87D1D1"/>
+        <bgColor rgb="FFC0C0C0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor rgb="FFC0C0C0"/>
+        <bgColor rgb="FF87D1D1"/>
       </patternFill>
     </fill>
   </fills>
@@ -192,13 +201,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -209,7 +222,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -217,7 +230,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -276,7 +289,7 @@
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FF87D1D1"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
@@ -308,8 +321,8 @@
   </sheetPr>
   <dimension ref="A1:O104"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A69" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D78" activeCellId="0" sqref="D78"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N34" activeCellId="0" sqref="N34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -876,7 +889,7 @@
         <v>-1.13737952260659</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>5</v>
       </c>
@@ -886,9 +899,18 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
-    </row>
-    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="n">
+      <c r="I26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="2" t="n">
         <f aca="false">IF(A18&lt;0,0,A18)</f>
         <v>0.29973878860774</v>
       </c>
@@ -896,7 +918,7 @@
         <f aca="false">IF(B18&lt;0,0,B18)</f>
         <v>0.14573618884283</v>
       </c>
-      <c r="C27" s="0" t="n">
+      <c r="C27" s="2" t="n">
         <f aca="false">IF(C18&lt;0,0,C18)</f>
         <v>0.227470224200259</v>
       </c>
@@ -908,12 +930,36 @@
         <f aca="false">IF(E18&lt;0,0,E18)</f>
         <v>0.181724188351327</v>
       </c>
-      <c r="F27" s="0" t="n">
+      <c r="F27" s="2" t="n">
         <f aca="false">IF(F18&lt;0,0,F18)</f>
         <v>0.24138013677554</v>
       </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I27" s="2" t="n">
+        <f aca="false">A76</f>
+        <v>0.0141965350688645</v>
+      </c>
+      <c r="J27" s="0" t="n">
+        <f aca="false">IF(J18&lt;0,0,J18)</f>
+        <v>0</v>
+      </c>
+      <c r="K27" s="2" t="n">
+        <f aca="false">A77</f>
+        <v>0.0228260392577935</v>
+      </c>
+      <c r="L27" s="0" t="n">
+        <f aca="false">IF(L18&lt;0,0,L18)</f>
+        <v>0</v>
+      </c>
+      <c r="M27" s="0" t="n">
+        <f aca="false">IF(M18&lt;0,0,M18)</f>
+        <v>0</v>
+      </c>
+      <c r="N27" s="2" t="n">
+        <f aca="false">A78</f>
+        <v>0.0393891869125942</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
         <f aca="false">IF(A19&lt;0,0,A19)</f>
         <v>0</v>
@@ -938,8 +984,32 @@
         <f aca="false">IF(F19&lt;0,0,F19)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I28" s="0" t="n">
+        <f aca="false">IF(I19&lt;0,0,I19)</f>
+        <v>0</v>
+      </c>
+      <c r="J28" s="0" t="n">
+        <f aca="false">IF(J19&lt;0,0,J19)</f>
+        <v>0</v>
+      </c>
+      <c r="K28" s="0" t="n">
+        <f aca="false">IF(K19&lt;0,0,K19)</f>
+        <v>0</v>
+      </c>
+      <c r="L28" s="0" t="n">
+        <f aca="false">IF(L19&lt;0,0,L19)</f>
+        <v>0</v>
+      </c>
+      <c r="M28" s="0" t="n">
+        <f aca="false">IF(M19&lt;0,0,M19)</f>
+        <v>0</v>
+      </c>
+      <c r="N28" s="0" t="n">
+        <f aca="false">IF(N19&lt;0,0,N19)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
         <f aca="false">IF(A20&lt;0,0,A20)</f>
         <v>0</v>
@@ -964,9 +1034,33 @@
         <f aca="false">IF(F20&lt;0,0,F20)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="n">
+      <c r="I29" s="0" t="n">
+        <f aca="false">IF(I20&lt;0,0,I20)</f>
+        <v>0</v>
+      </c>
+      <c r="J29" s="0" t="n">
+        <f aca="false">IF(J20&lt;0,0,J20)</f>
+        <v>0</v>
+      </c>
+      <c r="K29" s="0" t="n">
+        <f aca="false">IF(K20&lt;0,0,K20)</f>
+        <v>0</v>
+      </c>
+      <c r="L29" s="0" t="n">
+        <f aca="false">IF(L20&lt;0,0,L20)</f>
+        <v>0</v>
+      </c>
+      <c r="M29" s="0" t="n">
+        <f aca="false">IF(M20&lt;0,0,M20)</f>
+        <v>0</v>
+      </c>
+      <c r="N29" s="0" t="n">
+        <f aca="false">IF(N20&lt;0,0,N20)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="2" t="n">
         <f aca="false">IF(A21&lt;0,0,A21)</f>
         <v>0.0536414502436412</v>
       </c>
@@ -978,7 +1072,7 @@
         <f aca="false">IF(C21&lt;0,0,C21)</f>
         <v>0</v>
       </c>
-      <c r="D30" s="0" t="n">
+      <c r="D30" s="2" t="n">
         <f aca="false">IF(D21&lt;0,0,D21)</f>
         <v>0.0639727464095352</v>
       </c>
@@ -986,12 +1080,36 @@
         <f aca="false">IF(E21&lt;0,0,E21)</f>
         <v>0.0539002998319844</v>
       </c>
-      <c r="F30" s="0" t="n">
+      <c r="F30" s="2" t="n">
         <f aca="false">IF(F21&lt;0,0,F21)</f>
         <v>0.0872007548167718</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I30" s="2" t="n">
+        <f aca="false">A79</f>
+        <v>0.057093090804489</v>
+      </c>
+      <c r="J30" s="0" t="n">
+        <f aca="false">IF(J21&lt;0,0,J21)</f>
+        <v>0</v>
+      </c>
+      <c r="K30" s="0" t="n">
+        <f aca="false">IF(K21&lt;0,0,K21)</f>
+        <v>0</v>
+      </c>
+      <c r="L30" s="2" t="n">
+        <f aca="false">A80</f>
+        <v>0.0197294245364713</v>
+      </c>
+      <c r="M30" s="0" t="n">
+        <f aca="false">IF(M21&lt;0,0,M21)</f>
+        <v>0</v>
+      </c>
+      <c r="N30" s="2" t="n">
+        <f aca="false">A81</f>
+        <v>0.00484691506609497</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
         <f aca="false">IF(A22&lt;0,0,A22)</f>
         <v>0.0826020094808472</v>
@@ -1000,7 +1118,7 @@
         <f aca="false">IF(B22&lt;0,0,B22)</f>
         <v>0</v>
       </c>
-      <c r="C31" s="0" t="n">
+      <c r="C31" s="2" t="n">
         <f aca="false">IF(C22&lt;0,0,C22)</f>
         <v>0</v>
       </c>
@@ -1016,9 +1134,33 @@
         <f aca="false">IF(F22&lt;0,0,F22)</f>
         <v>0.088960978417416</v>
       </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="n">
+      <c r="I31" s="0" t="n">
+        <f aca="false">IF(I22&lt;0,0,I22)</f>
+        <v>0</v>
+      </c>
+      <c r="J31" s="0" t="n">
+        <f aca="false">IF(J22&lt;0,0,J22)</f>
+        <v>0</v>
+      </c>
+      <c r="K31" s="2" t="n">
+        <f aca="false">A82</f>
+        <v>0.0304320382368629</v>
+      </c>
+      <c r="L31" s="0" t="n">
+        <f aca="false">IF(L22&lt;0,0,L22)</f>
+        <v>0</v>
+      </c>
+      <c r="M31" s="0" t="n">
+        <f aca="false">IF(M22&lt;0,0,M22)</f>
+        <v>0</v>
+      </c>
+      <c r="N31" s="0" t="n">
+        <f aca="false">IF(N22&lt;0,0,N22)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="2" t="n">
         <f aca="false">IF(A23&lt;0,0,A23)</f>
         <v>0.111562568718053</v>
       </c>
@@ -1038,13 +1180,37 @@
         <f aca="false">IF(E23&lt;0,0,E23)</f>
         <v>0</v>
       </c>
-      <c r="F32" s="0" t="n">
+      <c r="F32" s="2" t="n">
         <f aca="false">IF(F23&lt;0,0,F23)</f>
         <v>0.122561913243983</v>
       </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="n">
+      <c r="I32" s="2" t="n">
+        <f aca="false">A83</f>
+        <v>0.0365566994654057</v>
+      </c>
+      <c r="J32" s="0" t="n">
+        <f aca="false">IF(J23&lt;0,0,J23)</f>
+        <v>0</v>
+      </c>
+      <c r="K32" s="0" t="n">
+        <f aca="false">IF(K23&lt;0,0,K23)</f>
+        <v>0</v>
+      </c>
+      <c r="L32" s="0" t="n">
+        <f aca="false">IF(L23&lt;0,0,L23)</f>
+        <v>0</v>
+      </c>
+      <c r="M32" s="0" t="n">
+        <f aca="false">IF(M23&lt;0,0,M23)</f>
+        <v>0</v>
+      </c>
+      <c r="N32" s="2" t="n">
+        <f aca="false">A84</f>
+        <v>0.0969334222788538</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="2" t="n">
         <f aca="false">IF(A24&lt;0,0,A24)</f>
         <v>0.140523127955259</v>
       </c>
@@ -1052,7 +1218,7 @@
         <f aca="false">IF(B24&lt;0,0,B24)</f>
         <v>0</v>
       </c>
-      <c r="C33" s="0" t="n">
+      <c r="C33" s="2" t="n">
         <f aca="false">IF(C24&lt;0,0,C24)</f>
         <v>0</v>
       </c>
@@ -1060,7 +1226,7 @@
         <f aca="false">IF(D24&lt;0,0,D24)</f>
         <v>0</v>
       </c>
-      <c r="E33" s="0" t="n">
+      <c r="E33" s="2" t="n">
         <f aca="false">IF(E24&lt;0,0,E24)</f>
         <v>0</v>
       </c>
@@ -1068,10 +1234,34 @@
         <f aca="false">IF(F24&lt;0,0,F24)</f>
         <v>0</v>
       </c>
+      <c r="I33" s="2" t="n">
+        <f aca="false">A85</f>
+        <v>0.0194337868222081</v>
+      </c>
+      <c r="J33" s="0" t="n">
+        <f aca="false">IF(J24&lt;0,0,J24)</f>
+        <v>0</v>
+      </c>
+      <c r="K33" s="2" t="n">
+        <f aca="false">A86</f>
+        <v>0.00868917434519041</v>
+      </c>
+      <c r="L33" s="0" t="n">
+        <f aca="false">IF(L24&lt;0,0,L24)</f>
+        <v>0</v>
+      </c>
+      <c r="M33" s="2" t="n">
+        <f aca="false">A87</f>
+        <v>0.0392648873210714</v>
+      </c>
+      <c r="N33" s="0" t="n">
+        <f aca="false">IF(N24&lt;0,0,N24)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1134,58 +1324,58 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="E42" s="2" t="s">
+      <c r="A42" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G42" s="2" t="s">
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="E42" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="K42" s="2" t="s">
+      <c r="G42" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L42" s="2"/>
-      <c r="M42" s="2"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+      <c r="K42" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L42" s="3"/>
+      <c r="M42" s="3"/>
       <c r="O42" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B43" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G43" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="C43" s="0" t="s">
+      <c r="H43" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="E43" s="2" t="s">
+      <c r="I43" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="G43" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="H43" s="0" t="s">
+      <c r="K43" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="I43" s="0" t="s">
+      <c r="L43" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="K43" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="L43" s="0" t="s">
-        <v>13</v>
-      </c>
       <c r="M43" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="O43" s="0" t="n">
         <v>-0.1</v>
@@ -1283,11 +1473,11 @@
         <f aca="false">E46*C46</f>
         <v>0.0707489664131252</v>
       </c>
-      <c r="K46" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L46" s="2"/>
-      <c r="M46" s="2"/>
+      <c r="K46" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L46" s="3"/>
+      <c r="M46" s="3"/>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
@@ -1381,11 +1571,11 @@
         <f aca="false">E49*C49</f>
         <v>0.0656249367548498</v>
       </c>
-      <c r="K49" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L49" s="2"/>
-      <c r="M49" s="2"/>
+      <c r="K49" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L49" s="3"/>
+      <c r="M49" s="3"/>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="n">
@@ -1479,11 +1669,11 @@
         <f aca="false">E52*C52</f>
         <v>0.00973798809486858</v>
       </c>
-      <c r="K52" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L52" s="2"/>
-      <c r="M52" s="2"/>
+      <c r="K52" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L52" s="3"/>
+      <c r="M52" s="3"/>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="n">
@@ -1511,7 +1701,7 @@
         <f aca="false">E53*C53</f>
         <v>0.097245459636807</v>
       </c>
-      <c r="K53" s="3" t="n">
+      <c r="K53" s="4" t="n">
         <v>0.32</v>
       </c>
       <c r="L53" s="0" t="n">
@@ -1574,23 +1764,23 @@
         <f aca="false">E55*C55</f>
         <v>0</v>
       </c>
-      <c r="K55" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L55" s="2"/>
-      <c r="M55" s="2"/>
+      <c r="K55" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L55" s="3"/>
+      <c r="M55" s="3"/>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="4" t="n">
+      <c r="A56" s="5" t="n">
         <v>0.530585715350705</v>
       </c>
-      <c r="B56" s="4" t="n">
+      <c r="B56" s="5" t="n">
         <v>0.25354050051506</v>
       </c>
-      <c r="C56" s="4" t="n">
+      <c r="C56" s="5" t="n">
         <v>0.282080994964924</v>
       </c>
-      <c r="E56" s="4" t="n">
+      <c r="E56" s="5" t="n">
         <v>1</v>
       </c>
       <c r="G56" s="0" t="n">
@@ -1619,16 +1809,16 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="4" t="s">
-        <v>20</v>
+      <c r="A57" s="5" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K58" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="L58" s="5"/>
-      <c r="M58" s="5"/>
+      <c r="K58" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L58" s="6"/>
+      <c r="M58" s="6"/>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K59" s="0" t="n">
@@ -1645,296 +1835,296 @@
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
-      <c r="E61" s="2"/>
-      <c r="F61" s="2"/>
-      <c r="G61" s="2"/>
-      <c r="K61" s="5"/>
-      <c r="L61" s="5"/>
-      <c r="M61" s="5"/>
+      <c r="A61" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3"/>
+      <c r="G61" s="3"/>
+      <c r="K61" s="6"/>
+      <c r="L61" s="6"/>
+      <c r="M61" s="6"/>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="3" t="n">
+      <c r="A62" s="4" t="n">
         <f aca="false">K$59*A44</f>
         <v>0.0243144804084281</v>
       </c>
-      <c r="B62" s="3" t="n">
+      <c r="B62" s="4" t="n">
         <f aca="false">L$59*B44</f>
         <v>0.0272129513046061</v>
       </c>
-      <c r="C62" s="3" t="n">
+      <c r="C62" s="4" t="n">
         <f aca="false">M$59*C44</f>
         <v>-0.0373308966441698</v>
       </c>
-      <c r="D62" s="3"/>
+      <c r="D62" s="4"/>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="3" t="n">
+      <c r="A63" s="4" t="n">
         <f aca="false">K$59*A45</f>
         <v>0.0173130920197195</v>
       </c>
-      <c r="B63" s="3" t="n">
+      <c r="B63" s="4" t="n">
         <f aca="false">L$59*B45</f>
         <v>0.0201058844117969</v>
       </c>
-      <c r="C63" s="3" t="n">
+      <c r="C63" s="4" t="n">
         <f aca="false">M$59*C45</f>
         <v>-0.0145929371737229</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="3" t="n">
+      <c r="A64" s="4" t="n">
         <f aca="false">K$59*A46</f>
         <v>0.0378875492824237</v>
       </c>
-      <c r="B64" s="3" t="n">
+      <c r="B64" s="4" t="n">
         <f aca="false">L$59*B46</f>
         <v>0.0149495453867415</v>
       </c>
-      <c r="C64" s="3" t="n">
+      <c r="C64" s="4" t="n">
         <f aca="false">M$59*C46</f>
         <v>-0.013447907756571</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="3" t="n">
+      <c r="A65" s="4" t="n">
         <f aca="false">K$59*A47</f>
         <v>0.0548718518977952</v>
       </c>
-      <c r="B65" s="3" t="n">
+      <c r="B65" s="4" t="n">
         <f aca="false">L$59*B47</f>
         <v>0.0115437263154276</v>
       </c>
-      <c r="C65" s="3" t="n">
+      <c r="C65" s="4" t="n">
         <f aca="false">M$59*C47</f>
         <v>-0.00932248740873383</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="3" t="n">
+      <c r="A66" s="4" t="n">
         <f aca="false">K$59*A48</f>
         <v>0.0291593723758922</v>
       </c>
-      <c r="B66" s="3" t="n">
+      <c r="B66" s="4" t="n">
         <f aca="false">L$59*B48</f>
         <v>0.030142320303196</v>
       </c>
-      <c r="C66" s="3" t="n">
+      <c r="C66" s="4" t="n">
         <f aca="false">M$59*C48</f>
         <v>-0.0395722681426169</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="3" t="n">
+      <c r="A67" s="4" t="n">
         <f aca="false">K$59*A49</f>
         <v>0.0236844122487356</v>
       </c>
-      <c r="B67" s="3" t="n">
+      <c r="B67" s="4" t="n">
         <f aca="false">L$59*B49</f>
         <v>0.015691566720734</v>
       </c>
-      <c r="C67" s="3" t="n">
+      <c r="C67" s="4" t="n">
         <f aca="false">M$59*C49</f>
         <v>-0.0345290639033747</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="3" t="n">
+      <c r="A68" s="4" t="n">
         <f aca="false">K$59*A50</f>
         <v>0.016692429723613</v>
       </c>
-      <c r="B68" s="3" t="n">
+      <c r="B68" s="4" t="n">
         <f aca="false">L$59*B50</f>
         <v>0.0457060216855454</v>
       </c>
-      <c r="C68" s="3" t="n">
+      <c r="C68" s="4" t="n">
         <f aca="false">M$59*C50</f>
         <v>-0.0319664131722955</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="3" t="n">
+      <c r="A69" s="4" t="n">
         <f aca="false">K$59*A51</f>
         <v>0.0423260769589363</v>
       </c>
-      <c r="B69" s="3" t="n">
+      <c r="B69" s="4" t="n">
         <f aca="false">L$59*B51</f>
         <v>0.00149493701378588</v>
       </c>
-      <c r="C69" s="3" t="n">
+      <c r="C69" s="4" t="n">
         <f aca="false">M$59*C51</f>
         <v>-0.00726431450731645</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="3" t="n">
+      <c r="A70" s="4" t="n">
         <f aca="false">K$59*A52</f>
         <v>0.0490676965343318</v>
       </c>
-      <c r="B70" s="3" t="n">
+      <c r="B70" s="4" t="n">
         <f aca="false">L$59*B52</f>
         <v>0.0515111649367729</v>
       </c>
-      <c r="C70" s="3" t="n">
+      <c r="C70" s="4" t="n">
         <f aca="false">M$59*C52</f>
         <v>-0.00364543919225092</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="3" t="n">
+      <c r="A71" s="4" t="n">
         <f aca="false">K$59*A53</f>
         <v>0.0480621201404268</v>
       </c>
-      <c r="B71" s="3" t="n">
+      <c r="B71" s="4" t="n">
         <f aca="false">L$59*B53</f>
         <v>0.00312268627804925</v>
       </c>
-      <c r="C71" s="3" t="n">
+      <c r="C71" s="4" t="n">
         <f aca="false">M$59*C53</f>
         <v>-0.031751019596268</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="3" t="n">
+      <c r="A72" s="4" t="n">
         <f aca="false">K$59*A54</f>
         <v>0.0243638363265937</v>
       </c>
-      <c r="B72" s="3" t="n">
+      <c r="B72" s="4" t="n">
         <f aca="false">L$59*B54</f>
         <v>0.00915172773638514</v>
       </c>
-      <c r="C72" s="3" t="n">
+      <c r="C72" s="4" t="n">
         <f aca="false">M$59*C54</f>
         <v>-0.0248263897177885</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="3" t="n">
+      <c r="A73" s="4" t="n">
         <f aca="false">K$59*A55</f>
         <v>0.0439692207317199</v>
       </c>
-      <c r="B73" s="3" t="n">
+      <c r="B73" s="4" t="n">
         <f aca="false">L$59*B55</f>
         <v>0.0147104591991053</v>
       </c>
-      <c r="C73" s="3" t="n">
+      <c r="C73" s="4" t="n">
         <f aca="false">M$59*C55</f>
         <v>-0.0194147926097537</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="6" t="n">
+      <c r="A74" s="7" t="n">
         <f aca="false">K$59*A56</f>
         <v>0.0428727400634647</v>
       </c>
-      <c r="B74" s="6" t="n">
+      <c r="B74" s="7" t="n">
         <f aca="false">L$59*B56</f>
         <v>0.0133917239457459</v>
       </c>
-      <c r="C74" s="6" t="n">
+      <c r="C74" s="7" t="n">
         <f aca="false">M$59*C56</f>
         <v>-0.012942255755858</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="3"/>
+      <c r="A75" s="4"/>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="3" t="n">
+      <c r="A76" s="4" t="n">
         <f aca="false">SUM(A62:C62)</f>
         <v>0.0141965350688645</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="3" t="n">
+      <c r="A77" s="4" t="n">
         <f aca="false">SUM(A63:C63)</f>
         <v>0.0228260392577935</v>
       </c>
-      <c r="B77" s="7"/>
-      <c r="C77" s="7"/>
+      <c r="B77" s="8"/>
+      <c r="C77" s="8"/>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="3" t="n">
+      <c r="A78" s="4" t="n">
         <f aca="false">SUM(A64:C64)</f>
         <v>0.0393891869125942</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="3" t="n">
+      <c r="A79" s="4" t="n">
         <f aca="false">SUM(A65:C65)</f>
         <v>0.057093090804489</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="3" t="n">
+      <c r="A80" s="4" t="n">
         <f aca="false">SUM(A66:C66)</f>
         <v>0.0197294245364713</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="3" t="n">
+      <c r="A81" s="4" t="n">
         <f aca="false">SUM(A67:C67)</f>
         <v>0.00484691506609497</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="3" t="n">
+      <c r="A82" s="4" t="n">
         <f aca="false">SUM(A68:C68)</f>
         <v>0.0304320382368629</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="3" t="n">
+      <c r="A83" s="4" t="n">
         <f aca="false">SUM(A69:C69)</f>
         <v>0.0365566994654057</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="3" t="n">
+      <c r="A84" s="4" t="n">
         <f aca="false">SUM(A70:C70)</f>
         <v>0.0969334222788538</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="3" t="n">
+      <c r="A85" s="4" t="n">
         <f aca="false">SUM(A71:C71)</f>
         <v>0.0194337868222081</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="3" t="n">
+      <c r="A86" s="4" t="n">
         <f aca="false">SUM(A72:C72)</f>
         <v>0.00868917434519041</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="3" t="n">
+      <c r="A87" s="4" t="n">
         <f aca="false">SUM(A73:C73)</f>
         <v>0.0392648873210714</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="6" t="n">
+      <c r="A88" s="7" t="n">
         <f aca="false">SUM(A74:C74)</f>
         <v>0.0433222082533526</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D90" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1962,7 +2152,7 @@
         <f aca="false">C91+C44</f>
         <v>0.815015202899816</v>
       </c>
-      <c r="J91" s="8"/>
+      <c r="J91" s="9"/>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="n">
@@ -2251,27 +2441,27 @@
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="4" t="n">
+      <c r="A103" s="5" t="n">
         <f aca="false">$O$43*K$59*$E56</f>
         <v>-0.00808026654753169</v>
       </c>
-      <c r="B103" s="4" t="n">
+      <c r="B103" s="5" t="n">
         <f aca="false">$O$43*L$59*$E56</f>
         <v>-0.0052818874769676</v>
       </c>
-      <c r="C103" s="4" t="n">
+      <c r="C103" s="5" t="n">
         <f aca="false">$O$43*M$59*$E56</f>
         <v>0.00458813460916335</v>
       </c>
-      <c r="D103" s="4" t="n">
+      <c r="D103" s="5" t="n">
         <f aca="false">A103+A56</f>
         <v>0.522505448803173</v>
       </c>
-      <c r="E103" s="4" t="n">
+      <c r="E103" s="5" t="n">
         <f aca="false">B103+B56</f>
         <v>0.248258613038092</v>
       </c>
-      <c r="F103" s="4" t="n">
+      <c r="F103" s="5" t="n">
         <f aca="false">C103+C56</f>
         <v>0.286669129574087</v>
       </c>
@@ -2285,13 +2475,14 @@
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="20">
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="E12:G12"/>
     <mergeCell ref="I12:K12"/>
     <mergeCell ref="A17:G17"/>
     <mergeCell ref="A26:G26"/>
+    <mergeCell ref="I26:O26"/>
     <mergeCell ref="A35:D35"/>
     <mergeCell ref="A42:C42"/>
     <mergeCell ref="E42:E43"/>

</xml_diff>

<commit_message>
starting develope backprop for relu and conv + update excel
</commit_message>
<xml_diff>
--- a/vika_conv2.xlsx
+++ b/vika_conv2.xlsx
@@ -25,6 +25,9 @@
     <t xml:space="preserve">Изображение (8x9)</t>
   </si>
   <si>
+    <t xml:space="preserve">Deconvolve</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ядро свёртки</t>
   </si>
   <si>
@@ -38,9 +41,6 @@
   </si>
   <si>
     <t xml:space="preserve">ReLU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maxpooling local gradients</t>
   </si>
   <si>
     <t xml:space="preserve">Maxpooling</t>
@@ -201,13 +201,21 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -224,10 +232,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -319,15 +323,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O104"/>
+  <dimension ref="A1:T104"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N34" activeCellId="0" sqref="N34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -339,8 +343,18 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
-    </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>-0.1</v>
       </c>
@@ -365,8 +379,40 @@
       <c r="H2" s="0" t="n">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M2" s="0" t="n">
+        <f aca="false">G25*$I$13+H25*$J$13+I25*$K$13+G26*$I$14+H26*$J$14+I26*$K$14+G27*$I$15+H27*$J$15+I27*$K$15</f>
+        <v>0.00148581344862013</v>
+      </c>
+      <c r="N2" s="0" t="n">
+        <f aca="false">H25*$I$13+I25*$J$13+J25*$K$13+H26*$I$14+I26*$J$14+J26*$K$14+H27*$I$15+I27*$J$15+J27*$K$15</f>
+        <v>0.00625370271658454</v>
+      </c>
+      <c r="O2" s="0" t="n">
+        <f aca="false">I25*$I$13+J25*$J$13+K25*$K$13+I26*$I$14+J26*$J$14+K26*$K$14+I27*$I$15+J27*$J$15+K27*$K$15</f>
+        <v>0.00472516240860529</v>
+      </c>
+      <c r="P2" s="0" t="n">
+        <f aca="false">J25*$I$13+K25*$J$13+L25*$K$13+J26*$I$14+K26*$J$14+L26*$K$14+J27*$I$15+K27*$J$15+L27*$K$15</f>
+        <v>0.0100550777371303</v>
+      </c>
+      <c r="Q2" s="0" t="n">
+        <f aca="false">K25*$I$13+L25*$J$13+M25*$K$13+K26*$I$14+L26*$J$14+M26*$K$14+K27*$I$15+L27*$J$15+M27*$K$15</f>
+        <v>0.00375625423502984</v>
+      </c>
+      <c r="R2" s="0" t="n">
+        <f aca="false">L25*$I$13+M25*$J$13+N25*$K$13+L26*$I$14+M26*$J$14+N26*$K$14+L27*$I$15+M27*$J$15+N27*$K$15</f>
+        <v>0.00412248364555518</v>
+      </c>
+      <c r="S2" s="0" t="n">
+        <f aca="false">M25*$I$13+N25*$J$13+O25*$K$13+M26*$I$14+N26*$J$14+O26*$K$14+M27*$I$15+N27*$J$15+O27*$K$15</f>
+        <v>0.0173512948057014</v>
+      </c>
+      <c r="T2" s="0" t="n">
+        <f aca="false">N25*$I$13+O25*$J$13+P25*$K$13+N26*$I$14+O26*$J$14+P26*$K$14+N27*$I$15+O27*$J$15+P27*$K$15</f>
+        <v>0.00648188669456955</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>-0.9</v>
       </c>
@@ -391,8 +437,40 @@
       <c r="H3" s="0" t="n">
         <v>0.16</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M3" s="0" t="n">
+        <f aca="false">G26*$I$13+H26*$J$13+I26*$K$13+G27*$I$14+H27*$J$14+I27*$K$14+G28*$I$15+H28*$J$15+I28*$K$15</f>
+        <v>-0.000884242725892766</v>
+      </c>
+      <c r="N3" s="0" t="n">
+        <f aca="false">H26*$I$13+I26*$J$13+J26*$K$13+H27*$I$14+I27*$J$14+J27*$K$14+H28*$I$15+I28*$J$15+J28*$K$15</f>
+        <v>-0.00106988641570518</v>
+      </c>
+      <c r="O3" s="0" t="n">
+        <f aca="false">I26*$I$13+J26*$J$13+K26*$K$13+I27*$I$14+J27*$J$14+K27*$K$14+I28*$I$15+J28*$J$15+K28*$K$15</f>
+        <v>0.00123050189715738</v>
+      </c>
+      <c r="P3" s="0" t="n">
+        <f aca="false">J26*$I$13+K26*$J$13+L26*$K$13+J27*$I$14+K27*$J$14+L27*$K$14+J28*$I$15+K28*$J$15+L28*$K$15</f>
+        <v>-0.00172022745041687</v>
+      </c>
+      <c r="Q3" s="0" t="n">
+        <f aca="false">K26*$I$13+L26*$J$13+M26*$K$13+K27*$I$14+L27*$J$14+M27*$K$14+K28*$I$15+L28*$J$15+M28*$K$15</f>
+        <v>0.00426443079552625</v>
+      </c>
+      <c r="R3" s="0" t="n">
+        <f aca="false">L26*$I$13+M26*$J$13+N26*$K$13+L27*$I$14+M27*$J$14+N27*$K$14+L28*$I$15+M28*$J$15+N28*$K$15</f>
+        <v>-0.00245338752289489</v>
+      </c>
+      <c r="S3" s="0" t="n">
+        <f aca="false">M26*$I$13+N26*$J$13+O26*$K$13+M27*$I$14+N27*$J$14+O27*$K$14+M28*$I$15+N28*$J$15+O28*$K$15</f>
+        <v>-0.00296846771406084</v>
+      </c>
+      <c r="T3" s="0" t="n">
+        <f aca="false">N26*$I$13+O26*$J$13+P26*$K$13+N27*$I$14+O27*$J$14+P27*$K$14+N28*$I$15+O28*$J$15+P28*$K$15</f>
+        <v>0.00735880893674776</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>-0.17</v>
       </c>
@@ -417,8 +495,40 @@
       <c r="H4" s="0" t="n">
         <v>0.24</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M4" s="0" t="n">
+        <f aca="false">G27*$I$13+H27*$J$13+I27*$K$13+G28*$I$14+H28*$J$14+I28*$K$14+G29*$I$15+H29*$J$15+I29*$K$15</f>
+        <v>-0.00616644928929563</v>
+      </c>
+      <c r="N4" s="0" t="n">
+        <f aca="false">H27*$I$13+I27*$J$13+J27*$K$13+H28*$I$14+I28*$J$14+J28*$K$14+H29*$I$15+I29*$J$15+J29*$K$15</f>
+        <v>-0.00487623644566565</v>
+      </c>
+      <c r="O4" s="0" t="n">
+        <f aca="false">I27*$I$13+J27*$J$13+K27*$K$13+I28*$I$14+J28*$J$14+K28*$K$14+I29*$I$15+J29*$J$15+K29*$K$15</f>
+        <v>-0.015636422810026</v>
+      </c>
+      <c r="P4" s="0" t="n">
+        <f aca="false">J27*$I$13+K27*$J$13+L27*$K$13+J28*$I$14+K28*$J$14+L28*$K$14+J29*$I$15+K29*$J$15+L29*$K$15</f>
+        <v>-0.00784030497576549</v>
+      </c>
+      <c r="Q4" s="0" t="n">
+        <f aca="false">K27*$I$13+L27*$J$13+M27*$K$13+K28*$I$14+L28*$J$14+M28*$K$14+K29*$I$15+L29*$J$15+M29*$K$15</f>
+        <v>-0.00919958958334537</v>
+      </c>
+      <c r="R4" s="0" t="n">
+        <f aca="false">L27*$I$13+M27*$J$13+N27*$K$13+L28*$I$14+M28*$J$14+N28*$K$14+L29*$I$15+M29*$J$15+N29*$K$15</f>
+        <v>-0.0171092046379544</v>
+      </c>
+      <c r="S4" s="0" t="n">
+        <f aca="false">M27*$I$13+N27*$J$13+O27*$K$13+M28*$I$14+N28*$J$14+O28*$K$14+M29*$I$15+N29*$J$15+O29*$K$15</f>
+        <v>-0.0135294272762072</v>
+      </c>
+      <c r="T4" s="0" t="n">
+        <f aca="false">N27*$I$13+O27*$J$13+P27*$K$13+N28*$I$14+O28*$J$14+P28*$K$14+N29*$I$15+O29*$J$15+P29*$K$15</f>
+        <v>-0.0158750429509501</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>-0.25</v>
       </c>
@@ -443,8 +553,40 @@
       <c r="H5" s="0" t="n">
         <v>0.32</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M5" s="0" t="n">
+        <f aca="false">G28*$I$13+H28*$J$13+I28*$K$13+G29*$I$14+H29*$J$14+I29*$K$14+G30*$I$15+H30*$J$15+I30*$K$15</f>
+        <v>0.00597537932524441</v>
+      </c>
+      <c r="N5" s="0" t="n">
+        <f aca="false">H28*$I$13+I28*$J$13+J28*$K$13+H29*$I$14+I29*$J$14+J29*$K$14+H30*$I$15+I30*$J$15+J30*$K$15</f>
+        <v>0.0251500253639565</v>
+      </c>
+      <c r="O5" s="0" t="n">
+        <f aca="false">I28*$I$13+J28*$J$13+K28*$K$13+I29*$I$14+J29*$J$14+K29*$K$14+I30*$I$15+J30*$J$15+K30*$K$15</f>
+        <v>0.00939524206119479</v>
+      </c>
+      <c r="P5" s="0" t="n">
+        <f aca="false">J28*$I$13+K28*$J$13+L28*$K$13+J29*$I$14+K29*$J$14+L29*$K$14+J30*$I$15+K30*$J$15+L30*$K$15</f>
+        <v>0.00206488725365927</v>
+      </c>
+      <c r="Q5" s="0" t="n">
+        <f aca="false">K28*$I$13+L28*$J$13+M28*$K$13+K29*$I$14+L29*$J$14+M29*$K$14+K30*$I$15+L30*$J$15+M30*$K$15</f>
+        <v>0.00869099081021386</v>
+      </c>
+      <c r="R5" s="0" t="n">
+        <f aca="false">L28*$I$13+M28*$J$13+N28*$K$13+L29*$I$14+M29*$J$14+N29*$K$14+L30*$I$15+M30*$J$15+N30*$K$15</f>
+        <v>0.00375395467832216</v>
+      </c>
+      <c r="S5" s="0" t="n">
+        <f aca="false">M28*$I$13+N28*$J$13+O28*$K$13+M29*$I$14+N29*$J$14+O29*$K$14+M30*$I$15+N30*$J$15+O30*$K$15</f>
+        <v>0.00213511013559712</v>
+      </c>
+      <c r="T5" s="0" t="n">
+        <f aca="false">N28*$I$13+O28*$J$13+P28*$K$13+N29*$I$14+O29*$J$14+P29*$K$14+N30*$I$15+O30*$J$15+P30*$K$15</f>
+        <v>0.000797608601222089</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>-0.33</v>
       </c>
@@ -469,8 +611,40 @@
       <c r="H6" s="0" t="n">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M6" s="0" t="n">
+        <f aca="false">G29*$I$13+H29*$J$13+I29*$K$13+G30*$I$14+H30*$J$14+I30*$K$14+G31*$I$15+H31*$J$15+I31*$K$15</f>
+        <v>-0.00355608956676514</v>
+      </c>
+      <c r="N6" s="0" t="n">
+        <f aca="false">H29*$I$13+I29*$J$13+J29*$K$13+H30*$I$14+I30*$J$14+J30*$K$14+H31*$I$15+I31*$J$15+J31*$K$15</f>
+        <v>-0.00430267822296379</v>
+      </c>
+      <c r="O6" s="0" t="n">
+        <f aca="false">I29*$I$13+J29*$J$13+K29*$K$13+I30*$I$14+J30*$J$14+K30*$K$14+I31*$I$15+J31*$J$15+K31*$K$15</f>
+        <v>0.0138513325492524</v>
+      </c>
+      <c r="P6" s="0" t="n">
+        <f aca="false">J29*$I$13+K29*$J$13+L29*$K$13+J30*$I$14+K30*$J$14+L30*$K$14+J31*$I$15+K31*$J$15+L31*$K$15</f>
+        <v>0.0121767261674842</v>
+      </c>
+      <c r="Q6" s="0" t="n">
+        <f aca="false">K29*$I$13+L29*$J$13+M29*$K$13+K30*$I$14+L30*$J$14+M30*$K$14+K31*$I$15+L31*$J$15+M31*$K$15</f>
+        <v>0.00352103901739322</v>
+      </c>
+      <c r="R6" s="0" t="n">
+        <f aca="false">L29*$I$13+M29*$J$13+N29*$K$13+L30*$I$14+M30*$J$14+N30*$K$14+L31*$I$15+M31*$J$15+N31*$K$15</f>
+        <v>0.00338401767327591</v>
+      </c>
+      <c r="S6" s="0" t="n">
+        <f aca="false">M29*$I$13+N29*$J$13+O29*$K$13+M30*$I$14+N30*$J$14+O30*$K$14+M31*$I$15+N31*$J$15+O31*$K$15</f>
+        <v>-0.000365275650863909</v>
+      </c>
+      <c r="T6" s="0" t="n">
+        <f aca="false">N29*$I$13+O29*$J$13+P29*$K$13+N30*$I$14+O30*$J$14+P30*$K$14+N31*$I$15+O31*$J$15+P31*$K$15</f>
+        <v>0.000905515566573749</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>-0.41</v>
       </c>
@@ -495,8 +669,40 @@
       <c r="H7" s="0" t="n">
         <v>0.48</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M7" s="0" t="n">
+        <f aca="false">G30*$I$13+H30*$J$13+I30*$K$13+G31*$I$14+H31*$J$14+I31*$K$14+G32*$I$15+H32*$J$15+I32*$K$15</f>
+        <v>-0.0209730904102914</v>
+      </c>
+      <c r="N7" s="0" t="n">
+        <f aca="false">H30*$I$13+I30*$J$13+J30*$K$13+H31*$I$14+I31*$J$14+J31*$K$14+H32*$I$15+I32*$J$15+J32*$K$15</f>
+        <v>-0.00350681903569287</v>
+      </c>
+      <c r="O7" s="0" t="n">
+        <f aca="false">I30*$I$13+J30*$J$13+K30*$K$13+I31*$I$14+J31*$J$14+K31*$K$14+I32*$I$15+J32*$J$15+K32*$K$15</f>
+        <v>-0.0188899676812126</v>
+      </c>
+      <c r="P7" s="0" t="n">
+        <f aca="false">J30*$I$13+K30*$J$13+L30*$K$13+J31*$I$14+K31*$J$14+L31*$K$14+J32*$I$15+K32*$J$15+L32*$K$15</f>
+        <v>-0.0108631662215385</v>
+      </c>
+      <c r="Q7" s="0" t="n">
+        <f aca="false">K30*$I$13+L30*$J$13+M30*$K$13+K31*$I$14+L31*$J$14+M31*$K$14+K32*$I$15+L32*$J$15+M32*$K$15</f>
+        <v>-0.00109127054646023</v>
+      </c>
+      <c r="R7" s="0" t="n">
+        <f aca="false">L30*$I$13+M30*$J$13+N30*$K$13+L31*$I$14+M31*$J$14+N31*$K$14+L32*$I$15+M32*$J$15+N32*$K$15</f>
+        <v>8.81999523718244E-005</v>
+      </c>
+      <c r="S7" s="0" t="n">
+        <f aca="false">M30*$I$13+N30*$J$13+O30*$K$13+M31*$I$14+N31*$J$14+O31*$K$14+M32*$I$15+N32*$J$15+O32*$K$15</f>
+        <v>0.0410352314499908</v>
+      </c>
+      <c r="T7" s="0" t="n">
+        <f aca="false">N30*$I$13+O30*$J$13+P30*$K$13+N31*$I$14+O31*$J$14+P31*$K$14+N32*$I$15+O32*$J$15+P32*$K$15</f>
+        <v>0.0139979146179897</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>-0.49</v>
       </c>
@@ -521,8 +727,40 @@
       <c r="H8" s="0" t="n">
         <v>0.56</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M8" s="0" t="n">
+        <f aca="false">G31*$I$13+H31*$J$13+I31*$K$13+G32*$I$14+H32*$J$14+I32*$K$14+G33*$I$15+H33*$J$15+I33*$K$15</f>
+        <v>-0.000243018014617239</v>
+      </c>
+      <c r="N8" s="0" t="n">
+        <f aca="false">H31*$I$13+I31*$J$13+J31*$K$13+H32*$I$14+I32*$J$14+J32*$K$14+H33*$I$15+I33*$J$15+J33*$K$15</f>
+        <v>0.00580575533978555</v>
+      </c>
+      <c r="O8" s="0" t="n">
+        <f aca="false">I31*$I$13+J31*$J$13+K31*$K$13+I32*$I$14+J32*$J$14+K32*$K$14+I33*$I$15+J33*$J$15+K33*$K$15</f>
+        <v>-0.00228147942887293</v>
+      </c>
+      <c r="P8" s="0" t="n">
+        <f aca="false">J31*$I$13+K31*$J$13+L31*$K$13+J32*$I$14+K32*$J$14+L32*$K$14+J33*$I$15+K33*$J$15+L33*$K$15</f>
+        <v>-0.00662515890693393</v>
+      </c>
+      <c r="Q8" s="0" t="n">
+        <f aca="false">K31*$I$13+L31*$J$13+M31*$K$13+K32*$I$14+L32*$J$14+M32*$K$14+K33*$I$15+L33*$J$15+M33*$K$15</f>
+        <v>-0.00672567360383571</v>
+      </c>
+      <c r="R8" s="0" t="n">
+        <f aca="false">L31*$I$13+M31*$J$13+N31*$K$13+L32*$I$14+M32*$J$14+N32*$K$14+L33*$I$15+M33*$J$15+N33*$K$15</f>
+        <v>0.0112589627106092</v>
+      </c>
+      <c r="S8" s="0" t="n">
+        <f aca="false">M31*$I$13+N31*$J$13+O31*$K$13+M32*$I$14+N32*$J$14+O32*$K$14+M33*$I$15+N33*$J$15+O33*$K$15</f>
+        <v>-0.000843713373208826</v>
+      </c>
+      <c r="T8" s="0" t="n">
+        <f aca="false">N31*$I$13+O31*$J$13+P31*$K$13+N32*$I$14+O32*$J$14+P32*$K$14+N33*$I$15+O33*$J$15+P33*$K$15</f>
+        <v>0.0181093998136606</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>-0.57</v>
       </c>
@@ -547,8 +785,40 @@
       <c r="H9" s="0" t="n">
         <v>-0.64</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M9" s="0" t="n">
+        <f aca="false">G32*$I$13+H32*$J$13+I32*$K$13+G33*$I$14+H33*$J$14+I33*$K$14+G34*$I$15+H34*$J$15+I34*$K$15</f>
+        <v>-0.0170893261556207</v>
+      </c>
+      <c r="N9" s="0" t="n">
+        <f aca="false">H32*$I$13+I32*$J$13+J32*$K$13+H33*$I$14+I33*$J$14+J33*$K$14+H34*$I$15+I34*$J$15+J34*$K$15</f>
+        <v>-0.014021101193192</v>
+      </c>
+      <c r="O9" s="0" t="n">
+        <f aca="false">I32*$I$13+J32*$J$13+K32*$K$13+I33*$I$14+J33*$J$14+K33*$K$14+I34*$I$15+J34*$J$15+K34*$K$15</f>
+        <v>-0.011643996687636</v>
+      </c>
+      <c r="P9" s="0" t="n">
+        <f aca="false">J32*$I$13+K32*$J$13+L32*$K$13+J33*$I$14+K33*$J$14+L33*$K$14+J34*$I$15+K34*$J$15+L34*$K$15</f>
+        <v>-0.000654837927037695</v>
+      </c>
+      <c r="Q9" s="0" t="n">
+        <f aca="false">K32*$I$13+L32*$J$13+M32*$K$13+K33*$I$14+L33*$J$14+M33*$K$14+K34*$I$15+L34*$J$15+M34*$K$15</f>
+        <v>-0.000822307169958049</v>
+      </c>
+      <c r="R9" s="0" t="n">
+        <f aca="false">L32*$I$13+M32*$J$13+N32*$K$13+L33*$I$14+M33*$J$14+N33*$K$14+L34*$I$15+M34*$J$15+N34*$K$15</f>
+        <v>-0.0450633904242247</v>
+      </c>
+      <c r="S9" s="0" t="n">
+        <f aca="false">M32*$I$13+N32*$J$13+O32*$K$13+M33*$I$14+N33*$J$14+O33*$K$14+M34*$I$15+N34*$J$15+O34*$K$15</f>
+        <v>-0.0259591772205384</v>
+      </c>
+      <c r="T9" s="0" t="n">
+        <f aca="false">N32*$I$13+O32*$J$13+P32*$K$13+N33*$I$14+O33*$J$14+P33*$K$14+N34*$I$15+O34*$J$15+P34*$K$15</f>
+        <v>-0.0390671238143118</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>-0.65</v>
       </c>
@@ -573,20 +843,52 @@
       <c r="H10" s="0" t="n">
         <v>0.72</v>
       </c>
+      <c r="M10" s="0" t="n">
+        <f aca="false">G33*$I$13+H33*$J$13+I33*$K$13+G34*$I$14+H34*$J$14+I34*$K$14+G35*$I$15+H35*$J$15+I35*$K$15</f>
+        <v>-0.00844131757198644</v>
+      </c>
+      <c r="N10" s="0" t="n">
+        <f aca="false">H33*$I$13+I33*$J$13+J33*$K$13+H34*$I$14+I34*$J$14+J34*$K$14+H35*$I$15+I35*$J$15+J35*$K$15</f>
+        <v>-0.00667513158105609</v>
+      </c>
+      <c r="O10" s="0" t="n">
+        <f aca="false">I33*$I$13+J33*$J$13+K33*$K$13+I34*$I$14+J34*$J$14+K34*$K$14+I35*$I$15+J35*$J$15+K35*$K$15</f>
+        <v>-0.0116066641213838</v>
+      </c>
+      <c r="P10" s="0" t="n">
+        <f aca="false">J33*$I$13+K33*$J$13+L33*$K$13+J34*$I$14+K34*$J$14+L34*$K$14+J35*$I$15+K35*$J$15+L35*$K$15</f>
+        <v>-0.00298456407984271</v>
+      </c>
+      <c r="Q10" s="0" t="n">
+        <f aca="false">K33*$I$13+L33*$J$13+M33*$K$13+K34*$I$14+L34*$J$14+M34*$K$14+K35*$I$15+L35*$J$15+M35*$K$15</f>
+        <v>-0.0205572156134485</v>
+      </c>
+      <c r="R10" s="0" t="n">
+        <f aca="false">L33*$I$13+M33*$J$13+N33*$K$13+L34*$I$14+M34*$J$14+N34*$K$14+L35*$I$15+M35*$J$15+N35*$K$15</f>
+        <v>-0.0134867327598746</v>
+      </c>
+      <c r="S10" s="0" t="n">
+        <f aca="false">M33*$I$13+N33*$J$13+O33*$K$13+M34*$I$14+N34*$J$14+O34*$K$14+M35*$I$15+N35*$J$15+O35*$K$15</f>
+        <v>-0.01582494642678</v>
+      </c>
+      <c r="T10" s="0" t="n">
+        <f aca="false">N33*$I$13+O33*$J$13+P33*$K$13+N34*$I$14+O34*$J$14+P34*$K$14+N35*$I$15+O35*$J$15+P35*$K$15</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="E12" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="I12" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
@@ -696,9 +998,9 @@
         <v>0.10466028797962</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -707,7 +1009,7 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <f aca="false">$A$13*A2+$B$13*B2+$C$13*C2+$A$14*A3+$B$14*B3+$C$14*C3+$A$15*A4+$B$15*B4+$C$15*C4</f>
         <v>0.29973878860774</v>
@@ -733,7 +1035,7 @@
         <v>0.24138013677554</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <f aca="false">$A$13*A3+$B$13*B3+$C$13*C3+$A$14*A4+$B$14*B4+$C$14*C4+$A$15*A5+$B$15*B5+$C$15*C5</f>
         <v>-0.248149086792767</v>
@@ -759,7 +1061,7 @@
         <v>-0.244897984180467</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
         <f aca="false">$A$13*A4+$B$13*B4+$C$13*C4+$A$14*A5+$B$14*B5+$C$14*C5+$A$15*A6+$B$15*B6+$C$15*C6</f>
         <v>-0.0378519292165913</v>
@@ -785,7 +1087,7 @@
         <v>-0.278655585841809</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <f aca="false">$A$13*A5+$B$13*B5+$C$13*C5+$A$14*A6+$B$14*B6+$C$14*C6+$A$15*A7+$B$15*B7+$C$15*C7</f>
         <v>0.0536414502436412</v>
@@ -811,7 +1113,7 @@
         <v>0.0872007548167718</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
         <f aca="false">$A$13*A6+$B$13*B6+$C$13*C6+$A$14*A7+$B$14*B7+$C$14*C7+$A$15*A8+$B$15*B8+$C$15*C8</f>
         <v>0.0826020094808472</v>
@@ -837,7 +1139,7 @@
         <v>0.088960978417416</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
         <f aca="false">$A$13*A7+$B$13*B7+$C$13*C7+$A$14*A8+$B$14*B8+$C$14*C8+$A$15*A9+$B$15*B9+$C$15*C9</f>
         <v>0.111562568718053</v>
@@ -863,7 +1165,7 @@
         <v>0.122561913243983</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
         <f aca="false">$A$13*A8+$B$13*B8+$C$13*C8+$A$14*A9+$B$14*B9+$C$14*C9+$A$15*A10+$B$15*B10+$C$15*C10</f>
         <v>0.140523127955259</v>
@@ -890,27 +1192,19 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
+      <c r="A26" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
       <c r="G26" s="1"/>
-      <c r="I26" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
-      <c r="N26" s="1"/>
-      <c r="O26" s="1"/>
+      <c r="I26" s="1"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2" t="n">
+      <c r="A27" s="4" t="n">
         <f aca="false">IF(A18&lt;0,0,A18)</f>
         <v>0.29973878860774</v>
       </c>
@@ -918,7 +1212,7 @@
         <f aca="false">IF(B18&lt;0,0,B18)</f>
         <v>0.14573618884283</v>
       </c>
-      <c r="C27" s="2" t="n">
+      <c r="C27" s="4" t="n">
         <f aca="false">IF(C18&lt;0,0,C18)</f>
         <v>0.227470224200259</v>
       </c>
@@ -930,11 +1224,11 @@
         <f aca="false">IF(E18&lt;0,0,E18)</f>
         <v>0.181724188351327</v>
       </c>
-      <c r="F27" s="2" t="n">
+      <c r="F27" s="4" t="n">
         <f aca="false">IF(F18&lt;0,0,F18)</f>
         <v>0.24138013677554</v>
       </c>
-      <c r="I27" s="2" t="n">
+      <c r="I27" s="4" t="n">
         <f aca="false">A76</f>
         <v>0.0141965350688645</v>
       </c>
@@ -942,7 +1236,7 @@
         <f aca="false">IF(J18&lt;0,0,J18)</f>
         <v>0</v>
       </c>
-      <c r="K27" s="2" t="n">
+      <c r="K27" s="4" t="n">
         <f aca="false">A77</f>
         <v>0.0228260392577935</v>
       </c>
@@ -954,7 +1248,7 @@
         <f aca="false">IF(M18&lt;0,0,M18)</f>
         <v>0</v>
       </c>
-      <c r="N27" s="2" t="n">
+      <c r="N27" s="4" t="n">
         <f aca="false">A78</f>
         <v>0.0393891869125942</v>
       </c>
@@ -1060,7 +1354,7 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="2" t="n">
+      <c r="A30" s="4" t="n">
         <f aca="false">IF(A21&lt;0,0,A21)</f>
         <v>0.0536414502436412</v>
       </c>
@@ -1072,7 +1366,7 @@
         <f aca="false">IF(C21&lt;0,0,C21)</f>
         <v>0</v>
       </c>
-      <c r="D30" s="2" t="n">
+      <c r="D30" s="4" t="n">
         <f aca="false">IF(D21&lt;0,0,D21)</f>
         <v>0.0639727464095352</v>
       </c>
@@ -1080,11 +1374,11 @@
         <f aca="false">IF(E21&lt;0,0,E21)</f>
         <v>0.0539002998319844</v>
       </c>
-      <c r="F30" s="2" t="n">
+      <c r="F30" s="4" t="n">
         <f aca="false">IF(F21&lt;0,0,F21)</f>
         <v>0.0872007548167718</v>
       </c>
-      <c r="I30" s="2" t="n">
+      <c r="I30" s="4" t="n">
         <f aca="false">A79</f>
         <v>0.057093090804489</v>
       </c>
@@ -1096,7 +1390,7 @@
         <f aca="false">IF(K21&lt;0,0,K21)</f>
         <v>0</v>
       </c>
-      <c r="L30" s="2" t="n">
+      <c r="L30" s="4" t="n">
         <f aca="false">A80</f>
         <v>0.0197294245364713</v>
       </c>
@@ -1104,7 +1398,7 @@
         <f aca="false">IF(M21&lt;0,0,M21)</f>
         <v>0</v>
       </c>
-      <c r="N30" s="2" t="n">
+      <c r="N30" s="4" t="n">
         <f aca="false">A81</f>
         <v>0.00484691506609497</v>
       </c>
@@ -1118,7 +1412,7 @@
         <f aca="false">IF(B22&lt;0,0,B22)</f>
         <v>0</v>
       </c>
-      <c r="C31" s="2" t="n">
+      <c r="C31" s="4" t="n">
         <f aca="false">IF(C22&lt;0,0,C22)</f>
         <v>0</v>
       </c>
@@ -1142,7 +1436,7 @@
         <f aca="false">IF(J22&lt;0,0,J22)</f>
         <v>0</v>
       </c>
-      <c r="K31" s="2" t="n">
+      <c r="K31" s="4" t="n">
         <f aca="false">A82</f>
         <v>0.0304320382368629</v>
       </c>
@@ -1160,7 +1454,7 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="2" t="n">
+      <c r="A32" s="4" t="n">
         <f aca="false">IF(A23&lt;0,0,A23)</f>
         <v>0.111562568718053</v>
       </c>
@@ -1180,11 +1474,11 @@
         <f aca="false">IF(E23&lt;0,0,E23)</f>
         <v>0</v>
       </c>
-      <c r="F32" s="2" t="n">
+      <c r="F32" s="4" t="n">
         <f aca="false">IF(F23&lt;0,0,F23)</f>
         <v>0.122561913243983</v>
       </c>
-      <c r="I32" s="2" t="n">
+      <c r="I32" s="4" t="n">
         <f aca="false">A83</f>
         <v>0.0365566994654057</v>
       </c>
@@ -1204,13 +1498,13 @@
         <f aca="false">IF(M23&lt;0,0,M23)</f>
         <v>0</v>
       </c>
-      <c r="N32" s="2" t="n">
+      <c r="N32" s="4" t="n">
         <f aca="false">A84</f>
         <v>0.0969334222788538</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="2" t="n">
+      <c r="A33" s="4" t="n">
         <f aca="false">IF(A24&lt;0,0,A24)</f>
         <v>0.140523127955259</v>
       </c>
@@ -1218,7 +1512,7 @@
         <f aca="false">IF(B24&lt;0,0,B24)</f>
         <v>0</v>
       </c>
-      <c r="C33" s="2" t="n">
+      <c r="C33" s="4" t="n">
         <f aca="false">IF(C24&lt;0,0,C24)</f>
         <v>0</v>
       </c>
@@ -1226,7 +1520,7 @@
         <f aca="false">IF(D24&lt;0,0,D24)</f>
         <v>0</v>
       </c>
-      <c r="E33" s="2" t="n">
+      <c r="E33" s="4" t="n">
         <f aca="false">IF(E24&lt;0,0,E24)</f>
         <v>0</v>
       </c>
@@ -1234,7 +1528,7 @@
         <f aca="false">IF(F24&lt;0,0,F24)</f>
         <v>0</v>
       </c>
-      <c r="I33" s="2" t="n">
+      <c r="I33" s="4" t="n">
         <f aca="false">A85</f>
         <v>0.0194337868222081</v>
       </c>
@@ -1242,7 +1536,7 @@
         <f aca="false">IF(J24&lt;0,0,J24)</f>
         <v>0</v>
       </c>
-      <c r="K33" s="2" t="n">
+      <c r="K33" s="4" t="n">
         <f aca="false">A86</f>
         <v>0.00868917434519041</v>
       </c>
@@ -1250,7 +1544,7 @@
         <f aca="false">IF(L24&lt;0,0,L24)</f>
         <v>0</v>
       </c>
-      <c r="M33" s="2" t="n">
+      <c r="M33" s="4" t="n">
         <f aca="false">A87</f>
         <v>0.0392648873210714</v>
       </c>
@@ -1324,24 +1618,24 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="3" t="s">
+      <c r="A42" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="E42" s="3" t="s">
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="E42" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G42" s="3" t="s">
+      <c r="G42" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H42" s="3"/>
-      <c r="I42" s="3"/>
-      <c r="K42" s="3" t="s">
+      <c r="H42" s="5"/>
+      <c r="I42" s="5"/>
+      <c r="K42" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="L42" s="3"/>
-      <c r="M42" s="3"/>
+      <c r="L42" s="5"/>
+      <c r="M42" s="5"/>
       <c r="O42" s="0" t="s">
         <v>12</v>
       </c>
@@ -1356,7 +1650,7 @@
       <c r="C43" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="E43" s="3" t="s">
+      <c r="E43" s="5" t="s">
         <v>16</v>
       </c>
       <c r="G43" s="0" t="s">
@@ -1473,11 +1767,11 @@
         <f aca="false">E46*C46</f>
         <v>0.0707489664131252</v>
       </c>
-      <c r="K46" s="3" t="s">
+      <c r="K46" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="L46" s="3"/>
-      <c r="M46" s="3"/>
+      <c r="L46" s="5"/>
+      <c r="M46" s="5"/>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
@@ -1571,11 +1865,11 @@
         <f aca="false">E49*C49</f>
         <v>0.0656249367548498</v>
       </c>
-      <c r="K49" s="3" t="s">
+      <c r="K49" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="L49" s="3"/>
-      <c r="M49" s="3"/>
+      <c r="L49" s="5"/>
+      <c r="M49" s="5"/>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="n">
@@ -1669,11 +1963,11 @@
         <f aca="false">E52*C52</f>
         <v>0.00973798809486858</v>
       </c>
-      <c r="K52" s="3" t="s">
+      <c r="K52" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="L52" s="3"/>
-      <c r="M52" s="3"/>
+      <c r="L52" s="5"/>
+      <c r="M52" s="5"/>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="n">
@@ -1701,7 +1995,7 @@
         <f aca="false">E53*C53</f>
         <v>0.097245459636807</v>
       </c>
-      <c r="K53" s="4" t="n">
+      <c r="K53" s="6" t="n">
         <v>0.32</v>
       </c>
       <c r="L53" s="0" t="n">
@@ -1764,23 +2058,23 @@
         <f aca="false">E55*C55</f>
         <v>0</v>
       </c>
-      <c r="K55" s="3" t="s">
+      <c r="K55" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="L55" s="3"/>
-      <c r="M55" s="3"/>
+      <c r="L55" s="5"/>
+      <c r="M55" s="5"/>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="5" t="n">
+      <c r="A56" s="7" t="n">
         <v>0.530585715350705</v>
       </c>
-      <c r="B56" s="5" t="n">
+      <c r="B56" s="7" t="n">
         <v>0.25354050051506</v>
       </c>
-      <c r="C56" s="5" t="n">
+      <c r="C56" s="7" t="n">
         <v>0.282080994964924</v>
       </c>
-      <c r="E56" s="5" t="n">
+      <c r="E56" s="7" t="n">
         <v>1</v>
       </c>
       <c r="G56" s="0" t="n">
@@ -1809,16 +2103,16 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="5" t="s">
+      <c r="A57" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K58" s="6" t="s">
+      <c r="K58" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="L58" s="6"/>
-      <c r="M58" s="6"/>
+      <c r="L58" s="3"/>
+      <c r="M58" s="3"/>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K59" s="0" t="n">
@@ -1835,197 +2129,197 @@
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="3" t="s">
+      <c r="A61" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B61" s="3"/>
-      <c r="C61" s="3"/>
-      <c r="E61" s="3"/>
-      <c r="F61" s="3"/>
-      <c r="G61" s="3"/>
-      <c r="K61" s="6"/>
-      <c r="L61" s="6"/>
-      <c r="M61" s="6"/>
+      <c r="B61" s="5"/>
+      <c r="C61" s="5"/>
+      <c r="E61" s="5"/>
+      <c r="F61" s="5"/>
+      <c r="G61" s="5"/>
+      <c r="K61" s="3"/>
+      <c r="L61" s="3"/>
+      <c r="M61" s="3"/>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="4" t="n">
+      <c r="A62" s="6" t="n">
         <f aca="false">K$59*A44</f>
         <v>0.0243144804084281</v>
       </c>
-      <c r="B62" s="4" t="n">
+      <c r="B62" s="6" t="n">
         <f aca="false">L$59*B44</f>
         <v>0.0272129513046061</v>
       </c>
-      <c r="C62" s="4" t="n">
+      <c r="C62" s="6" t="n">
         <f aca="false">M$59*C44</f>
         <v>-0.0373308966441698</v>
       </c>
-      <c r="D62" s="4"/>
+      <c r="D62" s="6"/>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="4" t="n">
+      <c r="A63" s="6" t="n">
         <f aca="false">K$59*A45</f>
         <v>0.0173130920197195</v>
       </c>
-      <c r="B63" s="4" t="n">
+      <c r="B63" s="6" t="n">
         <f aca="false">L$59*B45</f>
         <v>0.0201058844117969</v>
       </c>
-      <c r="C63" s="4" t="n">
+      <c r="C63" s="6" t="n">
         <f aca="false">M$59*C45</f>
         <v>-0.0145929371737229</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="4" t="n">
+      <c r="A64" s="6" t="n">
         <f aca="false">K$59*A46</f>
         <v>0.0378875492824237</v>
       </c>
-      <c r="B64" s="4" t="n">
+      <c r="B64" s="6" t="n">
         <f aca="false">L$59*B46</f>
         <v>0.0149495453867415</v>
       </c>
-      <c r="C64" s="4" t="n">
+      <c r="C64" s="6" t="n">
         <f aca="false">M$59*C46</f>
         <v>-0.013447907756571</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="4" t="n">
+      <c r="A65" s="6" t="n">
         <f aca="false">K$59*A47</f>
         <v>0.0548718518977952</v>
       </c>
-      <c r="B65" s="4" t="n">
+      <c r="B65" s="6" t="n">
         <f aca="false">L$59*B47</f>
         <v>0.0115437263154276</v>
       </c>
-      <c r="C65" s="4" t="n">
+      <c r="C65" s="6" t="n">
         <f aca="false">M$59*C47</f>
         <v>-0.00932248740873383</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="4" t="n">
+      <c r="A66" s="6" t="n">
         <f aca="false">K$59*A48</f>
         <v>0.0291593723758922</v>
       </c>
-      <c r="B66" s="4" t="n">
+      <c r="B66" s="6" t="n">
         <f aca="false">L$59*B48</f>
         <v>0.030142320303196</v>
       </c>
-      <c r="C66" s="4" t="n">
+      <c r="C66" s="6" t="n">
         <f aca="false">M$59*C48</f>
         <v>-0.0395722681426169</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="4" t="n">
+      <c r="A67" s="6" t="n">
         <f aca="false">K$59*A49</f>
         <v>0.0236844122487356</v>
       </c>
-      <c r="B67" s="4" t="n">
+      <c r="B67" s="6" t="n">
         <f aca="false">L$59*B49</f>
         <v>0.015691566720734</v>
       </c>
-      <c r="C67" s="4" t="n">
+      <c r="C67" s="6" t="n">
         <f aca="false">M$59*C49</f>
         <v>-0.0345290639033747</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="4" t="n">
+      <c r="A68" s="6" t="n">
         <f aca="false">K$59*A50</f>
         <v>0.016692429723613</v>
       </c>
-      <c r="B68" s="4" t="n">
+      <c r="B68" s="6" t="n">
         <f aca="false">L$59*B50</f>
         <v>0.0457060216855454</v>
       </c>
-      <c r="C68" s="4" t="n">
+      <c r="C68" s="6" t="n">
         <f aca="false">M$59*C50</f>
         <v>-0.0319664131722955</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="4" t="n">
+      <c r="A69" s="6" t="n">
         <f aca="false">K$59*A51</f>
         <v>0.0423260769589363</v>
       </c>
-      <c r="B69" s="4" t="n">
+      <c r="B69" s="6" t="n">
         <f aca="false">L$59*B51</f>
         <v>0.00149493701378588</v>
       </c>
-      <c r="C69" s="4" t="n">
+      <c r="C69" s="6" t="n">
         <f aca="false">M$59*C51</f>
         <v>-0.00726431450731645</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="4" t="n">
+      <c r="A70" s="6" t="n">
         <f aca="false">K$59*A52</f>
         <v>0.0490676965343318</v>
       </c>
-      <c r="B70" s="4" t="n">
+      <c r="B70" s="6" t="n">
         <f aca="false">L$59*B52</f>
         <v>0.0515111649367729</v>
       </c>
-      <c r="C70" s="4" t="n">
+      <c r="C70" s="6" t="n">
         <f aca="false">M$59*C52</f>
         <v>-0.00364543919225092</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="4" t="n">
+      <c r="A71" s="6" t="n">
         <f aca="false">K$59*A53</f>
         <v>0.0480621201404268</v>
       </c>
-      <c r="B71" s="4" t="n">
+      <c r="B71" s="6" t="n">
         <f aca="false">L$59*B53</f>
         <v>0.00312268627804925</v>
       </c>
-      <c r="C71" s="4" t="n">
+      <c r="C71" s="6" t="n">
         <f aca="false">M$59*C53</f>
         <v>-0.031751019596268</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="4" t="n">
+      <c r="A72" s="6" t="n">
         <f aca="false">K$59*A54</f>
         <v>0.0243638363265937</v>
       </c>
-      <c r="B72" s="4" t="n">
+      <c r="B72" s="6" t="n">
         <f aca="false">L$59*B54</f>
         <v>0.00915172773638514</v>
       </c>
-      <c r="C72" s="4" t="n">
+      <c r="C72" s="6" t="n">
         <f aca="false">M$59*C54</f>
         <v>-0.0248263897177885</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="4" t="n">
+      <c r="A73" s="6" t="n">
         <f aca="false">K$59*A55</f>
         <v>0.0439692207317199</v>
       </c>
-      <c r="B73" s="4" t="n">
+      <c r="B73" s="6" t="n">
         <f aca="false">L$59*B55</f>
         <v>0.0147104591991053</v>
       </c>
-      <c r="C73" s="4" t="n">
+      <c r="C73" s="6" t="n">
         <f aca="false">M$59*C55</f>
         <v>-0.0194147926097537</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="7" t="n">
+      <c r="A74" s="8" t="n">
         <f aca="false">K$59*A56</f>
         <v>0.0428727400634647</v>
       </c>
-      <c r="B74" s="7" t="n">
+      <c r="B74" s="8" t="n">
         <f aca="false">L$59*B56</f>
         <v>0.0133917239457459</v>
       </c>
-      <c r="C74" s="7" t="n">
+      <c r="C74" s="8" t="n">
         <f aca="false">M$59*C56</f>
         <v>-0.012942255755858</v>
       </c>
@@ -2034,84 +2328,84 @@
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="4"/>
+      <c r="A75" s="6"/>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="4" t="n">
+      <c r="A76" s="6" t="n">
         <f aca="false">SUM(A62:C62)</f>
         <v>0.0141965350688645</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="4" t="n">
+      <c r="A77" s="6" t="n">
         <f aca="false">SUM(A63:C63)</f>
         <v>0.0228260392577935</v>
       </c>
-      <c r="B77" s="8"/>
-      <c r="C77" s="8"/>
+      <c r="B77" s="9"/>
+      <c r="C77" s="9"/>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="4" t="n">
+      <c r="A78" s="6" t="n">
         <f aca="false">SUM(A64:C64)</f>
         <v>0.0393891869125942</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="4" t="n">
+      <c r="A79" s="6" t="n">
         <f aca="false">SUM(A65:C65)</f>
         <v>0.057093090804489</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="4" t="n">
+      <c r="A80" s="6" t="n">
         <f aca="false">SUM(A66:C66)</f>
         <v>0.0197294245364713</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="4" t="n">
+      <c r="A81" s="6" t="n">
         <f aca="false">SUM(A67:C67)</f>
         <v>0.00484691506609497</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="4" t="n">
+      <c r="A82" s="6" t="n">
         <f aca="false">SUM(A68:C68)</f>
         <v>0.0304320382368629</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="4" t="n">
+      <c r="A83" s="6" t="n">
         <f aca="false">SUM(A69:C69)</f>
         <v>0.0365566994654057</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="4" t="n">
+      <c r="A84" s="6" t="n">
         <f aca="false">SUM(A70:C70)</f>
         <v>0.0969334222788538</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="4" t="n">
+      <c r="A85" s="6" t="n">
         <f aca="false">SUM(A71:C71)</f>
         <v>0.0194337868222081</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="4" t="n">
+      <c r="A86" s="6" t="n">
         <f aca="false">SUM(A72:C72)</f>
         <v>0.00868917434519041</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="4" t="n">
+      <c r="A87" s="6" t="n">
         <f aca="false">SUM(A73:C73)</f>
         <v>0.0392648873210714</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="7" t="n">
+      <c r="A88" s="8" t="n">
         <f aca="false">SUM(A74:C74)</f>
         <v>0.0433222082533526</v>
       </c>
@@ -2152,7 +2446,7 @@
         <f aca="false">C91+C44</f>
         <v>0.815015202899816</v>
       </c>
-      <c r="J91" s="9"/>
+      <c r="J91" s="10"/>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="n">
@@ -2441,27 +2735,27 @@
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="5" t="n">
+      <c r="A103" s="7" t="n">
         <f aca="false">$O$43*K$59*$E56</f>
         <v>-0.00808026654753169</v>
       </c>
-      <c r="B103" s="5" t="n">
+      <c r="B103" s="7" t="n">
         <f aca="false">$O$43*L$59*$E56</f>
         <v>-0.0052818874769676</v>
       </c>
-      <c r="C103" s="5" t="n">
+      <c r="C103" s="7" t="n">
         <f aca="false">$O$43*M$59*$E56</f>
         <v>0.00458813460916335</v>
       </c>
-      <c r="D103" s="5" t="n">
+      <c r="D103" s="7" t="n">
         <f aca="false">A103+A56</f>
         <v>0.522505448803173</v>
       </c>
-      <c r="E103" s="5" t="n">
+      <c r="E103" s="7" t="n">
         <f aca="false">B103+B56</f>
         <v>0.248258613038092</v>
       </c>
-      <c r="F103" s="5" t="n">
+      <c r="F103" s="7" t="n">
         <f aca="false">C103+C56</f>
         <v>0.286669129574087</v>
       </c>
@@ -2477,12 +2771,12 @@
   </sheetData>
   <mergeCells count="20">
     <mergeCell ref="A1:I1"/>
+    <mergeCell ref="M1:T1"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="E12:G12"/>
     <mergeCell ref="I12:K12"/>
     <mergeCell ref="A17:G17"/>
-    <mergeCell ref="A26:G26"/>
-    <mergeCell ref="I26:O26"/>
+    <mergeCell ref="A26:F26"/>
     <mergeCell ref="A35:D35"/>
     <mergeCell ref="A42:C42"/>
     <mergeCell ref="E42:E43"/>

</xml_diff>

<commit_message>
update excel and do gradients stuff for convolutional and relu layer
</commit_message>
<xml_diff>
--- a/vika_conv2.xlsx
+++ b/vika_conv2.xlsx
@@ -20,12 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
   <si>
     <t xml:space="preserve">Изображение (8x9)</t>
   </si>
   <si>
-    <t xml:space="preserve">Deconvolve</t>
+    <t xml:space="preserve">Deconvolve (local gradients for convolutional layer)</t>
   </si>
   <si>
     <t xml:space="preserve">Ядро свёртки</t>
@@ -40,7 +40,40 @@
     <t xml:space="preserve">Применение ядра свёртки к изображению</t>
   </si>
   <si>
+    <t xml:space="preserve">Корректировка весов</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deconvolve (input * relu grads)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">w11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">w12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">w13</t>
+  </si>
+  <si>
     <t xml:space="preserve">ReLU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">w21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">w22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">w23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">w31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">w32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">w33</t>
   </si>
   <si>
     <t xml:space="preserve">Maxpooling</t>
@@ -97,9 +130,6 @@
     <t xml:space="preserve">не учавствует в maxpool</t>
   </si>
   <si>
-    <t xml:space="preserve">Корректировка весов</t>
-  </si>
-  <si>
     <t xml:space="preserve">Новые веса</t>
   </si>
 </sst>
@@ -147,12 +177,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9D85BE"/>
+        <bgColor rgb="FF808080"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -201,7 +237,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -214,11 +250,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -230,11 +274,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -304,7 +348,7 @@
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF9D85BE"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
@@ -323,10 +367,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T104"/>
+  <dimension ref="A1:AL104"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q18" activeCellId="0" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -408,7 +452,7 @@
         <v>0.0173512948057014</v>
       </c>
       <c r="T2" s="0" t="n">
-        <f aca="false">N25*$I$13+O25*$J$13+P25*$K$13+N26*$I$14+O26*$J$14+P26*$K$14+N27*$I$15+O27*$J$15+P27*$K$15</f>
+        <f aca="false">N25*$I$13+O25*$J$13+P25*$K$13+N26*$I$14+O26*$J$14+N27*$I$15+O27*$J$15+P27*$K$15</f>
         <v>0.00648188669456955</v>
       </c>
     </row>
@@ -466,7 +510,7 @@
         <v>-0.00296846771406084</v>
       </c>
       <c r="T3" s="0" t="n">
-        <f aca="false">N26*$I$13+O26*$J$13+P26*$K$13+N27*$I$14+O27*$J$14+P27*$K$14+N28*$I$15+O28*$J$15+P28*$K$15</f>
+        <f aca="false">N26*$I$13+O26*$J$13+N27*$I$14+O27*$J$14+P27*$K$14+N28*$I$15+O28*$J$15+P28*$K$15</f>
         <v>0.00735880893674776</v>
       </c>
     </row>
@@ -814,7 +858,7 @@
         <v>-0.0259591772205384</v>
       </c>
       <c r="T9" s="0" t="n">
-        <f aca="false">N32*$I$13+O32*$J$13+P32*$K$13+N33*$I$14+O33*$J$14+P33*$K$14+N34*$I$15+O34*$J$15+P34*$K$15</f>
+        <f aca="false">N32*$I$13+O32*$J$13+P32*$K$13+N33*$I$14+O33*$J$14+P33*$K$14+N34*$I$15+O34*$J$15</f>
         <v>-0.0390671238143118</v>
       </c>
     </row>
@@ -872,7 +916,7 @@
         <v>-0.01582494642678</v>
       </c>
       <c r="T10" s="0" t="n">
-        <f aca="false">N33*$I$13+O33*$J$13+P33*$K$13+N34*$I$14+O34*$J$14+P34*$K$14+N35*$I$15+O35*$J$15+P35*$K$15</f>
+        <f aca="false">N33*$I$13+O33*$J$13+P33*$K$13+N34*$I$14+O34*$J$14+N35*$I$15+O35*$J$15+P35*$K$15</f>
         <v>0</v>
       </c>
     </row>
@@ -928,7 +972,7 @@
         <v>-0.434362980782524</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>-0.0622858128130198</v>
       </c>
@@ -963,7 +1007,7 @@
         <v>-0.0622858128130198</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>-0.434362980782524</v>
       </c>
@@ -1008,6 +1052,12 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
+      <c r="I17" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q17" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
@@ -1034,6 +1084,99 @@
         <f aca="false">$A$13*F2+$B$13*G2+$C$13*H2+$A$14*F3+$B$14*G3+$C$14*H3+$A$15*F4+$B$15*G4+$C$15*H4</f>
         <v>0.24138013677554</v>
       </c>
+      <c r="I18" s="3" t="n">
+        <f aca="false">SUM(Q18:V24)</f>
+        <v>-0.0224888606263517</v>
+      </c>
+      <c r="J18" s="3" t="n">
+        <f aca="false">SUM(Y18:AD24)</f>
+        <v>0.168916793186723</v>
+      </c>
+      <c r="K18" s="3" t="n">
+        <f aca="false">SUM(AG18:AL24)</f>
+        <v>0.113976679350958</v>
+      </c>
+      <c r="P18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q18" s="0" t="n">
+        <f aca="false">A2*I27</f>
+        <v>-0.00141965350688645</v>
+      </c>
+      <c r="R18" s="0" t="n">
+        <f aca="false">B2*J27</f>
+        <v>0</v>
+      </c>
+      <c r="S18" s="0" t="n">
+        <f aca="false">C2*K27</f>
+        <v>0.00684781177733805</v>
+      </c>
+      <c r="T18" s="0" t="n">
+        <f aca="false">D2*L27</f>
+        <v>0</v>
+      </c>
+      <c r="U18" s="0" t="n">
+        <f aca="false">E2*M27</f>
+        <v>0</v>
+      </c>
+      <c r="V18" s="0" t="n">
+        <f aca="false">F2*N27</f>
+        <v>0.0236335121475565</v>
+      </c>
+      <c r="X18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y18" s="0" t="n">
+        <f aca="false">B2*I27</f>
+        <v>0.0028393070137729</v>
+      </c>
+      <c r="Z18" s="0" t="n">
+        <f aca="false">C2*J27</f>
+        <v>0</v>
+      </c>
+      <c r="AA18" s="0" t="n">
+        <f aca="false">D2*K27</f>
+        <v>0.0091304157031174</v>
+      </c>
+      <c r="AB18" s="0" t="n">
+        <f aca="false">E2*L27</f>
+        <v>0</v>
+      </c>
+      <c r="AC18" s="0" t="n">
+        <f aca="false">F2*M27</f>
+        <v>0</v>
+      </c>
+      <c r="AD18" s="0" t="n">
+        <f aca="false">G2*N27</f>
+        <v>0.0275724308388159</v>
+      </c>
+      <c r="AF18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AG18" s="0" t="n">
+        <f aca="false">C2*I27</f>
+        <v>0.00425896052065935</v>
+      </c>
+      <c r="AH18" s="0" t="n">
+        <f aca="false">D2*J27</f>
+        <v>0</v>
+      </c>
+      <c r="AI18" s="0" t="n">
+        <f aca="false">E2*K27</f>
+        <v>0.0114130196288968</v>
+      </c>
+      <c r="AJ18" s="0" t="n">
+        <f aca="false">F2*L27</f>
+        <v>0</v>
+      </c>
+      <c r="AK18" s="0" t="n">
+        <f aca="false">G2*M27</f>
+        <v>0</v>
+      </c>
+      <c r="AL18" s="0" t="n">
+        <f aca="false">H2*N27</f>
+        <v>0.0315113495300753</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
@@ -1060,6 +1203,90 @@
         <f aca="false">$A$13*F3+$B$13*G3+$C$13*H3+$A$14*F4+$B$14*G4+$C$14*H4+$A$15*F5+$B$15*G5+$C$15*H5</f>
         <v>-0.244897984180467</v>
       </c>
+      <c r="I19" s="3" t="n">
+        <f aca="false">SUM(Q26:V32)</f>
+        <v>0.0508701468921475</v>
+      </c>
+      <c r="J19" s="3" t="n">
+        <f aca="false">SUM(Y26:AD32)</f>
+        <v>0.040414305318359</v>
+      </c>
+      <c r="K19" s="3" t="n">
+        <f aca="false">SUM(AG26:AL32)</f>
+        <v>0.168374062997019</v>
+      </c>
+      <c r="Q19" s="0" t="n">
+        <f aca="false">A3*I28</f>
+        <v>-0</v>
+      </c>
+      <c r="R19" s="0" t="n">
+        <f aca="false">B3*J28</f>
+        <v>-0</v>
+      </c>
+      <c r="S19" s="0" t="n">
+        <f aca="false">C3*K28</f>
+        <v>0</v>
+      </c>
+      <c r="T19" s="0" t="n">
+        <f aca="false">D3*L28</f>
+        <v>0</v>
+      </c>
+      <c r="U19" s="0" t="n">
+        <f aca="false">E3*M28</f>
+        <v>0</v>
+      </c>
+      <c r="V19" s="0" t="n">
+        <f aca="false">F3*N28</f>
+        <v>0</v>
+      </c>
+      <c r="Y19" s="0" t="n">
+        <f aca="false">B3*I28</f>
+        <v>-0</v>
+      </c>
+      <c r="Z19" s="0" t="n">
+        <f aca="false">C3*J28</f>
+        <v>0</v>
+      </c>
+      <c r="AA19" s="0" t="n">
+        <f aca="false">D3*K28</f>
+        <v>0</v>
+      </c>
+      <c r="AB19" s="0" t="n">
+        <f aca="false">E3*L28</f>
+        <v>0</v>
+      </c>
+      <c r="AC19" s="0" t="n">
+        <f aca="false">F3*M28</f>
+        <v>0</v>
+      </c>
+      <c r="AD19" s="0" t="n">
+        <f aca="false">G3*N28</f>
+        <v>0</v>
+      </c>
+      <c r="AG19" s="0" t="n">
+        <f aca="false">C3*I28</f>
+        <v>0</v>
+      </c>
+      <c r="AH19" s="0" t="n">
+        <f aca="false">D3*J28</f>
+        <v>0</v>
+      </c>
+      <c r="AI19" s="0" t="n">
+        <f aca="false">E3*K28</f>
+        <v>0</v>
+      </c>
+      <c r="AJ19" s="0" t="n">
+        <f aca="false">F3*L28</f>
+        <v>0</v>
+      </c>
+      <c r="AK19" s="0" t="n">
+        <f aca="false">G3*M28</f>
+        <v>0</v>
+      </c>
+      <c r="AL19" s="0" t="n">
+        <f aca="false">H3*N28</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
@@ -1086,6 +1313,90 @@
         <f aca="false">$A$13*F4+$B$13*G4+$C$13*H4+$A$14*F5+$B$14*G5+$C$14*H5+$A$15*F6+$B$15*G6+$C$15*H6</f>
         <v>-0.278655585841809</v>
       </c>
+      <c r="I20" s="3" t="n">
+        <f aca="false">SUM(Q35:V41)</f>
+        <v>0.060022761582676</v>
+      </c>
+      <c r="J20" s="3" t="n">
+        <f aca="false">SUM(Y34:AD41)</f>
+        <v>0.195631447005132</v>
+      </c>
+      <c r="K20" s="3" t="n">
+        <f aca="false">SUM(AG34:AL41)</f>
+        <v>0.0519048245896358</v>
+      </c>
+      <c r="Q20" s="0" t="n">
+        <f aca="false">A4*I29</f>
+        <v>-0</v>
+      </c>
+      <c r="R20" s="0" t="n">
+        <f aca="false">B4*J29</f>
+        <v>0</v>
+      </c>
+      <c r="S20" s="0" t="n">
+        <f aca="false">C4*K29</f>
+        <v>-0</v>
+      </c>
+      <c r="T20" s="0" t="n">
+        <f aca="false">D4*L29</f>
+        <v>0</v>
+      </c>
+      <c r="U20" s="0" t="n">
+        <f aca="false">E4*M29</f>
+        <v>0</v>
+      </c>
+      <c r="V20" s="0" t="n">
+        <f aca="false">F4*N29</f>
+        <v>0</v>
+      </c>
+      <c r="Y20" s="0" t="n">
+        <f aca="false">B4*I29</f>
+        <v>0</v>
+      </c>
+      <c r="Z20" s="0" t="n">
+        <f aca="false">C4*J29</f>
+        <v>-0</v>
+      </c>
+      <c r="AA20" s="0" t="n">
+        <f aca="false">D4*K29</f>
+        <v>0</v>
+      </c>
+      <c r="AB20" s="0" t="n">
+        <f aca="false">E4*L29</f>
+        <v>0</v>
+      </c>
+      <c r="AC20" s="0" t="n">
+        <f aca="false">F4*M29</f>
+        <v>0</v>
+      </c>
+      <c r="AD20" s="0" t="n">
+        <f aca="false">G4*N29</f>
+        <v>0</v>
+      </c>
+      <c r="AG20" s="0" t="n">
+        <f aca="false">C4*I29</f>
+        <v>-0</v>
+      </c>
+      <c r="AH20" s="0" t="n">
+        <f aca="false">D4*J29</f>
+        <v>0</v>
+      </c>
+      <c r="AI20" s="0" t="n">
+        <f aca="false">E4*K29</f>
+        <v>0</v>
+      </c>
+      <c r="AJ20" s="0" t="n">
+        <f aca="false">F4*L29</f>
+        <v>0</v>
+      </c>
+      <c r="AK20" s="0" t="n">
+        <f aca="false">G4*M29</f>
+        <v>0</v>
+      </c>
+      <c r="AL20" s="0" t="n">
+        <f aca="false">H4*N29</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
@@ -1112,6 +1423,79 @@
         <f aca="false">$A$13*F5+$B$13*G5+$C$13*H5+$A$14*F6+$B$14*G6+$C$14*H6+$A$15*F7+$B$15*G7+$C$15*H7</f>
         <v>0.0872007548167718</v>
       </c>
+      <c r="I21" s="4"/>
+      <c r="Q21" s="0" t="n">
+        <f aca="false">A5*I30</f>
+        <v>-0.0142732727011222</v>
+      </c>
+      <c r="R21" s="0" t="n">
+        <f aca="false">B5*J30</f>
+        <v>0</v>
+      </c>
+      <c r="S21" s="0" t="n">
+        <f aca="false">C5*K30</f>
+        <v>0</v>
+      </c>
+      <c r="T21" s="0" t="n">
+        <f aca="false">D5*L30</f>
+        <v>-0.00552423887021197</v>
+      </c>
+      <c r="U21" s="0" t="n">
+        <f aca="false">E5*M30</f>
+        <v>0</v>
+      </c>
+      <c r="V21" s="0" t="n">
+        <f aca="false">F5*N30</f>
+        <v>0.00145407451982849</v>
+      </c>
+      <c r="Y21" s="0" t="n">
+        <f aca="false">B5*I30</f>
+        <v>0.0148442036091671</v>
+      </c>
+      <c r="Z21" s="0" t="n">
+        <f aca="false">C5*J30</f>
+        <v>0</v>
+      </c>
+      <c r="AA21" s="0" t="n">
+        <f aca="false">D5*K30</f>
+        <v>-0</v>
+      </c>
+      <c r="AB21" s="0" t="n">
+        <f aca="false">E5*L30</f>
+        <v>0.00572153311557668</v>
+      </c>
+      <c r="AC21" s="0" t="n">
+        <f aca="false">F5*M30</f>
+        <v>0</v>
+      </c>
+      <c r="AD21" s="0" t="n">
+        <f aca="false">G5*N30</f>
+        <v>0.00150254367048944</v>
+      </c>
+      <c r="AG21" s="0" t="n">
+        <f aca="false">C5*I30</f>
+        <v>0.015415134517212</v>
+      </c>
+      <c r="AH21" s="0" t="n">
+        <f aca="false">D5*J30</f>
+        <v>-0</v>
+      </c>
+      <c r="AI21" s="0" t="n">
+        <f aca="false">E5*K30</f>
+        <v>0</v>
+      </c>
+      <c r="AJ21" s="0" t="n">
+        <f aca="false">F5*L30</f>
+        <v>0.00591882736094139</v>
+      </c>
+      <c r="AK21" s="0" t="n">
+        <f aca="false">G5*M30</f>
+        <v>0</v>
+      </c>
+      <c r="AL21" s="0" t="n">
+        <f aca="false">H5*N30</f>
+        <v>0.00155101282115039</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
@@ -1138,6 +1522,78 @@
         <f aca="false">$A$13*F6+$B$13*G6+$C$13*H6+$A$14*F7+$B$14*G7+$C$14*H7+$A$15*F8+$B$15*G8+$C$15*H8</f>
         <v>0.088960978417416</v>
       </c>
+      <c r="Q22" s="0" t="n">
+        <f aca="false">A6*I31</f>
+        <v>-0</v>
+      </c>
+      <c r="R22" s="0" t="n">
+        <f aca="false">B6*J31</f>
+        <v>0</v>
+      </c>
+      <c r="S22" s="0" t="n">
+        <f aca="false">C6*K31</f>
+        <v>0.010651213382902</v>
+      </c>
+      <c r="T22" s="0" t="n">
+        <f aca="false">D6*L31</f>
+        <v>0</v>
+      </c>
+      <c r="U22" s="0" t="n">
+        <f aca="false">E6*M31</f>
+        <v>-0</v>
+      </c>
+      <c r="V22" s="0" t="n">
+        <f aca="false">F6*N31</f>
+        <v>0</v>
+      </c>
+      <c r="Y22" s="0" t="n">
+        <f aca="false">B6*I31</f>
+        <v>0</v>
+      </c>
+      <c r="Z22" s="0" t="n">
+        <f aca="false">C6*J31</f>
+        <v>0</v>
+      </c>
+      <c r="AA22" s="0" t="n">
+        <f aca="false">D6*K31</f>
+        <v>0.0109555337652706</v>
+      </c>
+      <c r="AB22" s="0" t="n">
+        <f aca="false">E6*L31</f>
+        <v>-0</v>
+      </c>
+      <c r="AC22" s="0" t="n">
+        <f aca="false">F6*M31</f>
+        <v>0</v>
+      </c>
+      <c r="AD22" s="0" t="n">
+        <f aca="false">G6*N31</f>
+        <v>0</v>
+      </c>
+      <c r="AG22" s="0" t="n">
+        <f aca="false">C6*I31</f>
+        <v>0</v>
+      </c>
+      <c r="AH22" s="0" t="n">
+        <f aca="false">D6*J31</f>
+        <v>0</v>
+      </c>
+      <c r="AI22" s="0" t="n">
+        <f aca="false">E6*K31</f>
+        <v>-0.0112598541476393</v>
+      </c>
+      <c r="AJ22" s="0" t="n">
+        <f aca="false">F6*L31</f>
+        <v>0</v>
+      </c>
+      <c r="AK22" s="0" t="n">
+        <f aca="false">G6*M31</f>
+        <v>0</v>
+      </c>
+      <c r="AL22" s="0" t="n">
+        <f aca="false">H6*N31</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
@@ -1164,6 +1620,78 @@
         <f aca="false">$A$13*F7+$B$13*G7+$C$13*H7+$A$14*F8+$B$14*G8+$C$14*H8+$A$15*F9+$B$15*G9+$C$15*H9</f>
         <v>0.122561913243983</v>
       </c>
+      <c r="Q23" s="0" t="n">
+        <f aca="false">A7*I32</f>
+        <v>-0.0149882467808163</v>
+      </c>
+      <c r="R23" s="0" t="n">
+        <f aca="false">B7*J32</f>
+        <v>0</v>
+      </c>
+      <c r="S23" s="0" t="n">
+        <f aca="false">C7*K32</f>
+        <v>0</v>
+      </c>
+      <c r="T23" s="0" t="n">
+        <f aca="false">D7*L32</f>
+        <v>0</v>
+      </c>
+      <c r="U23" s="0" t="n">
+        <f aca="false">E7*M32</f>
+        <v>0</v>
+      </c>
+      <c r="V23" s="0" t="n">
+        <f aca="false">F7*N32</f>
+        <v>-0.0445893742482728</v>
+      </c>
+      <c r="Y23" s="0" t="n">
+        <f aca="false">B7*I32</f>
+        <v>0.0153538137754704</v>
+      </c>
+      <c r="Z23" s="0" t="n">
+        <f aca="false">C7*J32</f>
+        <v>0</v>
+      </c>
+      <c r="AA23" s="0" t="n">
+        <f aca="false">D7*K32</f>
+        <v>0</v>
+      </c>
+      <c r="AB23" s="0" t="n">
+        <f aca="false">E7*L32</f>
+        <v>0</v>
+      </c>
+      <c r="AC23" s="0" t="n">
+        <f aca="false">F7*M32</f>
+        <v>-0</v>
+      </c>
+      <c r="AD23" s="0" t="n">
+        <f aca="false">G7*N32</f>
+        <v>0.0455587084710613</v>
+      </c>
+      <c r="AG23" s="0" t="n">
+        <f aca="false">C7*I32</f>
+        <v>0.0157193807701244</v>
+      </c>
+      <c r="AH23" s="0" t="n">
+        <f aca="false">D7*J32</f>
+        <v>0</v>
+      </c>
+      <c r="AI23" s="0" t="n">
+        <f aca="false">E7*K32</f>
+        <v>0</v>
+      </c>
+      <c r="AJ23" s="0" t="n">
+        <f aca="false">F7*L32</f>
+        <v>-0</v>
+      </c>
+      <c r="AK23" s="0" t="n">
+        <f aca="false">G7*M32</f>
+        <v>0</v>
+      </c>
+      <c r="AL23" s="0" t="n">
+        <f aca="false">H7*N32</f>
+        <v>0.0465280426938498</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
@@ -1190,21 +1718,174 @@
         <f aca="false">$A$13*F8+$B$13*G8+$C$13*H8+$A$14*F9+$B$14*G9+$C$14*H9+$A$15*F10+$B$15*G10+$C$15*H10</f>
         <v>-1.13737952260659</v>
       </c>
+      <c r="Q24" s="0" t="n">
+        <f aca="false">A8*I33</f>
+        <v>-0.00952255554288196</v>
+      </c>
+      <c r="R24" s="0" t="n">
+        <f aca="false">B8*J33</f>
+        <v>0</v>
+      </c>
+      <c r="S24" s="0" t="n">
+        <f aca="false">C8*K33</f>
+        <v>0.00443147891604711</v>
+      </c>
+      <c r="T24" s="0" t="n">
+        <f aca="false">D8*L33</f>
+        <v>0</v>
+      </c>
+      <c r="U24" s="0" t="n">
+        <f aca="false">E8*M33</f>
+        <v>0.0208103902801679</v>
+      </c>
+      <c r="V24" s="0" t="n">
+        <f aca="false">F8*N33</f>
+        <v>0</v>
+      </c>
+      <c r="Y24" s="0" t="n">
+        <f aca="false">B8*I33</f>
+        <v>0.00971689341110404</v>
+      </c>
+      <c r="Z24" s="0" t="n">
+        <f aca="false">C8*J33</f>
+        <v>0</v>
+      </c>
+      <c r="AA24" s="0" t="n">
+        <f aca="false">D8*K33</f>
+        <v>0.00451837065949901</v>
+      </c>
+      <c r="AB24" s="0" t="n">
+        <f aca="false">E8*L33</f>
+        <v>0</v>
+      </c>
+      <c r="AC24" s="0" t="n">
+        <f aca="false">F8*M33</f>
+        <v>0.0212030391533786</v>
+      </c>
+      <c r="AD24" s="0" t="n">
+        <f aca="false">G8*N33</f>
+        <v>-0</v>
+      </c>
+      <c r="AG24" s="0" t="n">
+        <f aca="false">C8*I33</f>
+        <v>0.00991123127932612</v>
+      </c>
+      <c r="AH24" s="0" t="n">
+        <f aca="false">D8*J33</f>
+        <v>0</v>
+      </c>
+      <c r="AI24" s="0" t="n">
+        <f aca="false">E8*K33</f>
+        <v>0.00460526240295092</v>
+      </c>
+      <c r="AJ24" s="0" t="n">
+        <f aca="false">F8*L33</f>
+        <v>0</v>
+      </c>
+      <c r="AK24" s="0" t="n">
+        <f aca="false">G8*M33</f>
+        <v>-0.0215956880265893</v>
+      </c>
+      <c r="AL24" s="0" t="n">
+        <f aca="false">H8*N33</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
+      <c r="A26" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
       <c r="G26" s="1"/>
       <c r="I26" s="1"/>
+      <c r="P26" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q26" s="0" t="n">
+        <f aca="false">A3*I27</f>
+        <v>-0.0127768815619781</v>
+      </c>
+      <c r="R26" s="0" t="n">
+        <f aca="false">B3*J27</f>
+        <v>-0</v>
+      </c>
+      <c r="S26" s="0" t="n">
+        <f aca="false">C3*K27</f>
+        <v>0.00251086431835729</v>
+      </c>
+      <c r="T26" s="0" t="n">
+        <f aca="false">D3*L27</f>
+        <v>0</v>
+      </c>
+      <c r="U26" s="0" t="n">
+        <f aca="false">E3*M27</f>
+        <v>0</v>
+      </c>
+      <c r="V26" s="0" t="n">
+        <f aca="false">F3*N27</f>
+        <v>0.00551448616776318</v>
+      </c>
+      <c r="X26" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y26" s="0" t="n">
+        <f aca="false">B3*I27</f>
+        <v>-0.00141965350688645</v>
+      </c>
+      <c r="Z26" s="0" t="n">
+        <f aca="false">C3*J27</f>
+        <v>0</v>
+      </c>
+      <c r="AA26" s="0" t="n">
+        <f aca="false">D3*K27</f>
+        <v>0.00273912471093522</v>
+      </c>
+      <c r="AB26" s="0" t="n">
+        <f aca="false">E3*L27</f>
+        <v>0</v>
+      </c>
+      <c r="AC26" s="0" t="n">
+        <f aca="false">F3*M27</f>
+        <v>0</v>
+      </c>
+      <c r="AD26" s="0" t="n">
+        <f aca="false">G3*N27</f>
+        <v>0.00590837803688912</v>
+      </c>
+      <c r="AF26" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG26" s="0" t="n">
+        <f aca="false">C3*I27</f>
+        <v>0.0015616188575751</v>
+      </c>
+      <c r="AH26" s="0" t="n">
+        <f aca="false">D3*J27</f>
+        <v>0</v>
+      </c>
+      <c r="AI26" s="0" t="n">
+        <f aca="false">E3*K27</f>
+        <v>0.00296738510351316</v>
+      </c>
+      <c r="AJ26" s="0" t="n">
+        <f aca="false">F3*L27</f>
+        <v>0</v>
+      </c>
+      <c r="AK26" s="0" t="n">
+        <f aca="false">G3*M27</f>
+        <v>0</v>
+      </c>
+      <c r="AL26" s="0" t="n">
+        <f aca="false">H3*N27</f>
+        <v>0.00630226990601507</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="4" t="n">
+      <c r="A27" s="6" t="n">
         <f aca="false">IF(A18&lt;0,0,A18)</f>
         <v>0.29973878860774</v>
       </c>
@@ -1212,7 +1893,7 @@
         <f aca="false">IF(B18&lt;0,0,B18)</f>
         <v>0.14573618884283</v>
       </c>
-      <c r="C27" s="4" t="n">
+      <c r="C27" s="6" t="n">
         <f aca="false">IF(C18&lt;0,0,C18)</f>
         <v>0.227470224200259</v>
       </c>
@@ -1224,33 +1905,102 @@
         <f aca="false">IF(E18&lt;0,0,E18)</f>
         <v>0.181724188351327</v>
       </c>
-      <c r="F27" s="4" t="n">
+      <c r="F27" s="6" t="n">
         <f aca="false">IF(F18&lt;0,0,F18)</f>
         <v>0.24138013677554</v>
       </c>
-      <c r="I27" s="4" t="n">
+      <c r="I27" s="6" t="n">
         <f aca="false">A76</f>
         <v>0.0141965350688645</v>
       </c>
       <c r="J27" s="0" t="n">
-        <f aca="false">IF(J18&lt;0,0,J18)</f>
-        <v>0</v>
-      </c>
-      <c r="K27" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K27" s="6" t="n">
         <f aca="false">A77</f>
         <v>0.0228260392577935</v>
       </c>
       <c r="L27" s="0" t="n">
-        <f aca="false">IF(L18&lt;0,0,L18)</f>
         <v>0</v>
       </c>
       <c r="M27" s="0" t="n">
-        <f aca="false">IF(M18&lt;0,0,M18)</f>
-        <v>0</v>
-      </c>
-      <c r="N27" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N27" s="6" t="n">
         <f aca="false">A78</f>
         <v>0.0393891869125942</v>
+      </c>
+      <c r="Q27" s="0" t="n">
+        <f aca="false">A4*I28</f>
+        <v>-0</v>
+      </c>
+      <c r="R27" s="0" t="n">
+        <f aca="false">B4*J28</f>
+        <v>0</v>
+      </c>
+      <c r="S27" s="0" t="n">
+        <f aca="false">C4*K28</f>
+        <v>-0</v>
+      </c>
+      <c r="T27" s="0" t="n">
+        <f aca="false">D4*L28</f>
+        <v>0</v>
+      </c>
+      <c r="U27" s="0" t="n">
+        <f aca="false">E4*M28</f>
+        <v>0</v>
+      </c>
+      <c r="V27" s="0" t="n">
+        <f aca="false">F4*N28</f>
+        <v>0</v>
+      </c>
+      <c r="Y27" s="0" t="n">
+        <f aca="false">B4*I28</f>
+        <v>0</v>
+      </c>
+      <c r="Z27" s="0" t="n">
+        <f aca="false">C4*J28</f>
+        <v>-0</v>
+      </c>
+      <c r="AA27" s="0" t="n">
+        <f aca="false">D4*K28</f>
+        <v>0</v>
+      </c>
+      <c r="AB27" s="0" t="n">
+        <f aca="false">E4*L28</f>
+        <v>0</v>
+      </c>
+      <c r="AC27" s="0" t="n">
+        <f aca="false">F4*M28</f>
+        <v>0</v>
+      </c>
+      <c r="AD27" s="0" t="n">
+        <f aca="false">G4*N28</f>
+        <v>0</v>
+      </c>
+      <c r="AG27" s="0" t="n">
+        <f aca="false">C4*I28</f>
+        <v>-0</v>
+      </c>
+      <c r="AH27" s="0" t="n">
+        <f aca="false">D4*J28</f>
+        <v>0</v>
+      </c>
+      <c r="AI27" s="0" t="n">
+        <f aca="false">E4*K28</f>
+        <v>0</v>
+      </c>
+      <c r="AJ27" s="0" t="n">
+        <f aca="false">F4*L28</f>
+        <v>0</v>
+      </c>
+      <c r="AK27" s="0" t="n">
+        <f aca="false">G4*M28</f>
+        <v>0</v>
+      </c>
+      <c r="AL27" s="0" t="n">
+        <f aca="false">H4*N28</f>
+        <v>0</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1279,27 +2029,93 @@
         <v>0</v>
       </c>
       <c r="I28" s="0" t="n">
-        <f aca="false">IF(I19&lt;0,0,I19)</f>
         <v>0</v>
       </c>
       <c r="J28" s="0" t="n">
-        <f aca="false">IF(J19&lt;0,0,J19)</f>
         <v>0</v>
       </c>
       <c r="K28" s="0" t="n">
-        <f aca="false">IF(K19&lt;0,0,K19)</f>
         <v>0</v>
       </c>
       <c r="L28" s="0" t="n">
-        <f aca="false">IF(L19&lt;0,0,L19)</f>
         <v>0</v>
       </c>
       <c r="M28" s="0" t="n">
-        <f aca="false">IF(M19&lt;0,0,M19)</f>
         <v>0</v>
       </c>
       <c r="N28" s="0" t="n">
-        <f aca="false">IF(N19&lt;0,0,N19)</f>
+        <v>0</v>
+      </c>
+      <c r="Q28" s="0" t="n">
+        <f aca="false">A5*I29</f>
+        <v>-0</v>
+      </c>
+      <c r="R28" s="0" t="n">
+        <f aca="false">B5*J29</f>
+        <v>0</v>
+      </c>
+      <c r="S28" s="0" t="n">
+        <f aca="false">C5*K29</f>
+        <v>0</v>
+      </c>
+      <c r="T28" s="0" t="n">
+        <f aca="false">D5*L29</f>
+        <v>-0</v>
+      </c>
+      <c r="U28" s="0" t="n">
+        <f aca="false">E5*M29</f>
+        <v>0</v>
+      </c>
+      <c r="V28" s="0" t="n">
+        <f aca="false">F5*N29</f>
+        <v>0</v>
+      </c>
+      <c r="Y28" s="0" t="n">
+        <f aca="false">B5*I29</f>
+        <v>0</v>
+      </c>
+      <c r="Z28" s="0" t="n">
+        <f aca="false">C5*J29</f>
+        <v>0</v>
+      </c>
+      <c r="AA28" s="0" t="n">
+        <f aca="false">D5*K29</f>
+        <v>-0</v>
+      </c>
+      <c r="AB28" s="0" t="n">
+        <f aca="false">E5*L29</f>
+        <v>0</v>
+      </c>
+      <c r="AC28" s="0" t="n">
+        <f aca="false">F5*M29</f>
+        <v>0</v>
+      </c>
+      <c r="AD28" s="0" t="n">
+        <f aca="false">G5*N29</f>
+        <v>0</v>
+      </c>
+      <c r="AG28" s="0" t="n">
+        <f aca="false">C5*I29</f>
+        <v>0</v>
+      </c>
+      <c r="AH28" s="0" t="n">
+        <f aca="false">D5*J29</f>
+        <v>-0</v>
+      </c>
+      <c r="AI28" s="0" t="n">
+        <f aca="false">E5*K29</f>
+        <v>0</v>
+      </c>
+      <c r="AJ28" s="0" t="n">
+        <f aca="false">F5*L29</f>
+        <v>0</v>
+      </c>
+      <c r="AK28" s="0" t="n">
+        <f aca="false">G5*M29</f>
+        <v>0</v>
+      </c>
+      <c r="AL28" s="0" t="n">
+        <f aca="false">H5*N29</f>
         <v>0</v>
       </c>
     </row>
@@ -1329,32 +2145,98 @@
         <v>0</v>
       </c>
       <c r="I29" s="0" t="n">
-        <f aca="false">IF(I20&lt;0,0,I20)</f>
         <v>0</v>
       </c>
       <c r="J29" s="0" t="n">
-        <f aca="false">IF(J20&lt;0,0,J20)</f>
         <v>0</v>
       </c>
       <c r="K29" s="0" t="n">
-        <f aca="false">IF(K20&lt;0,0,K20)</f>
         <v>0</v>
       </c>
       <c r="L29" s="0" t="n">
-        <f aca="false">IF(L20&lt;0,0,L20)</f>
         <v>0</v>
       </c>
       <c r="M29" s="0" t="n">
-        <f aca="false">IF(M20&lt;0,0,M20)</f>
         <v>0</v>
       </c>
       <c r="N29" s="0" t="n">
-        <f aca="false">IF(N20&lt;0,0,N20)</f>
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="Q29" s="0" t="n">
+        <f aca="false">A6*I30</f>
+        <v>-0.0188407199654814</v>
+      </c>
+      <c r="R29" s="0" t="n">
+        <f aca="false">B6*J30</f>
+        <v>0</v>
+      </c>
+      <c r="S29" s="0" t="n">
+        <f aca="false">C6*K30</f>
+        <v>0</v>
+      </c>
+      <c r="T29" s="0" t="n">
+        <f aca="false">D6*L30</f>
+        <v>0.00710259283312967</v>
+      </c>
+      <c r="U29" s="0" t="n">
+        <f aca="false">E6*M30</f>
+        <v>-0</v>
+      </c>
+      <c r="V29" s="0" t="n">
+        <f aca="false">F6*N30</f>
+        <v>0.00184182772511609</v>
+      </c>
+      <c r="Y29" s="0" t="n">
+        <f aca="false">B6*I30</f>
+        <v>0.0194116508735263</v>
+      </c>
+      <c r="Z29" s="0" t="n">
+        <f aca="false">C6*J30</f>
+        <v>0</v>
+      </c>
+      <c r="AA29" s="0" t="n">
+        <f aca="false">D6*K30</f>
+        <v>0</v>
+      </c>
+      <c r="AB29" s="0" t="n">
+        <f aca="false">E6*L30</f>
+        <v>-0.00729988707849438</v>
+      </c>
+      <c r="AC29" s="0" t="n">
+        <f aca="false">F6*M30</f>
+        <v>0</v>
+      </c>
+      <c r="AD29" s="0" t="n">
+        <f aca="false">G6*N30</f>
+        <v>0.00189029687577704</v>
+      </c>
+      <c r="AG29" s="0" t="n">
+        <f aca="false">C6*I30</f>
+        <v>0.0199825817815711</v>
+      </c>
+      <c r="AH29" s="0" t="n">
+        <f aca="false">D6*J30</f>
+        <v>0</v>
+      </c>
+      <c r="AI29" s="0" t="n">
+        <f aca="false">E6*K30</f>
+        <v>-0</v>
+      </c>
+      <c r="AJ29" s="0" t="n">
+        <f aca="false">F6*L30</f>
+        <v>0.0074971813238591</v>
+      </c>
+      <c r="AK29" s="0" t="n">
+        <f aca="false">G6*M30</f>
+        <v>0</v>
+      </c>
+      <c r="AL29" s="0" t="n">
+        <f aca="false">H6*N30</f>
+        <v>0.00193876602643799</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="4" t="n">
+      <c r="A30" s="6" t="n">
         <f aca="false">IF(A21&lt;0,0,A21)</f>
         <v>0.0536414502436412</v>
       </c>
@@ -1366,7 +2248,7 @@
         <f aca="false">IF(C21&lt;0,0,C21)</f>
         <v>0</v>
       </c>
-      <c r="D30" s="4" t="n">
+      <c r="D30" s="6" t="n">
         <f aca="false">IF(D21&lt;0,0,D21)</f>
         <v>0.0639727464095352</v>
       </c>
@@ -1374,33 +2256,102 @@
         <f aca="false">IF(E21&lt;0,0,E21)</f>
         <v>0.0539002998319844</v>
       </c>
-      <c r="F30" s="4" t="n">
+      <c r="F30" s="6" t="n">
         <f aca="false">IF(F21&lt;0,0,F21)</f>
         <v>0.0872007548167718</v>
       </c>
-      <c r="I30" s="4" t="n">
+      <c r="I30" s="6" t="n">
         <f aca="false">A79</f>
         <v>0.057093090804489</v>
       </c>
       <c r="J30" s="0" t="n">
-        <f aca="false">IF(J21&lt;0,0,J21)</f>
         <v>0</v>
       </c>
       <c r="K30" s="0" t="n">
-        <f aca="false">IF(K21&lt;0,0,K21)</f>
-        <v>0</v>
-      </c>
-      <c r="L30" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L30" s="6" t="n">
         <f aca="false">A80</f>
         <v>0.0197294245364713</v>
       </c>
       <c r="M30" s="0" t="n">
-        <f aca="false">IF(M21&lt;0,0,M21)</f>
-        <v>0</v>
-      </c>
-      <c r="N30" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N30" s="6" t="n">
         <f aca="false">A81</f>
         <v>0.00484691506609497</v>
+      </c>
+      <c r="Q30" s="0" t="n">
+        <f aca="false">A7*I31</f>
+        <v>-0</v>
+      </c>
+      <c r="R30" s="0" t="n">
+        <f aca="false">B7*J31</f>
+        <v>0</v>
+      </c>
+      <c r="S30" s="0" t="n">
+        <f aca="false">C7*K31</f>
+        <v>0.0130857764418511</v>
+      </c>
+      <c r="T30" s="0" t="n">
+        <f aca="false">D7*L31</f>
+        <v>0</v>
+      </c>
+      <c r="U30" s="0" t="n">
+        <f aca="false">E7*M31</f>
+        <v>0</v>
+      </c>
+      <c r="V30" s="0" t="n">
+        <f aca="false">F7*N31</f>
+        <v>-0</v>
+      </c>
+      <c r="Y30" s="0" t="n">
+        <f aca="false">B7*I31</f>
+        <v>0</v>
+      </c>
+      <c r="Z30" s="0" t="n">
+        <f aca="false">C7*J31</f>
+        <v>0</v>
+      </c>
+      <c r="AA30" s="0" t="n">
+        <f aca="false">D7*K31</f>
+        <v>0.0133900968242197</v>
+      </c>
+      <c r="AB30" s="0" t="n">
+        <f aca="false">E7*L31</f>
+        <v>0</v>
+      </c>
+      <c r="AC30" s="0" t="n">
+        <f aca="false">F7*M31</f>
+        <v>-0</v>
+      </c>
+      <c r="AD30" s="0" t="n">
+        <f aca="false">G7*N31</f>
+        <v>0</v>
+      </c>
+      <c r="AG30" s="0" t="n">
+        <f aca="false">C7*I31</f>
+        <v>0</v>
+      </c>
+      <c r="AH30" s="0" t="n">
+        <f aca="false">D7*J31</f>
+        <v>0</v>
+      </c>
+      <c r="AI30" s="0" t="n">
+        <f aca="false">E7*K31</f>
+        <v>0.0136944172065883</v>
+      </c>
+      <c r="AJ30" s="0" t="n">
+        <f aca="false">F7*L31</f>
+        <v>-0</v>
+      </c>
+      <c r="AK30" s="0" t="n">
+        <f aca="false">G7*M31</f>
+        <v>0</v>
+      </c>
+      <c r="AL30" s="0" t="n">
+        <f aca="false">H7*N31</f>
+        <v>0</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1412,7 +2363,7 @@
         <f aca="false">IF(B22&lt;0,0,B22)</f>
         <v>0</v>
       </c>
-      <c r="C31" s="4" t="n">
+      <c r="C31" s="6" t="n">
         <f aca="false">IF(C22&lt;0,0,C22)</f>
         <v>0</v>
       </c>
@@ -1429,32 +2380,99 @@
         <v>0.088960978417416</v>
       </c>
       <c r="I31" s="0" t="n">
-        <f aca="false">IF(I22&lt;0,0,I22)</f>
         <v>0</v>
       </c>
       <c r="J31" s="0" t="n">
-        <f aca="false">IF(J22&lt;0,0,J22)</f>
-        <v>0</v>
-      </c>
-      <c r="K31" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K31" s="6" t="n">
         <f aca="false">A82</f>
         <v>0.0304320382368629</v>
       </c>
       <c r="L31" s="0" t="n">
-        <f aca="false">IF(L22&lt;0,0,L22)</f>
         <v>0</v>
       </c>
       <c r="M31" s="0" t="n">
-        <f aca="false">IF(M22&lt;0,0,M22)</f>
         <v>0</v>
       </c>
       <c r="N31" s="0" t="n">
-        <f aca="false">IF(N22&lt;0,0,N22)</f>
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="Q31" s="0" t="n">
+        <f aca="false">A8*I32</f>
+        <v>-0.0179127827380488</v>
+      </c>
+      <c r="R31" s="0" t="n">
+        <f aca="false">B8*J32</f>
+        <v>0</v>
+      </c>
+      <c r="S31" s="0" t="n">
+        <f aca="false">C8*K32</f>
+        <v>0</v>
+      </c>
+      <c r="T31" s="0" t="n">
+        <f aca="false">D8*L32</f>
+        <v>0</v>
+      </c>
+      <c r="U31" s="0" t="n">
+        <f aca="false">E8*M32</f>
+        <v>0</v>
+      </c>
+      <c r="V31" s="0" t="n">
+        <f aca="false">F8*N32</f>
+        <v>0.0523440480305811</v>
+      </c>
+      <c r="Y31" s="0" t="n">
+        <f aca="false">B8*I32</f>
+        <v>0.0182783497327028</v>
+      </c>
+      <c r="Z31" s="0" t="n">
+        <f aca="false">C8*J32</f>
+        <v>0</v>
+      </c>
+      <c r="AA31" s="0" t="n">
+        <f aca="false">D8*K32</f>
+        <v>0</v>
+      </c>
+      <c r="AB31" s="0" t="n">
+        <f aca="false">E8*L32</f>
+        <v>0</v>
+      </c>
+      <c r="AC31" s="0" t="n">
+        <f aca="false">F8*M32</f>
+        <v>0</v>
+      </c>
+      <c r="AD31" s="0" t="n">
+        <f aca="false">G8*N32</f>
+        <v>-0.0533133822533696</v>
+      </c>
+      <c r="AG31" s="0" t="n">
+        <f aca="false">C8*I32</f>
+        <v>0.0186439167273569</v>
+      </c>
+      <c r="AH31" s="0" t="n">
+        <f aca="false">D8*J32</f>
+        <v>0</v>
+      </c>
+      <c r="AI31" s="0" t="n">
+        <f aca="false">E8*K32</f>
+        <v>0</v>
+      </c>
+      <c r="AJ31" s="0" t="n">
+        <f aca="false">F8*L32</f>
+        <v>0</v>
+      </c>
+      <c r="AK31" s="0" t="n">
+        <f aca="false">G8*M32</f>
+        <v>-0</v>
+      </c>
+      <c r="AL31" s="0" t="n">
+        <f aca="false">H8*N32</f>
+        <v>0.0542827164761582</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="4" t="n">
+      <c r="A32" s="6" t="n">
         <f aca="false">IF(A23&lt;0,0,A23)</f>
         <v>0.111562568718053</v>
       </c>
@@ -1474,37 +2492,105 @@
         <f aca="false">IF(E23&lt;0,0,E23)</f>
         <v>0</v>
       </c>
-      <c r="F32" s="4" t="n">
+      <c r="F32" s="6" t="n">
         <f aca="false">IF(F23&lt;0,0,F23)</f>
         <v>0.122561913243983</v>
       </c>
-      <c r="I32" s="4" t="n">
+      <c r="I32" s="6" t="n">
         <f aca="false">A83</f>
         <v>0.0365566994654057</v>
       </c>
       <c r="J32" s="0" t="n">
-        <f aca="false">IF(J23&lt;0,0,J23)</f>
         <v>0</v>
       </c>
       <c r="K32" s="0" t="n">
-        <f aca="false">IF(K23&lt;0,0,K23)</f>
         <v>0</v>
       </c>
       <c r="L32" s="0" t="n">
-        <f aca="false">IF(L23&lt;0,0,L23)</f>
         <v>0</v>
       </c>
       <c r="M32" s="0" t="n">
-        <f aca="false">IF(M23&lt;0,0,M23)</f>
-        <v>0</v>
-      </c>
-      <c r="N32" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N32" s="6" t="n">
         <f aca="false">A84</f>
         <v>0.0969334222788538</v>
       </c>
+      <c r="Q32" s="0" t="n">
+        <f aca="false">A9*I33</f>
+        <v>-0.0110772584886586</v>
+      </c>
+      <c r="R32" s="0" t="n">
+        <f aca="false">B9*J33</f>
+        <v>0</v>
+      </c>
+      <c r="S32" s="0" t="n">
+        <f aca="false">C9*K33</f>
+        <v>0.00512661286366234</v>
+      </c>
+      <c r="T32" s="0" t="n">
+        <f aca="false">D9*L33</f>
+        <v>0</v>
+      </c>
+      <c r="U32" s="0" t="n">
+        <f aca="false">E9*M33</f>
+        <v>0.0239515812658536</v>
+      </c>
+      <c r="V32" s="0" t="n">
+        <f aca="false">F9*N33</f>
+        <v>0</v>
+      </c>
+      <c r="Y32" s="0" t="n">
+        <f aca="false">B9*I33</f>
+        <v>0.0112715963568807</v>
+      </c>
+      <c r="Z32" s="0" t="n">
+        <f aca="false">C9*J33</f>
+        <v>0</v>
+      </c>
+      <c r="AA32" s="0" t="n">
+        <f aca="false">D9*K33</f>
+        <v>0.00521350460711425</v>
+      </c>
+      <c r="AB32" s="0" t="n">
+        <f aca="false">E9*L33</f>
+        <v>0</v>
+      </c>
+      <c r="AC32" s="0" t="n">
+        <f aca="false">F9*M33</f>
+        <v>0.0243442301390643</v>
+      </c>
+      <c r="AD32" s="0" t="n">
+        <f aca="false">G9*N33</f>
+        <v>0</v>
+      </c>
+      <c r="AG32" s="0" t="n">
+        <f aca="false">C9*I33</f>
+        <v>0.0114659342251028</v>
+      </c>
+      <c r="AH32" s="0" t="n">
+        <f aca="false">D9*J33</f>
+        <v>0</v>
+      </c>
+      <c r="AI32" s="0" t="n">
+        <f aca="false">E9*K33</f>
+        <v>0.00530039635056615</v>
+      </c>
+      <c r="AJ32" s="0" t="n">
+        <f aca="false">F9*L33</f>
+        <v>0</v>
+      </c>
+      <c r="AK32" s="0" t="n">
+        <f aca="false">G9*M33</f>
+        <v>0.024736879012275</v>
+      </c>
+      <c r="AL32" s="0" t="n">
+        <f aca="false">H9*N33</f>
+        <v>-0</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="4" t="n">
+      <c r="A33" s="6" t="n">
         <f aca="false">IF(A24&lt;0,0,A24)</f>
         <v>0.140523127955259</v>
       </c>
@@ -1512,7 +2598,7 @@
         <f aca="false">IF(B24&lt;0,0,B24)</f>
         <v>0</v>
       </c>
-      <c r="C33" s="4" t="n">
+      <c r="C33" s="6" t="n">
         <f aca="false">IF(C24&lt;0,0,C24)</f>
         <v>0</v>
       </c>
@@ -1520,7 +2606,7 @@
         <f aca="false">IF(D24&lt;0,0,D24)</f>
         <v>0</v>
       </c>
-      <c r="E33" s="4" t="n">
+      <c r="E33" s="6" t="n">
         <f aca="false">IF(E24&lt;0,0,E24)</f>
         <v>0</v>
       </c>
@@ -1528,40 +2614,168 @@
         <f aca="false">IF(F24&lt;0,0,F24)</f>
         <v>0</v>
       </c>
-      <c r="I33" s="4" t="n">
+      <c r="I33" s="6" t="n">
         <f aca="false">A85</f>
         <v>0.0194337868222081</v>
       </c>
       <c r="J33" s="0" t="n">
-        <f aca="false">IF(J24&lt;0,0,J24)</f>
-        <v>0</v>
-      </c>
-      <c r="K33" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K33" s="6" t="n">
         <f aca="false">A86</f>
         <v>0.00868917434519041</v>
       </c>
       <c r="L33" s="0" t="n">
-        <f aca="false">IF(L24&lt;0,0,L24)</f>
-        <v>0</v>
-      </c>
-      <c r="M33" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M33" s="6" t="n">
         <f aca="false">A87</f>
         <v>0.0392648873210714</v>
       </c>
       <c r="N33" s="0" t="n">
-        <f aca="false">IF(N24&lt;0,0,N24)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P34" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="X34" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y34" s="0" t="n">
+        <f aca="false">B4*I27</f>
+        <v>0.00255537631239561</v>
+      </c>
+      <c r="Z34" s="0" t="n">
+        <f aca="false">C4*J27</f>
+        <v>-0</v>
+      </c>
+      <c r="AA34" s="0" t="n">
+        <f aca="false">D4*K27</f>
+        <v>0.0045652078515587</v>
+      </c>
+      <c r="AB34" s="0" t="n">
+        <f aca="false">E4*L27</f>
+        <v>0</v>
+      </c>
+      <c r="AC34" s="0" t="n">
+        <f aca="false">F4*M27</f>
+        <v>0</v>
+      </c>
+      <c r="AD34" s="0" t="n">
+        <f aca="false">G4*N27</f>
+        <v>0.00905951298989666</v>
+      </c>
+      <c r="AF34" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG34" s="0" t="n">
+        <f aca="false">C4*I27</f>
+        <v>-0.00269734166308426</v>
+      </c>
+      <c r="AH34" s="0" t="n">
+        <f aca="false">D4*J27</f>
+        <v>0</v>
+      </c>
+      <c r="AI34" s="0" t="n">
+        <f aca="false">E4*K27</f>
+        <v>0.00479346824413664</v>
+      </c>
+      <c r="AJ34" s="0" t="n">
+        <f aca="false">F4*L27</f>
+        <v>0</v>
+      </c>
+      <c r="AK34" s="0" t="n">
+        <f aca="false">G4*M27</f>
+        <v>0</v>
+      </c>
+      <c r="AL34" s="0" t="n">
+        <f aca="false">H4*N27</f>
+        <v>0.0094534048590226</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
-    </row>
-    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q35" s="0" t="n">
+        <f aca="false">A4*I27</f>
+        <v>-0.00241341096170697</v>
+      </c>
+      <c r="R35" s="0" t="n">
+        <f aca="false">B4*J27</f>
+        <v>0</v>
+      </c>
+      <c r="S35" s="0" t="n">
+        <f aca="false">C4*K27</f>
+        <v>-0.00433694745898077</v>
+      </c>
+      <c r="T35" s="0" t="n">
+        <f aca="false">D4*L27</f>
+        <v>0</v>
+      </c>
+      <c r="U35" s="0" t="n">
+        <f aca="false">E4*M27</f>
+        <v>0</v>
+      </c>
+      <c r="V35" s="0" t="n">
+        <f aca="false">F4*N27</f>
+        <v>0.00866562112077071</v>
+      </c>
+      <c r="Y35" s="0" t="n">
+        <f aca="false">B5*I28</f>
+        <v>0</v>
+      </c>
+      <c r="Z35" s="0" t="n">
+        <f aca="false">C5*J28</f>
+        <v>0</v>
+      </c>
+      <c r="AA35" s="0" t="n">
+        <f aca="false">D5*K28</f>
+        <v>-0</v>
+      </c>
+      <c r="AB35" s="0" t="n">
+        <f aca="false">E5*L28</f>
+        <v>0</v>
+      </c>
+      <c r="AC35" s="0" t="n">
+        <f aca="false">F5*M28</f>
+        <v>0</v>
+      </c>
+      <c r="AD35" s="0" t="n">
+        <f aca="false">G5*N28</f>
+        <v>0</v>
+      </c>
+      <c r="AG35" s="0" t="n">
+        <f aca="false">C5*I28</f>
+        <v>0</v>
+      </c>
+      <c r="AH35" s="0" t="n">
+        <f aca="false">D5*J28</f>
+        <v>-0</v>
+      </c>
+      <c r="AI35" s="0" t="n">
+        <f aca="false">E5*K28</f>
+        <v>0</v>
+      </c>
+      <c r="AJ35" s="0" t="n">
+        <f aca="false">F5*L28</f>
+        <v>0</v>
+      </c>
+      <c r="AK35" s="0" t="n">
+        <f aca="false">G5*M28</f>
+        <v>0</v>
+      </c>
+      <c r="AL35" s="0" t="n">
+        <f aca="false">H5*N28</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
         <f aca="false">MAX(A27:B28)</f>
         <v>0.29973878860774</v>
@@ -1574,8 +2788,80 @@
         <f aca="false">MAX(E27:F28)</f>
         <v>0.24138013677554</v>
       </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q36" s="0" t="n">
+        <f aca="false">A5*I28</f>
+        <v>-0</v>
+      </c>
+      <c r="R36" s="0" t="n">
+        <f aca="false">B5*J28</f>
+        <v>0</v>
+      </c>
+      <c r="S36" s="0" t="n">
+        <f aca="false">C5*K28</f>
+        <v>0</v>
+      </c>
+      <c r="T36" s="0" t="n">
+        <f aca="false">D5*L28</f>
+        <v>-0</v>
+      </c>
+      <c r="U36" s="0" t="n">
+        <f aca="false">E5*M28</f>
+        <v>0</v>
+      </c>
+      <c r="V36" s="0" t="n">
+        <f aca="false">F5*N28</f>
+        <v>0</v>
+      </c>
+      <c r="Y36" s="0" t="n">
+        <f aca="false">B6*I29</f>
+        <v>0</v>
+      </c>
+      <c r="Z36" s="0" t="n">
+        <f aca="false">C6*J29</f>
+        <v>0</v>
+      </c>
+      <c r="AA36" s="0" t="n">
+        <f aca="false">D6*K29</f>
+        <v>0</v>
+      </c>
+      <c r="AB36" s="0" t="n">
+        <f aca="false">E6*L29</f>
+        <v>-0</v>
+      </c>
+      <c r="AC36" s="0" t="n">
+        <f aca="false">F6*M29</f>
+        <v>0</v>
+      </c>
+      <c r="AD36" s="0" t="n">
+        <f aca="false">G6*N29</f>
+        <v>0</v>
+      </c>
+      <c r="AG36" s="0" t="n">
+        <f aca="false">C6*I29</f>
+        <v>0</v>
+      </c>
+      <c r="AH36" s="0" t="n">
+        <f aca="false">D6*J29</f>
+        <v>0</v>
+      </c>
+      <c r="AI36" s="0" t="n">
+        <f aca="false">E6*K29</f>
+        <v>-0</v>
+      </c>
+      <c r="AJ36" s="0" t="n">
+        <f aca="false">F6*L29</f>
+        <v>0</v>
+      </c>
+      <c r="AK36" s="0" t="n">
+        <f aca="false">G6*M29</f>
+        <v>0</v>
+      </c>
+      <c r="AL36" s="0" t="n">
+        <f aca="false">H6*N29</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
         <f aca="false">MAX(A29:B30)</f>
         <v>0.053641450243641</v>
@@ -1588,8 +2874,80 @@
         <f aca="false">MAX(E29:F30)</f>
         <v>0.0872007548167718</v>
       </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q37" s="0" t="n">
+        <f aca="false">A6*I29</f>
+        <v>-0</v>
+      </c>
+      <c r="R37" s="0" t="n">
+        <f aca="false">B6*J29</f>
+        <v>0</v>
+      </c>
+      <c r="S37" s="0" t="n">
+        <f aca="false">C6*K29</f>
+        <v>0</v>
+      </c>
+      <c r="T37" s="0" t="n">
+        <f aca="false">D6*L29</f>
+        <v>0</v>
+      </c>
+      <c r="U37" s="0" t="n">
+        <f aca="false">E6*M29</f>
+        <v>-0</v>
+      </c>
+      <c r="V37" s="0" t="n">
+        <f aca="false">F6*N29</f>
+        <v>0</v>
+      </c>
+      <c r="Y37" s="0" t="n">
+        <f aca="false">B7*I30</f>
+        <v>0.0239790981378854</v>
+      </c>
+      <c r="Z37" s="0" t="n">
+        <f aca="false">C7*J30</f>
+        <v>0</v>
+      </c>
+      <c r="AA37" s="0" t="n">
+        <f aca="false">D7*K30</f>
+        <v>0</v>
+      </c>
+      <c r="AB37" s="0" t="n">
+        <f aca="false">E7*L30</f>
+        <v>0.00887824104141209</v>
+      </c>
+      <c r="AC37" s="0" t="n">
+        <f aca="false">F7*M30</f>
+        <v>-0</v>
+      </c>
+      <c r="AD37" s="0" t="n">
+        <f aca="false">G7*N30</f>
+        <v>0.00227805008106464</v>
+      </c>
+      <c r="AG37" s="0" t="n">
+        <f aca="false">C7*I30</f>
+        <v>0.0245500290459303</v>
+      </c>
+      <c r="AH37" s="0" t="n">
+        <f aca="false">D7*J30</f>
+        <v>0</v>
+      </c>
+      <c r="AI37" s="0" t="n">
+        <f aca="false">E7*K30</f>
+        <v>0</v>
+      </c>
+      <c r="AJ37" s="0" t="n">
+        <f aca="false">F7*L30</f>
+        <v>-0.0090755352867768</v>
+      </c>
+      <c r="AK37" s="0" t="n">
+        <f aca="false">G7*M30</f>
+        <v>0</v>
+      </c>
+      <c r="AL37" s="0" t="n">
+        <f aca="false">H7*N30</f>
+        <v>0.00232651923172559</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
         <f aca="false">MAX(A31:B32)</f>
         <v>0.111562568718053</v>
@@ -1602,8 +2960,80 @@
         <f aca="false">MAX(E31:F32)</f>
         <v>0.122561913243983</v>
       </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q38" s="0" t="n">
+        <f aca="false">A7*I30</f>
+        <v>-0.0234081672298405</v>
+      </c>
+      <c r="R38" s="0" t="n">
+        <f aca="false">B7*J30</f>
+        <v>0</v>
+      </c>
+      <c r="S38" s="0" t="n">
+        <f aca="false">C7*K30</f>
+        <v>0</v>
+      </c>
+      <c r="T38" s="0" t="n">
+        <f aca="false">D7*L30</f>
+        <v>0.00868094679604737</v>
+      </c>
+      <c r="U38" s="0" t="n">
+        <f aca="false">E7*M30</f>
+        <v>0</v>
+      </c>
+      <c r="V38" s="0" t="n">
+        <f aca="false">F7*N30</f>
+        <v>-0.00222958093040369</v>
+      </c>
+      <c r="Y38" s="0" t="n">
+        <f aca="false">B8*I31</f>
+        <v>0</v>
+      </c>
+      <c r="Z38" s="0" t="n">
+        <f aca="false">C8*J31</f>
+        <v>0</v>
+      </c>
+      <c r="AA38" s="0" t="n">
+        <f aca="false">D8*K31</f>
+        <v>0.0158246598831687</v>
+      </c>
+      <c r="AB38" s="0" t="n">
+        <f aca="false">E8*L31</f>
+        <v>0</v>
+      </c>
+      <c r="AC38" s="0" t="n">
+        <f aca="false">F8*M31</f>
+        <v>0</v>
+      </c>
+      <c r="AD38" s="0" t="n">
+        <f aca="false">G8*N31</f>
+        <v>-0</v>
+      </c>
+      <c r="AG38" s="0" t="n">
+        <f aca="false">C8*I31</f>
+        <v>0</v>
+      </c>
+      <c r="AH38" s="0" t="n">
+        <f aca="false">D8*J31</f>
+        <v>0</v>
+      </c>
+      <c r="AI38" s="0" t="n">
+        <f aca="false">E8*K31</f>
+        <v>0.0161289802655373</v>
+      </c>
+      <c r="AJ38" s="0" t="n">
+        <f aca="false">F8*L31</f>
+        <v>0</v>
+      </c>
+      <c r="AK38" s="0" t="n">
+        <f aca="false">G8*M31</f>
+        <v>-0</v>
+      </c>
+      <c r="AL38" s="0" t="n">
+        <f aca="false">H8*N31</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
         <f aca="false">MAX(A33:B34)</f>
         <v>0.140523127955259</v>
@@ -1616,60 +3046,280 @@
         <f aca="false">MAX(E33:F34)</f>
         <v>0</v>
       </c>
+      <c r="Q39" s="0" t="n">
+        <f aca="false">A8*I31</f>
+        <v>-0</v>
+      </c>
+      <c r="R39" s="0" t="n">
+        <f aca="false">B8*J31</f>
+        <v>0</v>
+      </c>
+      <c r="S39" s="0" t="n">
+        <f aca="false">C8*K31</f>
+        <v>0.0155203395008001</v>
+      </c>
+      <c r="T39" s="0" t="n">
+        <f aca="false">D8*L31</f>
+        <v>0</v>
+      </c>
+      <c r="U39" s="0" t="n">
+        <f aca="false">E8*M31</f>
+        <v>0</v>
+      </c>
+      <c r="V39" s="0" t="n">
+        <f aca="false">F8*N31</f>
+        <v>0</v>
+      </c>
+      <c r="Y39" s="0" t="n">
+        <f aca="false">B9*I32</f>
+        <v>0.0212028856899353</v>
+      </c>
+      <c r="Z39" s="0" t="n">
+        <f aca="false">C9*J32</f>
+        <v>0</v>
+      </c>
+      <c r="AA39" s="0" t="n">
+        <f aca="false">D9*K32</f>
+        <v>0</v>
+      </c>
+      <c r="AB39" s="0" t="n">
+        <f aca="false">E9*L32</f>
+        <v>0</v>
+      </c>
+      <c r="AC39" s="0" t="n">
+        <f aca="false">F9*M32</f>
+        <v>0</v>
+      </c>
+      <c r="AD39" s="0" t="n">
+        <f aca="false">G9*N32</f>
+        <v>0.0610680560356779</v>
+      </c>
+      <c r="AG39" s="0" t="n">
+        <f aca="false">C9*I32</f>
+        <v>0.0215684526845894</v>
+      </c>
+      <c r="AH39" s="0" t="n">
+        <f aca="false">D9*J32</f>
+        <v>0</v>
+      </c>
+      <c r="AI39" s="0" t="n">
+        <f aca="false">E9*K32</f>
+        <v>0</v>
+      </c>
+      <c r="AJ39" s="0" t="n">
+        <f aca="false">F9*L32</f>
+        <v>0</v>
+      </c>
+      <c r="AK39" s="0" t="n">
+        <f aca="false">G9*M32</f>
+        <v>0</v>
+      </c>
+      <c r="AL39" s="0" t="n">
+        <f aca="false">H9*N32</f>
+        <v>-0.0620373902584664</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q40" s="0" t="n">
+        <f aca="false">A9*I32</f>
+        <v>-0.0208373186952812</v>
+      </c>
+      <c r="R40" s="0" t="n">
+        <f aca="false">B9*J32</f>
+        <v>0</v>
+      </c>
+      <c r="S40" s="0" t="n">
+        <f aca="false">C9*K32</f>
+        <v>0</v>
+      </c>
+      <c r="T40" s="0" t="n">
+        <f aca="false">D9*L32</f>
+        <v>0</v>
+      </c>
+      <c r="U40" s="0" t="n">
+        <f aca="false">E9*M32</f>
+        <v>0</v>
+      </c>
+      <c r="V40" s="0" t="n">
+        <f aca="false">F9*N32</f>
+        <v>0.0600987218128894</v>
+      </c>
+      <c r="Y40" s="0" t="n">
+        <f aca="false">B10*I33</f>
+        <v>0.0128262993026573</v>
+      </c>
+      <c r="Z40" s="0" t="n">
+        <f aca="false">C10*J33</f>
+        <v>0</v>
+      </c>
+      <c r="AA40" s="0" t="n">
+        <f aca="false">D10*K33</f>
+        <v>0.00590863855472948</v>
+      </c>
+      <c r="AB40" s="0" t="n">
+        <f aca="false">E10*L33</f>
+        <v>0</v>
+      </c>
+      <c r="AC40" s="0" t="n">
+        <f aca="false">F10*M33</f>
+        <v>0.02748542112475</v>
+      </c>
+      <c r="AD40" s="0" t="n">
+        <f aca="false">G10*N33</f>
+        <v>0</v>
+      </c>
+      <c r="AG40" s="0" t="n">
+        <f aca="false">C10*I33</f>
+        <v>0.0130206371708794</v>
+      </c>
+      <c r="AH40" s="0" t="n">
+        <f aca="false">D10*J33</f>
+        <v>0</v>
+      </c>
+      <c r="AI40" s="0" t="n">
+        <f aca="false">E10*K33</f>
+        <v>0.00599553029818138</v>
+      </c>
+      <c r="AJ40" s="0" t="n">
+        <f aca="false">F10*L33</f>
+        <v>0</v>
+      </c>
+      <c r="AK40" s="0" t="n">
+        <f aca="false">G10*M33</f>
+        <v>0.0278780699979607</v>
+      </c>
+      <c r="AL40" s="0" t="n">
+        <f aca="false">H10*N33</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q41" s="0" t="n">
+        <f aca="false">A10*I33</f>
+        <v>-0.0126319614344352</v>
+      </c>
+      <c r="R41" s="0" t="n">
+        <f aca="false">B10*J33</f>
+        <v>0</v>
+      </c>
+      <c r="S41" s="0" t="n">
+        <f aca="false">C10*K33</f>
+        <v>0.00582174681127758</v>
+      </c>
+      <c r="T41" s="0" t="n">
+        <f aca="false">D10*L33</f>
+        <v>0</v>
+      </c>
+      <c r="U41" s="0" t="n">
+        <f aca="false">E10*M33</f>
+        <v>0.0270927722515393</v>
+      </c>
+      <c r="V41" s="0" t="n">
+        <f aca="false">F10*N33</f>
+        <v>0</v>
+      </c>
+      <c r="Y41" s="0" t="n">
+        <f aca="false">B11*I34</f>
+        <v>0</v>
+      </c>
+      <c r="Z41" s="0" t="n">
+        <f aca="false">C11*J34</f>
+        <v>0</v>
+      </c>
+      <c r="AA41" s="0" t="n">
+        <f aca="false">D11*K34</f>
+        <v>0</v>
+      </c>
+      <c r="AB41" s="0" t="n">
+        <f aca="false">E11*L34</f>
+        <v>0</v>
+      </c>
+      <c r="AC41" s="0" t="n">
+        <f aca="false">F11*M34</f>
+        <v>0</v>
+      </c>
+      <c r="AD41" s="0" t="n">
+        <f aca="false">G11*N34</f>
+        <v>0</v>
+      </c>
+      <c r="AG41" s="0" t="n">
+        <f aca="false">C11*I34</f>
+        <v>0</v>
+      </c>
+      <c r="AH41" s="0" t="n">
+        <f aca="false">D11*J34</f>
+        <v>0</v>
+      </c>
+      <c r="AI41" s="0" t="n">
+        <f aca="false">E11*K34</f>
+        <v>0</v>
+      </c>
+      <c r="AJ41" s="0" t="n">
+        <f aca="false">F11*L34</f>
+        <v>0</v>
+      </c>
+      <c r="AK41" s="0" t="n">
+        <f aca="false">G11*M34</f>
+        <v>0</v>
+      </c>
+      <c r="AL41" s="0" t="n">
+        <f aca="false">H11*N34</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
-      <c r="E42" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G42" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H42" s="5"/>
-      <c r="I42" s="5"/>
-      <c r="K42" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="L42" s="5"/>
-      <c r="M42" s="5"/>
+      <c r="A42" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
+      <c r="E42" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G42" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H42" s="7"/>
+      <c r="I42" s="7"/>
+      <c r="K42" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L42" s="7"/>
+      <c r="M42" s="7"/>
       <c r="O42" s="0" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>16</v>
+        <v>26</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>27</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="H43" s="0" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I43" s="0" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="K43" s="0" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="L43" s="0" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="M43" s="0" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="O43" s="0" t="n">
         <v>-0.1</v>
@@ -1767,11 +3417,11 @@
         <f aca="false">E46*C46</f>
         <v>0.0707489664131252</v>
       </c>
-      <c r="K46" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="L46" s="5"/>
-      <c r="M46" s="5"/>
+      <c r="K46" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="L46" s="7"/>
+      <c r="M46" s="7"/>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
@@ -1865,11 +3515,11 @@
         <f aca="false">E49*C49</f>
         <v>0.0656249367548498</v>
       </c>
-      <c r="K49" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L49" s="5"/>
-      <c r="M49" s="5"/>
+      <c r="K49" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="L49" s="7"/>
+      <c r="M49" s="7"/>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="n">
@@ -1963,11 +3613,11 @@
         <f aca="false">E52*C52</f>
         <v>0.00973798809486858</v>
       </c>
-      <c r="K52" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="L52" s="5"/>
-      <c r="M52" s="5"/>
+      <c r="K52" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="L52" s="7"/>
+      <c r="M52" s="7"/>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="n">
@@ -1995,7 +3645,7 @@
         <f aca="false">E53*C53</f>
         <v>0.097245459636807</v>
       </c>
-      <c r="K53" s="6" t="n">
+      <c r="K53" s="8" t="n">
         <v>0.32</v>
       </c>
       <c r="L53" s="0" t="n">
@@ -2058,23 +3708,23 @@
         <f aca="false">E55*C55</f>
         <v>0</v>
       </c>
-      <c r="K55" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="L55" s="5"/>
-      <c r="M55" s="5"/>
+      <c r="K55" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="L55" s="7"/>
+      <c r="M55" s="7"/>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="7" t="n">
+      <c r="A56" s="9" t="n">
         <v>0.530585715350705</v>
       </c>
-      <c r="B56" s="7" t="n">
+      <c r="B56" s="9" t="n">
         <v>0.25354050051506</v>
       </c>
-      <c r="C56" s="7" t="n">
+      <c r="C56" s="9" t="n">
         <v>0.282080994964924</v>
       </c>
-      <c r="E56" s="7" t="n">
+      <c r="E56" s="9" t="n">
         <v>1</v>
       </c>
       <c r="G56" s="0" t="n">
@@ -2103,16 +3753,16 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="7" t="s">
-        <v>21</v>
+      <c r="A57" s="9" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K58" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L58" s="3"/>
-      <c r="M58" s="3"/>
+      <c r="K58" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L58" s="5"/>
+      <c r="M58" s="5"/>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K59" s="0" t="n">
@@ -2129,296 +3779,296 @@
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B61" s="5"/>
-      <c r="C61" s="5"/>
-      <c r="E61" s="5"/>
-      <c r="F61" s="5"/>
-      <c r="G61" s="5"/>
-      <c r="K61" s="3"/>
-      <c r="L61" s="3"/>
-      <c r="M61" s="3"/>
+      <c r="A61" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B61" s="7"/>
+      <c r="C61" s="7"/>
+      <c r="E61" s="7"/>
+      <c r="F61" s="7"/>
+      <c r="G61" s="7"/>
+      <c r="K61" s="5"/>
+      <c r="L61" s="5"/>
+      <c r="M61" s="5"/>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="6" t="n">
+      <c r="A62" s="8" t="n">
         <f aca="false">K$59*A44</f>
         <v>0.0243144804084281</v>
       </c>
-      <c r="B62" s="6" t="n">
+      <c r="B62" s="8" t="n">
         <f aca="false">L$59*B44</f>
         <v>0.0272129513046061</v>
       </c>
-      <c r="C62" s="6" t="n">
+      <c r="C62" s="8" t="n">
         <f aca="false">M$59*C44</f>
         <v>-0.0373308966441698</v>
       </c>
-      <c r="D62" s="6"/>
+      <c r="D62" s="8"/>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="6" t="n">
+      <c r="A63" s="8" t="n">
         <f aca="false">K$59*A45</f>
         <v>0.0173130920197195</v>
       </c>
-      <c r="B63" s="6" t="n">
+      <c r="B63" s="8" t="n">
         <f aca="false">L$59*B45</f>
         <v>0.0201058844117969</v>
       </c>
-      <c r="C63" s="6" t="n">
+      <c r="C63" s="8" t="n">
         <f aca="false">M$59*C45</f>
         <v>-0.0145929371737229</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="6" t="n">
+      <c r="A64" s="8" t="n">
         <f aca="false">K$59*A46</f>
         <v>0.0378875492824237</v>
       </c>
-      <c r="B64" s="6" t="n">
+      <c r="B64" s="8" t="n">
         <f aca="false">L$59*B46</f>
         <v>0.0149495453867415</v>
       </c>
-      <c r="C64" s="6" t="n">
+      <c r="C64" s="8" t="n">
         <f aca="false">M$59*C46</f>
         <v>-0.013447907756571</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="6" t="n">
+      <c r="A65" s="8" t="n">
         <f aca="false">K$59*A47</f>
         <v>0.0548718518977952</v>
       </c>
-      <c r="B65" s="6" t="n">
+      <c r="B65" s="8" t="n">
         <f aca="false">L$59*B47</f>
         <v>0.0115437263154276</v>
       </c>
-      <c r="C65" s="6" t="n">
+      <c r="C65" s="8" t="n">
         <f aca="false">M$59*C47</f>
         <v>-0.00932248740873383</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="6" t="n">
+      <c r="A66" s="8" t="n">
         <f aca="false">K$59*A48</f>
         <v>0.0291593723758922</v>
       </c>
-      <c r="B66" s="6" t="n">
+      <c r="B66" s="8" t="n">
         <f aca="false">L$59*B48</f>
         <v>0.030142320303196</v>
       </c>
-      <c r="C66" s="6" t="n">
+      <c r="C66" s="8" t="n">
         <f aca="false">M$59*C48</f>
         <v>-0.0395722681426169</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="6" t="n">
+      <c r="A67" s="8" t="n">
         <f aca="false">K$59*A49</f>
         <v>0.0236844122487356</v>
       </c>
-      <c r="B67" s="6" t="n">
+      <c r="B67" s="8" t="n">
         <f aca="false">L$59*B49</f>
         <v>0.015691566720734</v>
       </c>
-      <c r="C67" s="6" t="n">
+      <c r="C67" s="8" t="n">
         <f aca="false">M$59*C49</f>
         <v>-0.0345290639033747</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="6" t="n">
+      <c r="A68" s="8" t="n">
         <f aca="false">K$59*A50</f>
         <v>0.016692429723613</v>
       </c>
-      <c r="B68" s="6" t="n">
+      <c r="B68" s="8" t="n">
         <f aca="false">L$59*B50</f>
         <v>0.0457060216855454</v>
       </c>
-      <c r="C68" s="6" t="n">
+      <c r="C68" s="8" t="n">
         <f aca="false">M$59*C50</f>
         <v>-0.0319664131722955</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="6" t="n">
+      <c r="A69" s="8" t="n">
         <f aca="false">K$59*A51</f>
         <v>0.0423260769589363</v>
       </c>
-      <c r="B69" s="6" t="n">
+      <c r="B69" s="8" t="n">
         <f aca="false">L$59*B51</f>
         <v>0.00149493701378588</v>
       </c>
-      <c r="C69" s="6" t="n">
+      <c r="C69" s="8" t="n">
         <f aca="false">M$59*C51</f>
         <v>-0.00726431450731645</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="6" t="n">
+      <c r="A70" s="8" t="n">
         <f aca="false">K$59*A52</f>
         <v>0.0490676965343318</v>
       </c>
-      <c r="B70" s="6" t="n">
+      <c r="B70" s="8" t="n">
         <f aca="false">L$59*B52</f>
         <v>0.0515111649367729</v>
       </c>
-      <c r="C70" s="6" t="n">
+      <c r="C70" s="8" t="n">
         <f aca="false">M$59*C52</f>
         <v>-0.00364543919225092</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="6" t="n">
+      <c r="A71" s="8" t="n">
         <f aca="false">K$59*A53</f>
         <v>0.0480621201404268</v>
       </c>
-      <c r="B71" s="6" t="n">
+      <c r="B71" s="8" t="n">
         <f aca="false">L$59*B53</f>
         <v>0.00312268627804925</v>
       </c>
-      <c r="C71" s="6" t="n">
+      <c r="C71" s="8" t="n">
         <f aca="false">M$59*C53</f>
         <v>-0.031751019596268</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="6" t="n">
+      <c r="A72" s="8" t="n">
         <f aca="false">K$59*A54</f>
         <v>0.0243638363265937</v>
       </c>
-      <c r="B72" s="6" t="n">
+      <c r="B72" s="8" t="n">
         <f aca="false">L$59*B54</f>
         <v>0.00915172773638514</v>
       </c>
-      <c r="C72" s="6" t="n">
+      <c r="C72" s="8" t="n">
         <f aca="false">M$59*C54</f>
         <v>-0.0248263897177885</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="6" t="n">
+      <c r="A73" s="8" t="n">
         <f aca="false">K$59*A55</f>
         <v>0.0439692207317199</v>
       </c>
-      <c r="B73" s="6" t="n">
+      <c r="B73" s="8" t="n">
         <f aca="false">L$59*B55</f>
         <v>0.0147104591991053</v>
       </c>
-      <c r="C73" s="6" t="n">
+      <c r="C73" s="8" t="n">
         <f aca="false">M$59*C55</f>
         <v>-0.0194147926097537</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="8" t="n">
+      <c r="A74" s="10" t="n">
         <f aca="false">K$59*A56</f>
         <v>0.0428727400634647</v>
       </c>
-      <c r="B74" s="8" t="n">
+      <c r="B74" s="10" t="n">
         <f aca="false">L$59*B56</f>
         <v>0.0133917239457459</v>
       </c>
-      <c r="C74" s="8" t="n">
+      <c r="C74" s="10" t="n">
         <f aca="false">M$59*C56</f>
         <v>-0.012942255755858</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="6"/>
+      <c r="A75" s="8"/>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="6" t="n">
+      <c r="A76" s="8" t="n">
         <f aca="false">SUM(A62:C62)</f>
         <v>0.0141965350688645</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="6" t="n">
+      <c r="A77" s="8" t="n">
         <f aca="false">SUM(A63:C63)</f>
         <v>0.0228260392577935</v>
       </c>
-      <c r="B77" s="9"/>
-      <c r="C77" s="9"/>
+      <c r="B77" s="11"/>
+      <c r="C77" s="11"/>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="6" t="n">
+      <c r="A78" s="8" t="n">
         <f aca="false">SUM(A64:C64)</f>
         <v>0.0393891869125942</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="6" t="n">
+      <c r="A79" s="8" t="n">
         <f aca="false">SUM(A65:C65)</f>
         <v>0.057093090804489</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="6" t="n">
+      <c r="A80" s="8" t="n">
         <f aca="false">SUM(A66:C66)</f>
         <v>0.0197294245364713</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="6" t="n">
+      <c r="A81" s="8" t="n">
         <f aca="false">SUM(A67:C67)</f>
         <v>0.00484691506609497</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="6" t="n">
+      <c r="A82" s="8" t="n">
         <f aca="false">SUM(A68:C68)</f>
         <v>0.0304320382368629</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="6" t="n">
+      <c r="A83" s="8" t="n">
         <f aca="false">SUM(A69:C69)</f>
         <v>0.0365566994654057</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="6" t="n">
+      <c r="A84" s="8" t="n">
         <f aca="false">SUM(A70:C70)</f>
         <v>0.0969334222788538</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="6" t="n">
+      <c r="A85" s="8" t="n">
         <f aca="false">SUM(A71:C71)</f>
         <v>0.0194337868222081</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="6" t="n">
+      <c r="A86" s="8" t="n">
         <f aca="false">SUM(A72:C72)</f>
         <v>0.00868917434519041</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="6" t="n">
+      <c r="A87" s="8" t="n">
         <f aca="false">SUM(A73:C73)</f>
         <v>0.0392648873210714</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="8" t="n">
+      <c r="A88" s="10" t="n">
         <f aca="false">SUM(A74:C74)</f>
         <v>0.0433222082533526</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="D90" s="0" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2446,7 +4096,7 @@
         <f aca="false">C91+C44</f>
         <v>0.815015202899816</v>
       </c>
-      <c r="J91" s="10"/>
+      <c r="J91" s="12"/>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="n">
@@ -2735,27 +4385,27 @@
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="7" t="n">
+      <c r="A103" s="9" t="n">
         <f aca="false">$O$43*K$59*$E56</f>
         <v>-0.00808026654753169</v>
       </c>
-      <c r="B103" s="7" t="n">
+      <c r="B103" s="9" t="n">
         <f aca="false">$O$43*L$59*$E56</f>
         <v>-0.0052818874769676</v>
       </c>
-      <c r="C103" s="7" t="n">
+      <c r="C103" s="9" t="n">
         <f aca="false">$O$43*M$59*$E56</f>
         <v>0.00458813460916335</v>
       </c>
-      <c r="D103" s="7" t="n">
+      <c r="D103" s="9" t="n">
         <f aca="false">A103+A56</f>
         <v>0.522505448803173</v>
       </c>
-      <c r="E103" s="7" t="n">
+      <c r="E103" s="9" t="n">
         <f aca="false">B103+B56</f>
         <v>0.248258613038092</v>
       </c>
-      <c r="F103" s="7" t="n">
+      <c r="F103" s="9" t="n">
         <f aca="false">C103+C56</f>
         <v>0.286669129574087</v>
       </c>

</xml_diff>